<commit_message>
Add windows for floors 8-6
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8306A494-43C2-4AFA-9B83-1CAEA887BB8E}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19DE14D-9A81-4306-AF89-0BF1666D3109}"/>
   <bookViews>
     <workbookView xWindow="-15795" yWindow="-4305" windowWidth="15105" windowHeight="13320" activeTab="1" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Columns</t>
   </si>
@@ -109,6 +109,30 @@
   </si>
   <si>
     <t>Floors: 8</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1527,8 @@
   <dimension ref="A1:AD62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R54" sqref="R54"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,7 +1996,9 @@
       <c r="F13" s="43">
         <v>11</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="30" t="s">
+        <v>31</v>
+      </c>
       <c r="H13" s="32"/>
       <c r="I13" s="21"/>
       <c r="J13" s="22"/>
@@ -2091,7 +2117,9 @@
       <c r="F17" s="43">
         <v>15</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="H17" s="32"/>
       <c r="I17" s="30"/>
       <c r="J17" s="32"/>
@@ -2265,7 +2293,9 @@
       <c r="F23" s="43">
         <v>21</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="32"/>
       <c r="I23" s="30"/>
       <c r="J23" s="32"/>
@@ -2439,7 +2469,9 @@
       <c r="F29" s="43">
         <v>27</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="H29" s="32"/>
       <c r="I29" s="30"/>
       <c r="J29" s="32"/>
@@ -2613,7 +2645,9 @@
       <c r="F35" s="43">
         <v>33</v>
       </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="30" t="s">
+        <v>27</v>
+      </c>
       <c r="H35" s="32"/>
       <c r="I35" s="30"/>
       <c r="J35" s="32"/>
@@ -2787,7 +2821,9 @@
       <c r="F41" s="43">
         <v>39</v>
       </c>
-      <c r="G41" s="30"/>
+      <c r="G41" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="H41" s="32"/>
       <c r="I41" s="30"/>
       <c r="J41" s="32"/>
@@ -2961,7 +2997,9 @@
       <c r="F47" s="43">
         <v>45</v>
       </c>
-      <c r="G47" s="30"/>
+      <c r="G47" s="30" t="s">
+        <v>25</v>
+      </c>
       <c r="H47" s="32"/>
       <c r="I47" s="30"/>
       <c r="J47" s="32"/>
@@ -3135,7 +3173,9 @@
       <c r="F53" s="43">
         <v>51</v>
       </c>
-      <c r="G53" s="30"/>
+      <c r="G53" s="30" t="s">
+        <v>24</v>
+      </c>
       <c r="H53" s="32"/>
       <c r="I53" s="30"/>
       <c r="J53" s="32"/>

</xml_diff>

<commit_message>
Add windows B2 H2 floors 8-7
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19DE14D-9A81-4306-AF89-0BF1666D3109}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55DE1F9A-BDBB-4006-893F-6C849277D036}"/>
   <bookViews>
-    <workbookView xWindow="-15795" yWindow="-4305" windowWidth="15105" windowHeight="13320" activeTab="1" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-15795" yWindow="-4305" windowWidth="15105" windowHeight="13320" activeTab="2" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
-    <sheet name="B2" sheetId="3" r:id="rId2"/>
+    <sheet name="B2-H1" sheetId="3" r:id="rId2"/>
+    <sheet name="B2-H2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>Columns</t>
   </si>
@@ -1526,9 +1527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A03D14-663C-42B7-B26E-A63445663F92}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,4 +3459,918 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C69FB0-708A-40A2-9151-AAEA467E5F20}">
+  <dimension ref="A1:AC62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="3.28515625" customWidth="1"/>
+    <col min="15" max="15" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>300</v>
+      </c>
+      <c r="C2">
+        <f>B2/5</f>
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3" si="0">B3/5</f>
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="37"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="43">
+        <v>7</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="37"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="43">
+        <v>8</v>
+      </c>
+      <c r="G10" s="40"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="41"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="43">
+        <v>9</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="35"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="43">
+        <v>10</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="37"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="37"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F13" s="43">
+        <v>11</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="37"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="37"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="43">
+        <v>12</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F15" s="43">
+        <v>13</v>
+      </c>
+      <c r="G15" s="39"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F16" s="43">
+        <v>14</v>
+      </c>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="41"/>
+    </row>
+    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F17" s="43">
+        <v>15</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="35"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="35"/>
+    </row>
+    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F18" s="43">
+        <v>16</v>
+      </c>
+      <c r="G18" s="39"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F19" s="43">
+        <v>17</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="37"/>
+    </row>
+    <row r="20" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F20" s="43">
+        <v>18</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F21" s="43">
+        <v>19</v>
+      </c>
+      <c r="G21" s="39"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="37"/>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F22" s="43">
+        <v>20</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="41"/>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F23" s="43">
+        <v>21</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="35"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F24" s="43">
+        <v>22</v>
+      </c>
+      <c r="G24" s="39"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="37"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F25" s="43">
+        <v>23</v>
+      </c>
+      <c r="G25" s="39"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="37"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F26" s="43">
+        <v>24</v>
+      </c>
+      <c r="G26" s="39"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="37"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F27" s="43">
+        <v>25</v>
+      </c>
+      <c r="G27" s="39"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="37"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F28" s="43">
+        <v>26</v>
+      </c>
+      <c r="G28" s="40"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="41"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F29" s="43">
+        <v>27</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="35"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="35"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F30" s="43">
+        <v>28</v>
+      </c>
+      <c r="G30" s="39"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="37"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F31" s="43">
+        <v>29</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="37"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F32" s="43">
+        <v>30</v>
+      </c>
+      <c r="G32" s="39"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="37"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F33" s="43">
+        <v>31</v>
+      </c>
+      <c r="G33" s="39"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="37"/>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="43">
+        <v>32</v>
+      </c>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="41"/>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F35" s="43">
+        <v>33</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" s="35"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="35"/>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F36" s="43">
+        <v>34</v>
+      </c>
+      <c r="G36" s="39"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="37"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="37"/>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F37" s="43">
+        <v>35</v>
+      </c>
+      <c r="G37" s="39"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="37"/>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F38" s="43">
+        <v>36</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="37"/>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F39" s="43">
+        <v>37</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="37"/>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F40" s="43">
+        <v>38</v>
+      </c>
+      <c r="G40" s="40"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="41"/>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F41" s="43">
+        <v>39</v>
+      </c>
+      <c r="G41" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="35"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="35"/>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F42" s="43">
+        <v>40</v>
+      </c>
+      <c r="G42" s="39"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="37"/>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F43" s="43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="39"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="37"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="37"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="37"/>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F44" s="43">
+        <v>42</v>
+      </c>
+      <c r="G44" s="39"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="37"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="37"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="37"/>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45" s="43">
+        <v>43</v>
+      </c>
+      <c r="G45" s="39"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="37"/>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F46" s="43">
+        <v>44</v>
+      </c>
+      <c r="G46" s="40"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="41"/>
+    </row>
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F47" s="43">
+        <v>45</v>
+      </c>
+      <c r="G47" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="35"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="38"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="38"/>
+      <c r="N47" s="35"/>
+    </row>
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F48" s="43">
+        <v>46</v>
+      </c>
+      <c r="G48" s="39"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="37"/>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F49" s="43">
+        <v>47</v>
+      </c>
+      <c r="G49" s="39"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="37"/>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F50" s="43">
+        <v>48</v>
+      </c>
+      <c r="G50" s="39"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="37"/>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F51" s="43">
+        <v>49</v>
+      </c>
+      <c r="G51" s="39"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="39"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="39"/>
+      <c r="N51" s="37"/>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F52" s="43">
+        <v>50</v>
+      </c>
+      <c r="G52" s="40"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="41"/>
+      <c r="M52" s="40"/>
+      <c r="N52" s="41"/>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F53" s="43">
+        <v>51</v>
+      </c>
+      <c r="G53" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="35"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="38"/>
+      <c r="N53" s="35"/>
+    </row>
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F54" s="43">
+        <v>52</v>
+      </c>
+      <c r="G54" s="39"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="37"/>
+    </row>
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F55" s="43">
+        <v>53</v>
+      </c>
+      <c r="G55" s="39"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="39"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="37"/>
+    </row>
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F56" s="43">
+        <v>54</v>
+      </c>
+      <c r="G56" s="39"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="39"/>
+      <c r="N56" s="37"/>
+    </row>
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F57" s="43">
+        <v>55</v>
+      </c>
+      <c r="G57" s="39"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="39"/>
+      <c r="N57" s="37"/>
+    </row>
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F58" s="43">
+        <v>56</v>
+      </c>
+      <c r="G58" s="40"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="40"/>
+      <c r="L58" s="41"/>
+      <c r="M58" s="40"/>
+      <c r="N58" s="41"/>
+    </row>
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F59" s="43">
+        <v>57</v>
+      </c>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+    </row>
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F60" s="43"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+    </row>
+    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F61" s="43"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+    </row>
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F62" s="43"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add all windows to B3 Half 1
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="505" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51FBC75F-8ADE-4941-8210-B7F829ABA418}"/>
+  <xr:revisionPtr revIDLastSave="517" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C9A2A0-C9EB-435C-BD6E-4EE4A7C81C49}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="3" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView minimized="1" xWindow="-14955" yWindow="1470" windowWidth="15105" windowHeight="13320" activeTab="3" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
@@ -4266,7 +4266,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="A15:B16"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4829,7 +4829,7 @@
       <c r="G12" s="46"/>
       <c r="H12" s="47"/>
       <c r="I12" s="5" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="J12" s="41"/>
       <c r="K12" s="6"/>
@@ -5005,7 +5005,7 @@
       <c r="G16" s="46"/>
       <c r="H16" s="47"/>
       <c r="I16" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="J16" s="41"/>
       <c r="K16" s="6"/>
@@ -5247,7 +5247,7 @@
       <c r="G22" s="46"/>
       <c r="H22" s="47"/>
       <c r="I22" s="5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="J22" s="41"/>
       <c r="K22" s="6"/>
@@ -5529,7 +5529,7 @@
       <c r="G29" s="46"/>
       <c r="H29" s="47"/>
       <c r="I29" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J29" s="41"/>
       <c r="K29" s="6"/>
@@ -5771,7 +5771,7 @@
       <c r="G35" s="46"/>
       <c r="H35" s="47"/>
       <c r="I35" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J35" s="41"/>
       <c r="K35" s="6"/>
@@ -6013,7 +6013,7 @@
       <c r="G41" s="46"/>
       <c r="H41" s="47"/>
       <c r="I41" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J41" s="41"/>
       <c r="K41" s="6"/>
@@ -6255,7 +6255,7 @@
       <c r="G47" s="46"/>
       <c r="H47" s="47"/>
       <c r="I47" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J47" s="41"/>
       <c r="K47" s="6"/>
@@ -6497,7 +6497,7 @@
       <c r="G53" s="46"/>
       <c r="H53" s="47"/>
       <c r="I53" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J53" s="41"/>
       <c r="K53" s="6"/>
@@ -6739,7 +6739,7 @@
       <c r="G59" s="46"/>
       <c r="H59" s="47"/>
       <c r="I59" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J59" s="41"/>
       <c r="K59" s="6"/>
@@ -6981,7 +6981,7 @@
       <c r="G65" s="46"/>
       <c r="H65" s="47"/>
       <c r="I65" s="5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="J65" s="41"/>
       <c r="K65" s="6"/>
@@ -7223,7 +7223,7 @@
       <c r="G71" s="46"/>
       <c r="H71" s="47"/>
       <c r="I71" s="5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J71" s="41"/>
       <c r="K71" s="6"/>
@@ -7465,7 +7465,7 @@
       <c r="G77" s="46"/>
       <c r="H77" s="47"/>
       <c r="I77" s="5" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="J77" s="41"/>
       <c r="K77" s="6"/>

</xml_diff>

<commit_message>
Add all windows to B3 Half2
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="517" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70C9A2A0-C9EB-435C-BD6E-4EE4A7C81C49}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B66BB655-7D6B-4689-8ACF-8CC8EBAD3D8E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-14955" yWindow="1470" windowWidth="15105" windowHeight="13320" activeTab="3" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="4" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
     <sheet name="B2-H1" sheetId="3" r:id="rId2"/>
     <sheet name="B2-H2" sheetId="5" r:id="rId3"/>
     <sheet name="B3-H1" sheetId="6" r:id="rId4"/>
+    <sheet name="B3-H2" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
   <si>
     <t>Columns</t>
   </si>
@@ -4264,9 +4265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5669387-3D46-4462-BFC6-BE1B7800A31B}">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4872,6 +4873,10 @@
         <f>B11*5</f>
         <v>110</v>
       </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>65</v>
+      </c>
       <c r="F13">
         <v>11</v>
       </c>
@@ -4919,6 +4924,10 @@
         <f>B12*5</f>
         <v>390</v>
       </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>390</v>
+      </c>
       <c r="F14">
         <v>12</v>
       </c>
@@ -7703,4 +7712,1623 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278E81A6-9D9A-455C-A555-1D86B421F969}">
+  <dimension ref="A1:S82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V34" sqref="V34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="18" width="3.140625" customWidth="1"/>
+    <col min="19" max="19" width="3.28515625" customWidth="1"/>
+    <col min="20" max="20" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="54"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="57"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="57"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="57"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>390</v>
+      </c>
+      <c r="C7">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="55"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="57"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>175</v>
+      </c>
+      <c r="C8">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="55"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+      <c r="S8" s="57"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="46"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="48"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="48"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="46"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="48"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>78</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="5">
+        <v>12</v>
+      </c>
+      <c r="J12" s="41"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="48"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>110</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="48"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>390</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>390</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="48"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="48"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="48"/>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="41">
+        <v>11</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="48"/>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="48"/>
+    </row>
+    <row r="19" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="48"/>
+    </row>
+    <row r="20" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="46"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="48"/>
+    </row>
+    <row r="21" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="48"/>
+    </row>
+    <row r="22" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="48"/>
+    </row>
+    <row r="23" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="41"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="48"/>
+    </row>
+    <row r="24" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="46"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="5">
+        <v>10</v>
+      </c>
+      <c r="J24" s="41"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="41"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="48"/>
+    </row>
+    <row r="25" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="41"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="48"/>
+    </row>
+    <row r="26" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="46"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="48"/>
+    </row>
+    <row r="27" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="48"/>
+    </row>
+    <row r="28" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="47"/>
+      <c r="S28" s="48"/>
+    </row>
+    <row r="29" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="46"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="47"/>
+      <c r="S29" s="48"/>
+    </row>
+    <row r="30" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="41">
+        <v>9</v>
+      </c>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="48"/>
+    </row>
+    <row r="31" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="48"/>
+    </row>
+    <row r="32" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="46"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="48"/>
+    </row>
+    <row r="33" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="46"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="48"/>
+    </row>
+    <row r="34" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="46"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="48"/>
+    </row>
+    <row r="35" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="46"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="41">
+        <v>8</v>
+      </c>
+      <c r="K35" s="6"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="48"/>
+    </row>
+    <row r="36" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="46"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="41"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="48"/>
+    </row>
+    <row r="37" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="46"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="48"/>
+    </row>
+    <row r="38" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="46"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="47"/>
+      <c r="S38" s="48"/>
+    </row>
+    <row r="39" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="47"/>
+      <c r="S39" s="48"/>
+    </row>
+    <row r="40" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="46"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="47"/>
+      <c r="S40" s="48"/>
+    </row>
+    <row r="41" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="46"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="48"/>
+    </row>
+    <row r="42" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="46"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="41">
+        <v>7</v>
+      </c>
+      <c r="K42" s="6"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="48"/>
+    </row>
+    <row r="43" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="46"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="41"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="48"/>
+    </row>
+    <row r="44" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="46"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="47"/>
+      <c r="S44" s="48"/>
+    </row>
+    <row r="45" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="46"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="47"/>
+      <c r="S45" s="48"/>
+    </row>
+    <row r="46" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="46"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="47"/>
+      <c r="S46" s="48"/>
+    </row>
+    <row r="47" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="46"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="41"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="47"/>
+      <c r="S47" s="48"/>
+    </row>
+    <row r="48" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="46"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="41">
+        <v>6</v>
+      </c>
+      <c r="K48" s="6"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="41"/>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="47"/>
+      <c r="S48" s="48"/>
+    </row>
+    <row r="49" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="46"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="41"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="41"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="47"/>
+      <c r="S49" s="48"/>
+    </row>
+    <row r="50" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="46"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="47"/>
+      <c r="S50" s="48"/>
+    </row>
+    <row r="51" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="46"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="47"/>
+      <c r="S51" s="48"/>
+    </row>
+    <row r="52" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" s="46"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="41"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="41"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="47"/>
+      <c r="S52" s="48"/>
+    </row>
+    <row r="53" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>51</v>
+      </c>
+      <c r="G53" s="46"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="41"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="47"/>
+      <c r="S53" s="48"/>
+    </row>
+    <row r="54" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>52</v>
+      </c>
+      <c r="G54" s="46"/>
+      <c r="H54" s="47"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="41">
+        <v>5</v>
+      </c>
+      <c r="K54" s="6"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="41"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="47"/>
+      <c r="S54" s="48"/>
+    </row>
+    <row r="55" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>53</v>
+      </c>
+      <c r="G55" s="46"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="41"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="41"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="47"/>
+      <c r="S55" s="48"/>
+    </row>
+    <row r="56" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>54</v>
+      </c>
+      <c r="G56" s="46"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="47"/>
+      <c r="S56" s="48"/>
+    </row>
+    <row r="57" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" s="46"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="47"/>
+      <c r="S57" s="48"/>
+    </row>
+    <row r="58" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" s="46"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="41"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="41"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="47"/>
+      <c r="S58" s="48"/>
+    </row>
+    <row r="59" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>57</v>
+      </c>
+      <c r="G59" s="46"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="41">
+        <v>4</v>
+      </c>
+      <c r="K59" s="6"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="41"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="41"/>
+      <c r="Q59" s="6"/>
+      <c r="R59" s="47"/>
+      <c r="S59" s="48"/>
+    </row>
+    <row r="60" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="46"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="41"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="41"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="6"/>
+      <c r="R60" s="47"/>
+      <c r="S60" s="48"/>
+    </row>
+    <row r="61" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="46"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="41"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="41"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="41"/>
+      <c r="Q61" s="6"/>
+      <c r="R61" s="47"/>
+      <c r="S61" s="48"/>
+    </row>
+    <row r="62" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="46"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="8"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="8"/>
+      <c r="Q62" s="9"/>
+      <c r="R62" s="47"/>
+      <c r="S62" s="48"/>
+    </row>
+    <row r="63" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="46"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="47"/>
+      <c r="S63" s="48"/>
+    </row>
+    <row r="64" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="G64" s="46"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="41"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="41"/>
+      <c r="N64" s="6"/>
+      <c r="O64" s="5"/>
+      <c r="P64" s="41"/>
+      <c r="Q64" s="6"/>
+      <c r="R64" s="47"/>
+      <c r="S64" s="48"/>
+    </row>
+    <row r="65" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="G65" s="46"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="5">
+        <v>3</v>
+      </c>
+      <c r="J65" s="41"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="41"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="41"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="47"/>
+      <c r="S65" s="48"/>
+    </row>
+    <row r="66" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66" s="46"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="41"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="41"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="41"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="47"/>
+      <c r="S66" s="48"/>
+    </row>
+    <row r="67" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67" s="46"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="41"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="41"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="41"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="47"/>
+      <c r="S67" s="48"/>
+    </row>
+    <row r="68" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="G68" s="46"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="47"/>
+      <c r="S68" s="48"/>
+    </row>
+    <row r="69" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="G69" s="46"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="47"/>
+      <c r="S69" s="48"/>
+    </row>
+    <row r="70" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="G70" s="46"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="5">
+        <v>2</v>
+      </c>
+      <c r="J70" s="41"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="41"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="41"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="47"/>
+      <c r="S70" s="48"/>
+    </row>
+    <row r="71" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
+      </c>
+      <c r="G71" s="46"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="41"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="41"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="41"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="47"/>
+      <c r="S71" s="48"/>
+    </row>
+    <row r="72" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="G72" s="46"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="41"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="41"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="5"/>
+      <c r="P72" s="41"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="47"/>
+      <c r="S72" s="48"/>
+    </row>
+    <row r="73" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>71</v>
+      </c>
+      <c r="G73" s="46"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="41"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="41"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="41"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="47"/>
+      <c r="S73" s="48"/>
+    </row>
+    <row r="74" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>72</v>
+      </c>
+      <c r="G74" s="46"/>
+      <c r="H74" s="47"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="9"/>
+      <c r="O74" s="7"/>
+      <c r="P74" s="8"/>
+      <c r="Q74" s="9"/>
+      <c r="R74" s="47"/>
+      <c r="S74" s="48"/>
+    </row>
+    <row r="75" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>73</v>
+      </c>
+      <c r="G75" s="46"/>
+      <c r="H75" s="47"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="47"/>
+      <c r="S75" s="48"/>
+    </row>
+    <row r="76" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>74</v>
+      </c>
+      <c r="G76" s="46"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="41"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="41"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="41"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="47"/>
+      <c r="S76" s="48"/>
+    </row>
+    <row r="77" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>75</v>
+      </c>
+      <c r="G77" s="46"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="5">
+        <v>1</v>
+      </c>
+      <c r="J77" s="41"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="41"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="41"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="47"/>
+      <c r="S77" s="48"/>
+    </row>
+    <row r="78" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>76</v>
+      </c>
+      <c r="G78" s="46"/>
+      <c r="H78" s="47"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="41"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="41"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="41"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="47"/>
+      <c r="S78" s="48"/>
+    </row>
+    <row r="79" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>77</v>
+      </c>
+      <c r="G79" s="46"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="41"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="41"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="41"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="47"/>
+      <c r="S79" s="48"/>
+    </row>
+    <row r="80" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>78</v>
+      </c>
+      <c r="G80" s="49"/>
+      <c r="H80" s="50"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="8"/>
+      <c r="N80" s="9"/>
+      <c r="O80" s="7"/>
+      <c r="P80" s="8"/>
+      <c r="Q80" s="9"/>
+      <c r="R80" s="50"/>
+      <c r="S80" s="51"/>
+    </row>
+    <row r="81" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>79</v>
+      </c>
+      <c r="G81" s="42"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="42"/>
+      <c r="P81" s="42"/>
+      <c r="Q81" s="42"/>
+      <c r="R81" s="42"/>
+      <c r="S81" s="42"/>
+    </row>
+    <row r="82" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>80</v>
+      </c>
+      <c r="G82" s="42"/>
+      <c r="H82" s="42"/>
+      <c r="I82" s="42"/>
+      <c r="J82" s="42"/>
+      <c r="K82" s="42"/>
+      <c r="L82" s="42"/>
+      <c r="M82" s="42"/>
+      <c r="N82" s="42"/>
+      <c r="O82" s="42"/>
+      <c r="P82" s="42"/>
+      <c r="Q82" s="42"/>
+      <c r="R82" s="42"/>
+      <c r="S82" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add html structure for Building 4
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="550" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B66BB655-7D6B-4689-8ACF-8CC8EBAD3D8E}"/>
+  <xr:revisionPtr revIDLastSave="680" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44C1A61D-465B-4E17-B9C5-B75D4F865C35}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="4" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="B2-H2" sheetId="5" r:id="rId3"/>
     <sheet name="B3-H1" sheetId="6" r:id="rId4"/>
     <sheet name="B3-H2" sheetId="7" r:id="rId5"/>
+    <sheet name="B4-H1" sheetId="9" r:id="rId6"/>
+    <sheet name="B4-H2" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="45">
   <si>
     <t>Columns</t>
   </si>
@@ -166,6 +168,15 @@
   </si>
   <si>
     <t>#12</t>
+  </si>
+  <si>
+    <t>H: 3</t>
+  </si>
+  <si>
+    <t>W: 10</t>
+  </si>
+  <si>
+    <t>H: 7</t>
   </si>
 </sst>
 </file>
@@ -331,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -390,6 +401,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +743,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G6"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7718,8 +7733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278E81A6-9D9A-455C-A555-1D86B421F969}">
   <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
@@ -9331,4 +9346,2952 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA38ED-18F1-4CB9-A8B5-69652EFF8644}">
+  <dimension ref="A1:AD81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="30" width="3.140625" customWidth="1"/>
+    <col min="31" max="31" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="H1" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2" s="42">
+        <v>12</v>
+      </c>
+      <c r="S2" s="42">
+        <v>13</v>
+      </c>
+      <c r="T2" s="42">
+        <v>14</v>
+      </c>
+      <c r="U2" s="42">
+        <v>15</v>
+      </c>
+      <c r="V2" s="42">
+        <v>16</v>
+      </c>
+      <c r="W2" s="42">
+        <v>17</v>
+      </c>
+      <c r="X2" s="42">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="42">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="42">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="42">
+        <v>21</v>
+      </c>
+      <c r="AB2">
+        <v>23</v>
+      </c>
+      <c r="AC2">
+        <v>24</v>
+      </c>
+      <c r="AD2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="58"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="58"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="26"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="27"/>
+      <c r="AD5" s="58"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="58"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>120</v>
+      </c>
+      <c r="C7">
+        <f>B7/5</f>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="36"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="58"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>195</v>
+      </c>
+      <c r="C8">
+        <f>B8/5</f>
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="36"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="58"/>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="36"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="36"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="58"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="36"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="36"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="58"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="58"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="32"/>
+      <c r="AB12" s="59"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="58"/>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="58"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>195</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="34"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="58"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="36"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="58"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="58"/>
+    </row>
+    <row r="17" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="58"/>
+    </row>
+    <row r="18" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="28"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="30"/>
+      <c r="AD18" s="58"/>
+    </row>
+    <row r="19" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="34"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="30"/>
+      <c r="AD19" s="58"/>
+    </row>
+    <row r="20" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="34"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="34"/>
+      <c r="Z20" s="36"/>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="30"/>
+      <c r="AD20" s="58"/>
+    </row>
+    <row r="21" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="30"/>
+      <c r="AD21" s="58"/>
+    </row>
+    <row r="22" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="30"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="58"/>
+    </row>
+    <row r="23" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="30"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="37"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="30"/>
+      <c r="AD23" s="58"/>
+    </row>
+    <row r="24" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="32"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="30"/>
+      <c r="AD24" s="58"/>
+    </row>
+    <row r="25" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="28"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="30"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="34"/>
+      <c r="X25" s="36"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="36"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="30"/>
+      <c r="AD25" s="58"/>
+    </row>
+    <row r="26" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="34"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="34"/>
+      <c r="Z26" s="36"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="30"/>
+      <c r="AD26" s="58"/>
+    </row>
+    <row r="27" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="28"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="34"/>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="36"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="30"/>
+      <c r="AD27" s="58"/>
+    </row>
+    <row r="28" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="28"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="36"/>
+      <c r="W28" s="34"/>
+      <c r="X28" s="36"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="36"/>
+      <c r="AA28" s="34"/>
+      <c r="AB28" s="28"/>
+      <c r="AC28" s="30"/>
+      <c r="AD28" s="58"/>
+    </row>
+    <row r="29" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="37"/>
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="28"/>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="58"/>
+    </row>
+    <row r="30" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="30"/>
+      <c r="V30" s="23"/>
+      <c r="W30" s="24"/>
+      <c r="X30" s="24"/>
+      <c r="Y30" s="24"/>
+      <c r="Z30" s="24"/>
+      <c r="AA30" s="60"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="58"/>
+    </row>
+    <row r="31" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="28"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="59"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="30"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="30"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="59"/>
+      <c r="AA31" s="30"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="58"/>
+    </row>
+    <row r="32" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="28"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="26"/>
+      <c r="P32" s="26"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="26"/>
+      <c r="X32" s="26"/>
+      <c r="Y32" s="26"/>
+      <c r="Z32" s="26"/>
+      <c r="AA32" s="27"/>
+      <c r="AB32" s="28"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="58"/>
+    </row>
+    <row r="33" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="28"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="31"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="31"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="32"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="30"/>
+      <c r="V33" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="W33" s="32"/>
+      <c r="X33" s="31"/>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="35"/>
+      <c r="AA33" s="32"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="58"/>
+    </row>
+    <row r="34" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="28"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="39"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="W34" s="38"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="38"/>
+      <c r="Z34" s="37"/>
+      <c r="AA34" s="38"/>
+      <c r="AB34" s="28"/>
+      <c r="AC34" s="30"/>
+      <c r="AD34" s="58"/>
+    </row>
+    <row r="35" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="28"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="61"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="34"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="W35" s="34"/>
+      <c r="X35" s="61"/>
+      <c r="Y35" s="34"/>
+      <c r="Z35" s="36"/>
+      <c r="AA35" s="34"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="30"/>
+      <c r="AD35" s="58"/>
+    </row>
+    <row r="36" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="28"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="61"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="61"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="61"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="W36" s="34"/>
+      <c r="X36" s="61"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="36"/>
+      <c r="AA36" s="34"/>
+      <c r="AB36" s="28"/>
+      <c r="AC36" s="30"/>
+      <c r="AD36" s="58"/>
+    </row>
+    <row r="37" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="36"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="28"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="36"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="61"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="36"/>
+      <c r="AA37" s="34"/>
+      <c r="AB37" s="28"/>
+      <c r="AC37" s="30"/>
+      <c r="AD37" s="58"/>
+    </row>
+    <row r="38" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="34"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="36"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="36"/>
+      <c r="W38" s="34"/>
+      <c r="X38" s="61"/>
+      <c r="Y38" s="34"/>
+      <c r="Z38" s="36"/>
+      <c r="AA38" s="34"/>
+      <c r="AB38" s="28"/>
+      <c r="AC38" s="30"/>
+      <c r="AD38" s="58"/>
+    </row>
+    <row r="39" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="28"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="61"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="61"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="36"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="30"/>
+      <c r="AD39" s="58"/>
+    </row>
+    <row r="40" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="28"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="61"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="36"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="61"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="36"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="28"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="58"/>
+    </row>
+    <row r="41" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="37"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="25"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="25"/>
+      <c r="U41" s="27"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="38"/>
+      <c r="X41" s="39"/>
+      <c r="Y41" s="38"/>
+      <c r="Z41" s="37"/>
+      <c r="AA41" s="38"/>
+      <c r="AB41" s="25"/>
+      <c r="AC41" s="27"/>
+      <c r="AD41" s="58"/>
+    </row>
+    <row r="42" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="58"/>
+      <c r="S42" s="58"/>
+      <c r="T42" s="58"/>
+      <c r="U42" s="58"/>
+      <c r="V42" s="58"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="58"/>
+      <c r="Y42" s="58"/>
+      <c r="Z42" s="58"/>
+      <c r="AA42" s="58"/>
+      <c r="AB42" s="58"/>
+      <c r="AC42" s="58"/>
+      <c r="AD42" s="58"/>
+    </row>
+    <row r="43" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="58"/>
+      <c r="S43" s="58"/>
+      <c r="T43" s="58"/>
+      <c r="U43" s="58"/>
+      <c r="V43" s="58"/>
+      <c r="W43" s="58"/>
+      <c r="X43" s="58"/>
+      <c r="Y43" s="58"/>
+      <c r="Z43" s="58"/>
+      <c r="AA43" s="58"/>
+      <c r="AB43" s="58"/>
+      <c r="AC43" s="58"/>
+      <c r="AD43" s="58"/>
+    </row>
+    <row r="44" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="58"/>
+      <c r="R44" s="58"/>
+      <c r="S44" s="58"/>
+      <c r="T44" s="58"/>
+      <c r="U44" s="58"/>
+      <c r="V44" s="58"/>
+      <c r="W44" s="58"/>
+      <c r="X44" s="58"/>
+      <c r="Y44" s="58"/>
+      <c r="Z44" s="58"/>
+      <c r="AA44" s="58"/>
+      <c r="AB44" s="58"/>
+      <c r="AC44" s="58"/>
+      <c r="AD44" s="58"/>
+    </row>
+    <row r="45" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
+      <c r="R45" s="58"/>
+      <c r="S45" s="58"/>
+      <c r="T45" s="58"/>
+      <c r="U45" s="58"/>
+      <c r="V45" s="58"/>
+      <c r="W45" s="58"/>
+      <c r="X45" s="58"/>
+      <c r="Y45" s="58"/>
+      <c r="Z45" s="58"/>
+      <c r="AA45" s="58"/>
+      <c r="AB45" s="58"/>
+      <c r="AC45" s="58"/>
+      <c r="AD45" s="58"/>
+    </row>
+    <row r="46" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="58"/>
+      <c r="R46" s="58"/>
+      <c r="S46" s="58"/>
+      <c r="T46" s="58"/>
+      <c r="U46" s="58"/>
+      <c r="V46" s="58"/>
+      <c r="W46" s="58"/>
+      <c r="X46" s="58"/>
+      <c r="Y46" s="58"/>
+      <c r="Z46" s="58"/>
+      <c r="AA46" s="58"/>
+      <c r="AB46" s="58"/>
+      <c r="AC46" s="58"/>
+      <c r="AD46" s="58"/>
+    </row>
+    <row r="47" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+      <c r="R47" s="58"/>
+      <c r="S47" s="58"/>
+      <c r="T47" s="58"/>
+      <c r="U47" s="58"/>
+      <c r="V47" s="58"/>
+      <c r="W47" s="58"/>
+      <c r="X47" s="58"/>
+      <c r="Y47" s="58"/>
+      <c r="Z47" s="58"/>
+      <c r="AA47" s="58"/>
+      <c r="AB47" s="58"/>
+      <c r="AC47" s="58"/>
+      <c r="AD47" s="58"/>
+    </row>
+    <row r="48" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+      <c r="R48" s="58"/>
+      <c r="S48" s="58"/>
+      <c r="T48" s="58"/>
+      <c r="U48" s="58"/>
+      <c r="V48" s="58"/>
+      <c r="W48" s="58"/>
+      <c r="X48" s="58"/>
+      <c r="Y48" s="58"/>
+      <c r="Z48" s="58"/>
+      <c r="AA48" s="58"/>
+      <c r="AB48" s="58"/>
+      <c r="AC48" s="58"/>
+      <c r="AD48" s="58"/>
+    </row>
+    <row r="49" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="58"/>
+      <c r="R49" s="58"/>
+      <c r="S49" s="58"/>
+      <c r="T49" s="58"/>
+      <c r="U49" s="58"/>
+      <c r="V49" s="58"/>
+      <c r="W49" s="58"/>
+      <c r="X49" s="58"/>
+      <c r="Y49" s="58"/>
+      <c r="Z49" s="58"/>
+      <c r="AA49" s="58"/>
+      <c r="AB49" s="58"/>
+      <c r="AC49" s="58"/>
+      <c r="AD49" s="58"/>
+    </row>
+    <row r="50" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="58"/>
+      <c r="R50" s="58"/>
+      <c r="S50" s="58"/>
+      <c r="T50" s="58"/>
+      <c r="U50" s="58"/>
+      <c r="V50" s="58"/>
+      <c r="W50" s="58"/>
+      <c r="X50" s="58"/>
+      <c r="Y50" s="58"/>
+      <c r="Z50" s="58"/>
+      <c r="AA50" s="58"/>
+      <c r="AB50" s="58"/>
+      <c r="AC50" s="58"/>
+      <c r="AD50" s="58"/>
+    </row>
+    <row r="51" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="58"/>
+      <c r="N51" s="58"/>
+      <c r="O51" s="58"/>
+      <c r="P51" s="58"/>
+      <c r="Q51" s="58"/>
+      <c r="R51" s="58"/>
+      <c r="S51" s="58"/>
+      <c r="T51" s="58"/>
+      <c r="U51" s="58"/>
+      <c r="V51" s="58"/>
+      <c r="W51" s="58"/>
+      <c r="X51" s="58"/>
+      <c r="Y51" s="58"/>
+      <c r="Z51" s="58"/>
+      <c r="AA51" s="58"/>
+      <c r="AB51" s="58"/>
+      <c r="AC51" s="58"/>
+      <c r="AD51" s="58"/>
+    </row>
+    <row r="52" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="58"/>
+      <c r="R52" s="58"/>
+      <c r="S52" s="58"/>
+      <c r="T52" s="58"/>
+      <c r="U52" s="58"/>
+      <c r="V52" s="58"/>
+      <c r="W52" s="58"/>
+      <c r="X52" s="58"/>
+      <c r="Y52" s="58"/>
+      <c r="Z52" s="58"/>
+      <c r="AA52" s="58"/>
+      <c r="AB52" s="58"/>
+      <c r="AC52" s="58"/>
+      <c r="AD52" s="58"/>
+    </row>
+    <row r="53" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
+      <c r="P53" s="58"/>
+      <c r="Q53" s="58"/>
+      <c r="R53" s="58"/>
+      <c r="S53" s="58"/>
+      <c r="T53" s="58"/>
+      <c r="U53" s="58"/>
+      <c r="V53" s="58"/>
+      <c r="W53" s="58"/>
+      <c r="X53" s="58"/>
+      <c r="Y53" s="58"/>
+      <c r="Z53" s="58"/>
+      <c r="AA53" s="58"/>
+      <c r="AB53" s="58"/>
+      <c r="AC53" s="58"/>
+      <c r="AD53" s="58"/>
+    </row>
+    <row r="54" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="58"/>
+      <c r="R54" s="58"/>
+      <c r="S54" s="58"/>
+      <c r="T54" s="58"/>
+      <c r="U54" s="58"/>
+      <c r="V54" s="58"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
+      <c r="Y54" s="58"/>
+      <c r="Z54" s="58"/>
+      <c r="AA54" s="58"/>
+      <c r="AB54" s="58"/>
+      <c r="AC54" s="58"/>
+      <c r="AD54" s="58"/>
+    </row>
+    <row r="55" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="58"/>
+      <c r="J55" s="58"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+      <c r="R55" s="58"/>
+      <c r="S55" s="58"/>
+      <c r="T55" s="58"/>
+      <c r="U55" s="58"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+      <c r="Z55" s="58"/>
+      <c r="AA55" s="58"/>
+      <c r="AB55" s="58"/>
+      <c r="AC55" s="58"/>
+      <c r="AD55" s="58"/>
+    </row>
+    <row r="56" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
+      <c r="P56" s="58"/>
+      <c r="Q56" s="58"/>
+      <c r="R56" s="58"/>
+      <c r="S56" s="58"/>
+      <c r="T56" s="58"/>
+      <c r="U56" s="58"/>
+      <c r="V56" s="58"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
+      <c r="Y56" s="58"/>
+      <c r="Z56" s="58"/>
+      <c r="AA56" s="58"/>
+      <c r="AB56" s="58"/>
+      <c r="AC56" s="58"/>
+      <c r="AD56" s="58"/>
+    </row>
+    <row r="57" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
+      <c r="P57" s="58"/>
+      <c r="Q57" s="58"/>
+      <c r="R57" s="58"/>
+      <c r="S57" s="58"/>
+      <c r="T57" s="58"/>
+      <c r="U57" s="58"/>
+      <c r="V57" s="58"/>
+      <c r="W57" s="58"/>
+      <c r="X57" s="58"/>
+      <c r="Y57" s="58"/>
+      <c r="Z57" s="58"/>
+      <c r="AA57" s="58"/>
+      <c r="AB57" s="58"/>
+      <c r="AC57" s="58"/>
+      <c r="AD57" s="58"/>
+    </row>
+    <row r="58" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="42"/>
+      <c r="P58" s="42"/>
+      <c r="Q58" s="42"/>
+      <c r="R58" s="42"/>
+      <c r="S58" s="42"/>
+      <c r="T58" s="42"/>
+      <c r="U58" s="42"/>
+      <c r="V58" s="42"/>
+      <c r="W58" s="42"/>
+      <c r="X58" s="42"/>
+      <c r="Y58" s="42"/>
+      <c r="Z58" s="42"/>
+      <c r="AA58" s="42"/>
+      <c r="AB58" s="42"/>
+      <c r="AC58" s="42"/>
+      <c r="AD58" s="58"/>
+    </row>
+    <row r="59" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD59" s="58"/>
+    </row>
+    <row r="60" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD60" s="58"/>
+    </row>
+    <row r="61" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD61" s="58"/>
+    </row>
+    <row r="62" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD62" s="58"/>
+    </row>
+    <row r="63" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD63" s="58"/>
+    </row>
+    <row r="64" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="AD64" s="58"/>
+    </row>
+    <row r="65" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD65" s="58"/>
+    </row>
+    <row r="66" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD66" s="58"/>
+    </row>
+    <row r="67" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD67" s="58"/>
+    </row>
+    <row r="68" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD68" s="58"/>
+    </row>
+    <row r="69" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD69" s="58"/>
+    </row>
+    <row r="70" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD70" s="58"/>
+    </row>
+    <row r="71" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD71" s="58"/>
+    </row>
+    <row r="72" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD72" s="58"/>
+    </row>
+    <row r="73" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD73" s="58"/>
+    </row>
+    <row r="74" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD74" s="58"/>
+    </row>
+    <row r="75" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD75" s="58"/>
+    </row>
+    <row r="76" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD76" s="58"/>
+    </row>
+    <row r="77" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD77" s="58"/>
+    </row>
+    <row r="78" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD78" s="58"/>
+    </row>
+    <row r="79" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD79" s="58"/>
+    </row>
+    <row r="80" spans="30:30" x14ac:dyDescent="0.25">
+      <c r="AD80" s="42"/>
+    </row>
+    <row r="81" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="G81" s="42"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="42"/>
+      <c r="P81" s="42"/>
+      <c r="Q81" s="42"/>
+      <c r="R81" s="42"/>
+      <c r="S81" s="42"/>
+      <c r="T81" s="42"/>
+      <c r="U81" s="42"/>
+      <c r="V81" s="42"/>
+      <c r="W81" s="42"/>
+      <c r="X81" s="42"/>
+      <c r="Y81" s="42"/>
+      <c r="Z81" s="42"/>
+      <c r="AA81" s="42"/>
+      <c r="AB81" s="42"/>
+      <c r="AC81" s="42"/>
+      <c r="AD81" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37977C-A20A-4B26-8AC1-43F48BE9948E}">
+  <dimension ref="A1:Q81"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="17" width="3.140625" customWidth="1"/>
+    <col min="18" max="18" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G1" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G2" s="42">
+        <v>1</v>
+      </c>
+      <c r="H2" s="42">
+        <v>2</v>
+      </c>
+      <c r="I2" s="42">
+        <v>3</v>
+      </c>
+      <c r="J2" s="42">
+        <v>4</v>
+      </c>
+      <c r="K2" s="42">
+        <v>5</v>
+      </c>
+      <c r="L2" s="42">
+        <v>6</v>
+      </c>
+      <c r="M2" s="42">
+        <v>7</v>
+      </c>
+      <c r="N2" s="42">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="58"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="58"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="58"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="58"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>120</v>
+      </c>
+      <c r="C7">
+        <f>B7/5</f>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="58"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>195</v>
+      </c>
+      <c r="C8">
+        <f>B8/5</f>
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="58"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="58"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="58"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="58"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>39</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="58"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>50</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="58"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>195</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="58"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="58"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="58"/>
+    </row>
+    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="58"/>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="28"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="58"/>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="58"/>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="58"/>
+    </row>
+    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="58"/>
+    </row>
+    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="28"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="58"/>
+    </row>
+    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="28"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="58"/>
+    </row>
+    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="58"/>
+    </row>
+    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="28"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="58"/>
+    </row>
+    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="58"/>
+    </row>
+    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="28"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="58"/>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="28"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="58"/>
+    </row>
+    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="58"/>
+    </row>
+    <row r="30" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="58"/>
+    </row>
+    <row r="31" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="28"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="58"/>
+    </row>
+    <row r="32" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="28"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="58"/>
+    </row>
+    <row r="33" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="28"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="32"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="30"/>
+      <c r="Q33" s="58"/>
+    </row>
+    <row r="34" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="28"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="38"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="58"/>
+    </row>
+    <row r="35" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="28"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="34"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="34"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="30"/>
+      <c r="Q35" s="58"/>
+    </row>
+    <row r="36" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="28"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="34"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="30"/>
+      <c r="Q36" s="58"/>
+    </row>
+    <row r="37" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="30"/>
+      <c r="Q37" s="58"/>
+    </row>
+    <row r="38" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="58"/>
+    </row>
+    <row r="39" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="28"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="34"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="30"/>
+      <c r="Q39" s="58"/>
+    </row>
+    <row r="40" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="28"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="34"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="58"/>
+    </row>
+    <row r="41" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="27"/>
+      <c r="Q41" s="58"/>
+    </row>
+    <row r="42" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+    </row>
+    <row r="43" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+    </row>
+    <row r="44" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="58"/>
+    </row>
+    <row r="45" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
+    </row>
+    <row r="46" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="58"/>
+    </row>
+    <row r="47" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+    </row>
+    <row r="48" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
+      <c r="P48" s="58"/>
+      <c r="Q48" s="58"/>
+    </row>
+    <row r="49" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
+      <c r="P49" s="58"/>
+      <c r="Q49" s="58"/>
+    </row>
+    <row r="50" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="58"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="58"/>
+    </row>
+    <row r="51" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="58"/>
+      <c r="N51" s="58"/>
+      <c r="O51" s="58"/>
+      <c r="P51" s="58"/>
+      <c r="Q51" s="58"/>
+    </row>
+    <row r="52" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="58"/>
+    </row>
+    <row r="53" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="58"/>
+      <c r="K53" s="58"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="58"/>
+      <c r="N53" s="58"/>
+      <c r="O53" s="58"/>
+      <c r="P53" s="58"/>
+      <c r="Q53" s="58"/>
+    </row>
+    <row r="54" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
+      <c r="M54" s="58"/>
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="58"/>
+    </row>
+    <row r="55" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="58"/>
+      <c r="J55" s="58"/>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+    </row>
+    <row r="56" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
+      <c r="P56" s="58"/>
+      <c r="Q56" s="58"/>
+    </row>
+    <row r="57" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G57" s="58"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
+      <c r="P57" s="58"/>
+      <c r="Q57" s="58"/>
+    </row>
+    <row r="58" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="42"/>
+      <c r="O58" s="42"/>
+      <c r="P58" s="42"/>
+      <c r="Q58" s="58"/>
+    </row>
+    <row r="59" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q59" s="58"/>
+    </row>
+    <row r="60" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q60" s="58"/>
+    </row>
+    <row r="61" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q61" s="58"/>
+    </row>
+    <row r="62" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q62" s="58"/>
+    </row>
+    <row r="63" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q63" s="58"/>
+    </row>
+    <row r="64" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="Q64" s="58"/>
+    </row>
+    <row r="65" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q65" s="58"/>
+    </row>
+    <row r="66" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q66" s="58"/>
+    </row>
+    <row r="67" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q67" s="58"/>
+    </row>
+    <row r="68" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q68" s="58"/>
+    </row>
+    <row r="69" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q69" s="58"/>
+    </row>
+    <row r="70" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q70" s="58"/>
+    </row>
+    <row r="71" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q71" s="58"/>
+    </row>
+    <row r="72" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q72" s="58"/>
+    </row>
+    <row r="73" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q73" s="58"/>
+    </row>
+    <row r="74" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q74" s="58"/>
+    </row>
+    <row r="75" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q75" s="58"/>
+    </row>
+    <row r="76" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q76" s="58"/>
+    </row>
+    <row r="77" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q77" s="58"/>
+    </row>
+    <row r="78" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q78" s="58"/>
+    </row>
+    <row r="79" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q79" s="58"/>
+    </row>
+    <row r="80" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q80" s="42"/>
+    </row>
+    <row r="81" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G81" s="42"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="42"/>
+      <c r="M81" s="42"/>
+      <c r="N81" s="42"/>
+      <c r="O81" s="42"/>
+      <c r="P81" s="42"/>
+      <c r="Q81" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add complete structure in html and css for Building 4
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="680" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44C1A61D-465B-4E17-B9C5-B75D4F865C35}"/>
+  <xr:revisionPtr revIDLastSave="693" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{837FFD54-CCCF-42AA-8739-3DE7FCDF1896}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="6" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
@@ -9352,9 +9352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA38ED-18F1-4CB9-A8B5-69652EFF8644}">
   <dimension ref="A1:AD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9582,11 +9582,11 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="C7">
         <f>B7/5</f>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -9627,11 +9627,11 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>195</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <f>B8/5</f>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
@@ -9641,7 +9641,9 @@
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="30"/>
-      <c r="I8" s="36"/>
+      <c r="I8" s="36">
+        <v>5</v>
+      </c>
       <c r="J8" s="61"/>
       <c r="K8" s="34"/>
       <c r="L8" s="36"/>
@@ -9855,7 +9857,9 @@
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="30"/>
-      <c r="I14" s="36"/>
+      <c r="I14" s="36">
+        <v>4</v>
+      </c>
       <c r="J14" s="61"/>
       <c r="K14" s="34"/>
       <c r="L14" s="36"/>
@@ -10029,7 +10033,9 @@
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="30"/>
-      <c r="I20" s="36"/>
+      <c r="I20" s="36">
+        <v>3</v>
+      </c>
       <c r="J20" s="61"/>
       <c r="K20" s="34"/>
       <c r="L20" s="36"/>
@@ -10203,7 +10209,9 @@
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="30"/>
-      <c r="I26" s="36"/>
+      <c r="I26" s="36">
+        <v>2</v>
+      </c>
       <c r="J26" s="61"/>
       <c r="K26" s="34"/>
       <c r="L26" s="36"/>
@@ -10596,7 +10604,9 @@
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="30"/>
-      <c r="I39" s="36"/>
+      <c r="I39" s="36">
+        <v>1</v>
+      </c>
       <c r="J39" s="61"/>
       <c r="K39" s="34"/>
       <c r="L39" s="36"/>
@@ -11223,9 +11233,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37977C-A20A-4B26-8AC1-43F48BE9948E}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11356,11 +11366,11 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>120</v>
+        <v>195</v>
       </c>
       <c r="C7">
         <f>B7/5</f>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -11388,11 +11398,11 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <f>B8/5</f>
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Add windows to B4 Half 1
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="693" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{837FFD54-CCCF-42AA-8739-3DE7FCDF1896}"/>
+  <xr:revisionPtr revIDLastSave="700" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6292DC1B-9EAD-4CD1-BA06-7EB1201697EC}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="6" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="5" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="45">
   <si>
     <t>Columns</t>
   </si>
@@ -9350,26 +9350,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA38ED-18F1-4CB9-A8B5-69652EFF8644}">
-  <dimension ref="A1:AD81"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="30" width="3.140625" customWidth="1"/>
-    <col min="31" max="31" width="3" customWidth="1"/>
+    <col min="6" max="20" width="3.140625" customWidth="1"/>
+    <col min="21" max="21" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H1" s="40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G2">
         <v>1</v>
       </c>
@@ -9409,41 +9409,11 @@
       <c r="S2" s="42">
         <v>13</v>
       </c>
-      <c r="T2" s="42">
+      <c r="T2">
         <v>14</v>
       </c>
-      <c r="U2" s="42">
-        <v>15</v>
-      </c>
-      <c r="V2" s="42">
-        <v>16</v>
-      </c>
-      <c r="W2" s="42">
-        <v>17</v>
-      </c>
-      <c r="X2" s="42">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="42">
-        <v>19</v>
-      </c>
-      <c r="Z2" s="42">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="42">
-        <v>21</v>
-      </c>
-      <c r="AB2">
-        <v>23</v>
-      </c>
-      <c r="AC2">
-        <v>24</v>
-      </c>
-      <c r="AD2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F3">
         <v>1</v>
       </c>
@@ -9462,21 +9432,9 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
       <c r="S3" s="24"/>
-      <c r="T3" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="58"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T3" s="58"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>2</v>
       </c>
@@ -9495,21 +9453,9 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="59"/>
       <c r="S4" s="59"/>
-      <c r="T4" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="58"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T4" s="58"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>3</v>
       </c>
@@ -9526,19 +9472,9 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="26"/>
       <c r="S5" s="26"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="27"/>
-      <c r="AD5" s="58"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T5" s="58"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
         <v>13</v>
       </c>
@@ -9563,21 +9499,9 @@
       <c r="Q6" s="34"/>
       <c r="R6" s="28"/>
       <c r="S6" s="30"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="34"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="58"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T6" s="58"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>10</v>
       </c>
@@ -9610,19 +9534,9 @@
       <c r="Q7" s="34"/>
       <c r="R7" s="28"/>
       <c r="S7" s="30"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="34"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="36"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="30"/>
-      <c r="AD7" s="58"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T7" s="58"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>11</v>
       </c>
@@ -9642,7 +9556,7 @@
       <c r="G8" s="28"/>
       <c r="H8" s="30"/>
       <c r="I8" s="36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8" s="61"/>
       <c r="K8" s="34"/>
@@ -9654,19 +9568,9 @@
       <c r="Q8" s="34"/>
       <c r="R8" s="28"/>
       <c r="S8" s="30"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="34"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="34"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="34"/>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="58"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T8" s="58"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>7</v>
       </c>
@@ -9683,19 +9587,9 @@
       <c r="Q9" s="34"/>
       <c r="R9" s="28"/>
       <c r="S9" s="30"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="34"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="34"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="34"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="58"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T9" s="58"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
         <v>32</v>
       </c>
@@ -9718,19 +9612,9 @@
       <c r="Q10" s="34"/>
       <c r="R10" s="28"/>
       <c r="S10" s="30"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="34"/>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="34"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="58"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T10" s="58"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>35</v>
       </c>
@@ -9753,19 +9637,9 @@
       <c r="Q11" s="38"/>
       <c r="R11" s="28"/>
       <c r="S11" s="30"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="37"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="28"/>
-      <c r="AC11" s="30"/>
-      <c r="AD11" s="58"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T11" s="58"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>34</v>
       </c>
@@ -9788,19 +9662,9 @@
       <c r="Q12" s="32"/>
       <c r="R12" s="59"/>
       <c r="S12" s="30"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="35"/>
-      <c r="AA12" s="32"/>
-      <c r="AB12" s="59"/>
-      <c r="AC12" s="30"/>
-      <c r="AD12" s="58"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T12" s="58"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -9828,19 +9692,9 @@
       <c r="Q13" s="34"/>
       <c r="R13" s="28"/>
       <c r="S13" s="30"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="36"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="30"/>
-      <c r="AD13" s="58"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T13" s="58"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -9858,7 +9712,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="30"/>
       <c r="I14" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J14" s="61"/>
       <c r="K14" s="34"/>
@@ -9870,19 +9724,9 @@
       <c r="Q14" s="34"/>
       <c r="R14" s="28"/>
       <c r="S14" s="30"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="34"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="34"/>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="30"/>
-      <c r="AD14" s="58"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T14" s="58"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>13</v>
       </c>
@@ -9899,19 +9743,9 @@
       <c r="Q15" s="34"/>
       <c r="R15" s="28"/>
       <c r="S15" s="30"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="34"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="34"/>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="34"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="58"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="T15" s="58"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>14</v>
       </c>
@@ -9928,19 +9762,9 @@
       <c r="Q16" s="34"/>
       <c r="R16" s="28"/>
       <c r="S16" s="30"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="34"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="34"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="30"/>
-      <c r="AD16" s="58"/>
-    </row>
-    <row r="17" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T16" s="58"/>
+    </row>
+    <row r="17" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>15</v>
       </c>
@@ -9957,19 +9781,9 @@
       <c r="Q17" s="38"/>
       <c r="R17" s="28"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="30"/>
-      <c r="AD17" s="58"/>
-    </row>
-    <row r="18" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T17" s="58"/>
+    </row>
+    <row r="18" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>16</v>
       </c>
@@ -9986,19 +9800,9 @@
       <c r="Q18" s="32"/>
       <c r="R18" s="28"/>
       <c r="S18" s="30"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="30"/>
-      <c r="AD18" s="58"/>
-    </row>
-    <row r="19" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T18" s="58"/>
+    </row>
+    <row r="19" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>17</v>
       </c>
@@ -10015,26 +9819,16 @@
       <c r="Q19" s="34"/>
       <c r="R19" s="28"/>
       <c r="S19" s="30"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="36"/>
-      <c r="Y19" s="34"/>
-      <c r="Z19" s="36"/>
-      <c r="AA19" s="34"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="30"/>
-      <c r="AD19" s="58"/>
-    </row>
-    <row r="20" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T19" s="58"/>
+    </row>
+    <row r="20" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>18</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="30"/>
       <c r="I20" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="61"/>
       <c r="K20" s="34"/>
@@ -10046,19 +9840,9 @@
       <c r="Q20" s="34"/>
       <c r="R20" s="28"/>
       <c r="S20" s="30"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="30"/>
-      <c r="AD20" s="58"/>
-    </row>
-    <row r="21" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T20" s="58"/>
+    </row>
+    <row r="21" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>19</v>
       </c>
@@ -10075,19 +9859,9 @@
       <c r="Q21" s="34"/>
       <c r="R21" s="28"/>
       <c r="S21" s="30"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="30"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="34"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="34"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="58"/>
-    </row>
-    <row r="22" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T21" s="58"/>
+    </row>
+    <row r="22" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>20</v>
       </c>
@@ -10104,19 +9878,9 @@
       <c r="Q22" s="34"/>
       <c r="R22" s="28"/>
       <c r="S22" s="30"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="30"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="34"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="30"/>
-      <c r="AD22" s="58"/>
-    </row>
-    <row r="23" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T22" s="58"/>
+    </row>
+    <row r="23" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>21</v>
       </c>
@@ -10133,19 +9897,9 @@
       <c r="Q23" s="38"/>
       <c r="R23" s="28"/>
       <c r="S23" s="30"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="38"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="38"/>
-      <c r="Z23" s="37"/>
-      <c r="AA23" s="38"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="30"/>
-      <c r="AD23" s="58"/>
-    </row>
-    <row r="24" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T23" s="58"/>
+    </row>
+    <row r="24" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>22</v>
       </c>
@@ -10162,19 +9916,9 @@
       <c r="Q24" s="32"/>
       <c r="R24" s="28"/>
       <c r="S24" s="30"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="32"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="30"/>
-      <c r="AD24" s="58"/>
-    </row>
-    <row r="25" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T24" s="58"/>
+    </row>
+    <row r="25" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>23</v>
       </c>
@@ -10191,26 +9935,16 @@
       <c r="Q25" s="34"/>
       <c r="R25" s="28"/>
       <c r="S25" s="30"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="34"/>
-      <c r="X25" s="36"/>
-      <c r="Y25" s="34"/>
-      <c r="Z25" s="36"/>
-      <c r="AA25" s="34"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="58"/>
-    </row>
-    <row r="26" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T25" s="58"/>
+    </row>
+    <row r="26" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>24</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="30"/>
       <c r="I26" s="36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J26" s="61"/>
       <c r="K26" s="34"/>
@@ -10222,19 +9956,9 @@
       <c r="Q26" s="34"/>
       <c r="R26" s="28"/>
       <c r="S26" s="30"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="36"/>
-      <c r="W26" s="34"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="34"/>
-      <c r="Z26" s="36"/>
-      <c r="AA26" s="34"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="58"/>
-    </row>
-    <row r="27" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T26" s="58"/>
+    </row>
+    <row r="27" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>25</v>
       </c>
@@ -10251,19 +9975,9 @@
       <c r="Q27" s="34"/>
       <c r="R27" s="28"/>
       <c r="S27" s="30"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="36"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="36"/>
-      <c r="Y27" s="34"/>
-      <c r="Z27" s="36"/>
-      <c r="AA27" s="34"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="58"/>
-    </row>
-    <row r="28" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T27" s="58"/>
+    </row>
+    <row r="28" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>26</v>
       </c>
@@ -10280,19 +9994,9 @@
       <c r="Q28" s="34"/>
       <c r="R28" s="28"/>
       <c r="S28" s="30"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="34"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="36"/>
-      <c r="AA28" s="34"/>
-      <c r="AB28" s="28"/>
-      <c r="AC28" s="30"/>
-      <c r="AD28" s="58"/>
-    </row>
-    <row r="29" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T28" s="58"/>
+    </row>
+    <row r="29" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F29">
         <v>27</v>
       </c>
@@ -10309,19 +10013,9 @@
       <c r="Q29" s="38"/>
       <c r="R29" s="28"/>
       <c r="S29" s="30"/>
-      <c r="T29" s="28"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="37"/>
-      <c r="W29" s="38"/>
-      <c r="X29" s="37"/>
-      <c r="Y29" s="38"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="38"/>
-      <c r="AB29" s="28"/>
-      <c r="AC29" s="30"/>
-      <c r="AD29" s="58"/>
-    </row>
-    <row r="30" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T29" s="58"/>
+    </row>
+    <row r="30" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F30">
         <v>28</v>
       </c>
@@ -10338,19 +10032,9 @@
       <c r="Q30" s="60"/>
       <c r="R30" s="28"/>
       <c r="S30" s="30"/>
-      <c r="T30" s="28"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="60"/>
-      <c r="AB30" s="28"/>
-      <c r="AC30" s="30"/>
-      <c r="AD30" s="58"/>
-    </row>
-    <row r="31" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T30" s="58"/>
+    </row>
+    <row r="31" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F31">
         <v>29</v>
       </c>
@@ -10367,19 +10051,9 @@
       <c r="Q31" s="30"/>
       <c r="R31" s="28"/>
       <c r="S31" s="30"/>
-      <c r="T31" s="28"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="28"/>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="59"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="28"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="58"/>
-    </row>
-    <row r="32" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T31" s="58"/>
+    </row>
+    <row r="32" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F32">
         <v>30</v>
       </c>
@@ -10396,19 +10070,9 @@
       <c r="Q32" s="27"/>
       <c r="R32" s="28"/>
       <c r="S32" s="30"/>
-      <c r="T32" s="28"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="25"/>
-      <c r="W32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="26"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="27"/>
-      <c r="AB32" s="28"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="58"/>
-    </row>
-    <row r="33" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T32" s="58"/>
+    </row>
+    <row r="33" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>31</v>
       </c>
@@ -10427,21 +10091,9 @@
       <c r="Q33" s="32"/>
       <c r="R33" s="28"/>
       <c r="S33" s="30"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="W33" s="32"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="32"/>
-      <c r="Z33" s="35"/>
-      <c r="AA33" s="32"/>
-      <c r="AB33" s="28"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="58"/>
-    </row>
-    <row r="34" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T33" s="58"/>
+    </row>
+    <row r="34" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>32</v>
       </c>
@@ -10451,7 +10103,9 @@
         <v>6</v>
       </c>
       <c r="J34" s="39"/>
-      <c r="K34" s="38"/>
+      <c r="K34" s="38">
+        <v>2</v>
+      </c>
       <c r="L34" s="37"/>
       <c r="M34" s="39"/>
       <c r="N34" s="38"/>
@@ -10460,21 +10114,9 @@
       <c r="Q34" s="38"/>
       <c r="R34" s="28"/>
       <c r="S34" s="30"/>
-      <c r="T34" s="28"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="W34" s="38"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="38"/>
-      <c r="Z34" s="37"/>
-      <c r="AA34" s="38"/>
-      <c r="AB34" s="28"/>
-      <c r="AC34" s="30"/>
-      <c r="AD34" s="58"/>
-    </row>
-    <row r="35" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T34" s="58"/>
+    </row>
+    <row r="35" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>33</v>
       </c>
@@ -10493,21 +10135,9 @@
       <c r="Q35" s="34"/>
       <c r="R35" s="28"/>
       <c r="S35" s="30"/>
-      <c r="T35" s="28"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="W35" s="34"/>
-      <c r="X35" s="61"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="36"/>
-      <c r="AA35" s="34"/>
-      <c r="AB35" s="28"/>
-      <c r="AC35" s="30"/>
-      <c r="AD35" s="58"/>
-    </row>
-    <row r="36" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T35" s="58"/>
+    </row>
+    <row r="36" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>34</v>
       </c>
@@ -10526,21 +10156,9 @@
       <c r="Q36" s="34"/>
       <c r="R36" s="28"/>
       <c r="S36" s="30"/>
-      <c r="T36" s="28"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="W36" s="34"/>
-      <c r="X36" s="61"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="36"/>
-      <c r="AA36" s="34"/>
-      <c r="AB36" s="28"/>
-      <c r="AC36" s="30"/>
-      <c r="AD36" s="58"/>
-    </row>
-    <row r="37" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T36" s="58"/>
+    </row>
+    <row r="37" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>35</v>
       </c>
@@ -10557,19 +10175,9 @@
       <c r="Q37" s="34"/>
       <c r="R37" s="28"/>
       <c r="S37" s="30"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="34"/>
-      <c r="X37" s="61"/>
-      <c r="Y37" s="34"/>
-      <c r="Z37" s="36"/>
-      <c r="AA37" s="34"/>
-      <c r="AB37" s="28"/>
-      <c r="AC37" s="30"/>
-      <c r="AD37" s="58"/>
-    </row>
-    <row r="38" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T37" s="58"/>
+    </row>
+    <row r="38" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>36</v>
       </c>
@@ -10586,19 +10194,9 @@
       <c r="Q38" s="34"/>
       <c r="R38" s="28"/>
       <c r="S38" s="30"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="34"/>
-      <c r="X38" s="61"/>
-      <c r="Y38" s="34"/>
-      <c r="Z38" s="36"/>
-      <c r="AA38" s="34"/>
-      <c r="AB38" s="28"/>
-      <c r="AC38" s="30"/>
-      <c r="AD38" s="58"/>
-    </row>
-    <row r="39" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T38" s="58"/>
+    </row>
+    <row r="39" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>37</v>
       </c>
@@ -10617,19 +10215,9 @@
       <c r="Q39" s="34"/>
       <c r="R39" s="28"/>
       <c r="S39" s="30"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="34"/>
-      <c r="X39" s="61"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="36"/>
-      <c r="AA39" s="34"/>
-      <c r="AB39" s="28"/>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="58"/>
-    </row>
-    <row r="40" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T39" s="58"/>
+    </row>
+    <row r="40" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>38</v>
       </c>
@@ -10646,19 +10234,9 @@
       <c r="Q40" s="34"/>
       <c r="R40" s="28"/>
       <c r="S40" s="30"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="30"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="34"/>
-      <c r="X40" s="61"/>
-      <c r="Y40" s="34"/>
-      <c r="Z40" s="36"/>
-      <c r="AA40" s="34"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="58"/>
-    </row>
-    <row r="41" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T40" s="58"/>
+    </row>
+    <row r="41" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>39</v>
       </c>
@@ -10675,19 +10253,9 @@
       <c r="Q41" s="38"/>
       <c r="R41" s="25"/>
       <c r="S41" s="27"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="38"/>
-      <c r="X41" s="39"/>
-      <c r="Y41" s="38"/>
-      <c r="Z41" s="37"/>
-      <c r="AA41" s="38"/>
-      <c r="AB41" s="25"/>
-      <c r="AC41" s="27"/>
-      <c r="AD41" s="58"/>
-    </row>
-    <row r="42" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="T41" s="58"/>
+    </row>
+    <row r="42" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>40</v>
       </c>
@@ -10705,18 +10273,8 @@
       <c r="R42" s="58"/>
       <c r="S42" s="58"/>
       <c r="T42" s="58"/>
-      <c r="U42" s="58"/>
-      <c r="V42" s="58"/>
-      <c r="W42" s="58"/>
-      <c r="X42" s="58"/>
-      <c r="Y42" s="58"/>
-      <c r="Z42" s="58"/>
-      <c r="AA42" s="58"/>
-      <c r="AB42" s="58"/>
-      <c r="AC42" s="58"/>
-      <c r="AD42" s="58"/>
-    </row>
-    <row r="43" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G43" s="58"/>
       <c r="H43" s="58"/>
       <c r="I43" s="58"/>
@@ -10731,18 +10289,8 @@
       <c r="R43" s="58"/>
       <c r="S43" s="58"/>
       <c r="T43" s="58"/>
-      <c r="U43" s="58"/>
-      <c r="V43" s="58"/>
-      <c r="W43" s="58"/>
-      <c r="X43" s="58"/>
-      <c r="Y43" s="58"/>
-      <c r="Z43" s="58"/>
-      <c r="AA43" s="58"/>
-      <c r="AB43" s="58"/>
-      <c r="AC43" s="58"/>
-      <c r="AD43" s="58"/>
-    </row>
-    <row r="44" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G44" s="58"/>
       <c r="H44" s="58"/>
       <c r="I44" s="58"/>
@@ -10757,18 +10305,8 @@
       <c r="R44" s="58"/>
       <c r="S44" s="58"/>
       <c r="T44" s="58"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="58"/>
-      <c r="X44" s="58"/>
-      <c r="Y44" s="58"/>
-      <c r="Z44" s="58"/>
-      <c r="AA44" s="58"/>
-      <c r="AB44" s="58"/>
-      <c r="AC44" s="58"/>
-      <c r="AD44" s="58"/>
-    </row>
-    <row r="45" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G45" s="58"/>
       <c r="H45" s="58"/>
       <c r="I45" s="58"/>
@@ -10783,18 +10321,8 @@
       <c r="R45" s="58"/>
       <c r="S45" s="58"/>
       <c r="T45" s="58"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="58"/>
-      <c r="W45" s="58"/>
-      <c r="X45" s="58"/>
-      <c r="Y45" s="58"/>
-      <c r="Z45" s="58"/>
-      <c r="AA45" s="58"/>
-      <c r="AB45" s="58"/>
-      <c r="AC45" s="58"/>
-      <c r="AD45" s="58"/>
-    </row>
-    <row r="46" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G46" s="58"/>
       <c r="H46" s="58"/>
       <c r="I46" s="58"/>
@@ -10809,18 +10337,8 @@
       <c r="R46" s="58"/>
       <c r="S46" s="58"/>
       <c r="T46" s="58"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="58"/>
-      <c r="W46" s="58"/>
-      <c r="X46" s="58"/>
-      <c r="Y46" s="58"/>
-      <c r="Z46" s="58"/>
-      <c r="AA46" s="58"/>
-      <c r="AB46" s="58"/>
-      <c r="AC46" s="58"/>
-      <c r="AD46" s="58"/>
-    </row>
-    <row r="47" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G47" s="58"/>
       <c r="H47" s="58"/>
       <c r="I47" s="58"/>
@@ -10835,18 +10353,8 @@
       <c r="R47" s="58"/>
       <c r="S47" s="58"/>
       <c r="T47" s="58"/>
-      <c r="U47" s="58"/>
-      <c r="V47" s="58"/>
-      <c r="W47" s="58"/>
-      <c r="X47" s="58"/>
-      <c r="Y47" s="58"/>
-      <c r="Z47" s="58"/>
-      <c r="AA47" s="58"/>
-      <c r="AB47" s="58"/>
-      <c r="AC47" s="58"/>
-      <c r="AD47" s="58"/>
-    </row>
-    <row r="48" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G48" s="58"/>
       <c r="H48" s="58"/>
       <c r="I48" s="58"/>
@@ -10861,18 +10369,8 @@
       <c r="R48" s="58"/>
       <c r="S48" s="58"/>
       <c r="T48" s="58"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
-      <c r="Z48" s="58"/>
-      <c r="AA48" s="58"/>
-      <c r="AB48" s="58"/>
-      <c r="AC48" s="58"/>
-      <c r="AD48" s="58"/>
-    </row>
-    <row r="49" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G49" s="58"/>
       <c r="H49" s="58"/>
       <c r="I49" s="58"/>
@@ -10887,18 +10385,8 @@
       <c r="R49" s="58"/>
       <c r="S49" s="58"/>
       <c r="T49" s="58"/>
-      <c r="U49" s="58"/>
-      <c r="V49" s="58"/>
-      <c r="W49" s="58"/>
-      <c r="X49" s="58"/>
-      <c r="Y49" s="58"/>
-      <c r="Z49" s="58"/>
-      <c r="AA49" s="58"/>
-      <c r="AB49" s="58"/>
-      <c r="AC49" s="58"/>
-      <c r="AD49" s="58"/>
-    </row>
-    <row r="50" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G50" s="58"/>
       <c r="H50" s="58"/>
       <c r="I50" s="58"/>
@@ -10913,18 +10401,8 @@
       <c r="R50" s="58"/>
       <c r="S50" s="58"/>
       <c r="T50" s="58"/>
-      <c r="U50" s="58"/>
-      <c r="V50" s="58"/>
-      <c r="W50" s="58"/>
-      <c r="X50" s="58"/>
-      <c r="Y50" s="58"/>
-      <c r="Z50" s="58"/>
-      <c r="AA50" s="58"/>
-      <c r="AB50" s="58"/>
-      <c r="AC50" s="58"/>
-      <c r="AD50" s="58"/>
-    </row>
-    <row r="51" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G51" s="58"/>
       <c r="H51" s="58"/>
       <c r="I51" s="58"/>
@@ -10939,18 +10417,8 @@
       <c r="R51" s="58"/>
       <c r="S51" s="58"/>
       <c r="T51" s="58"/>
-      <c r="U51" s="58"/>
-      <c r="V51" s="58"/>
-      <c r="W51" s="58"/>
-      <c r="X51" s="58"/>
-      <c r="Y51" s="58"/>
-      <c r="Z51" s="58"/>
-      <c r="AA51" s="58"/>
-      <c r="AB51" s="58"/>
-      <c r="AC51" s="58"/>
-      <c r="AD51" s="58"/>
-    </row>
-    <row r="52" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G52" s="58"/>
       <c r="H52" s="58"/>
       <c r="I52" s="58"/>
@@ -10965,18 +10433,8 @@
       <c r="R52" s="58"/>
       <c r="S52" s="58"/>
       <c r="T52" s="58"/>
-      <c r="U52" s="58"/>
-      <c r="V52" s="58"/>
-      <c r="W52" s="58"/>
-      <c r="X52" s="58"/>
-      <c r="Y52" s="58"/>
-      <c r="Z52" s="58"/>
-      <c r="AA52" s="58"/>
-      <c r="AB52" s="58"/>
-      <c r="AC52" s="58"/>
-      <c r="AD52" s="58"/>
-    </row>
-    <row r="53" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G53" s="58"/>
       <c r="H53" s="58"/>
       <c r="I53" s="58"/>
@@ -10991,18 +10449,8 @@
       <c r="R53" s="58"/>
       <c r="S53" s="58"/>
       <c r="T53" s="58"/>
-      <c r="U53" s="58"/>
-      <c r="V53" s="58"/>
-      <c r="W53" s="58"/>
-      <c r="X53" s="58"/>
-      <c r="Y53" s="58"/>
-      <c r="Z53" s="58"/>
-      <c r="AA53" s="58"/>
-      <c r="AB53" s="58"/>
-      <c r="AC53" s="58"/>
-      <c r="AD53" s="58"/>
-    </row>
-    <row r="54" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G54" s="58"/>
       <c r="H54" s="58"/>
       <c r="I54" s="58"/>
@@ -11017,18 +10465,8 @@
       <c r="R54" s="58"/>
       <c r="S54" s="58"/>
       <c r="T54" s="58"/>
-      <c r="U54" s="58"/>
-      <c r="V54" s="58"/>
-      <c r="W54" s="58"/>
-      <c r="X54" s="58"/>
-      <c r="Y54" s="58"/>
-      <c r="Z54" s="58"/>
-      <c r="AA54" s="58"/>
-      <c r="AB54" s="58"/>
-      <c r="AC54" s="58"/>
-      <c r="AD54" s="58"/>
-    </row>
-    <row r="55" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G55" s="58"/>
       <c r="H55" s="58"/>
       <c r="I55" s="58"/>
@@ -11043,18 +10481,8 @@
       <c r="R55" s="58"/>
       <c r="S55" s="58"/>
       <c r="T55" s="58"/>
-      <c r="U55" s="58"/>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
-      <c r="Z55" s="58"/>
-      <c r="AA55" s="58"/>
-      <c r="AB55" s="58"/>
-      <c r="AC55" s="58"/>
-      <c r="AD55" s="58"/>
-    </row>
-    <row r="56" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G56" s="58"/>
       <c r="H56" s="58"/>
       <c r="I56" s="58"/>
@@ -11069,18 +10497,8 @@
       <c r="R56" s="58"/>
       <c r="S56" s="58"/>
       <c r="T56" s="58"/>
-      <c r="U56" s="58"/>
-      <c r="V56" s="58"/>
-      <c r="W56" s="58"/>
-      <c r="X56" s="58"/>
-      <c r="Y56" s="58"/>
-      <c r="Z56" s="58"/>
-      <c r="AA56" s="58"/>
-      <c r="AB56" s="58"/>
-      <c r="AC56" s="58"/>
-      <c r="AD56" s="58"/>
-    </row>
-    <row r="57" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G57" s="58"/>
       <c r="H57" s="58"/>
       <c r="I57" s="58"/>
@@ -11095,18 +10513,8 @@
       <c r="R57" s="58"/>
       <c r="S57" s="58"/>
       <c r="T57" s="58"/>
-      <c r="U57" s="58"/>
-      <c r="V57" s="58"/>
-      <c r="W57" s="58"/>
-      <c r="X57" s="58"/>
-      <c r="Y57" s="58"/>
-      <c r="Z57" s="58"/>
-      <c r="AA57" s="58"/>
-      <c r="AB57" s="58"/>
-      <c r="AC57" s="58"/>
-      <c r="AD57" s="58"/>
-    </row>
-    <row r="58" spans="7:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G58" s="42"/>
       <c r="H58" s="42"/>
       <c r="I58" s="42"/>
@@ -11120,85 +10528,75 @@
       <c r="Q58" s="42"/>
       <c r="R58" s="42"/>
       <c r="S58" s="42"/>
-      <c r="T58" s="42"/>
-      <c r="U58" s="42"/>
-      <c r="V58" s="42"/>
-      <c r="W58" s="42"/>
-      <c r="X58" s="42"/>
-      <c r="Y58" s="42"/>
-      <c r="Z58" s="42"/>
-      <c r="AA58" s="42"/>
-      <c r="AB58" s="42"/>
-      <c r="AC58" s="42"/>
-      <c r="AD58" s="58"/>
-    </row>
-    <row r="59" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD59" s="58"/>
-    </row>
-    <row r="60" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD60" s="58"/>
-    </row>
-    <row r="61" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD61" s="58"/>
-    </row>
-    <row r="62" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD62" s="58"/>
-    </row>
-    <row r="63" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD63" s="58"/>
-    </row>
-    <row r="64" spans="7:30" x14ac:dyDescent="0.25">
-      <c r="AD64" s="58"/>
-    </row>
-    <row r="65" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD65" s="58"/>
-    </row>
-    <row r="66" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD66" s="58"/>
-    </row>
-    <row r="67" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD67" s="58"/>
-    </row>
-    <row r="68" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD68" s="58"/>
-    </row>
-    <row r="69" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD69" s="58"/>
-    </row>
-    <row r="70" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD70" s="58"/>
-    </row>
-    <row r="71" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD71" s="58"/>
-    </row>
-    <row r="72" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD72" s="58"/>
-    </row>
-    <row r="73" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD73" s="58"/>
-    </row>
-    <row r="74" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD74" s="58"/>
-    </row>
-    <row r="75" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD75" s="58"/>
-    </row>
-    <row r="76" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD76" s="58"/>
-    </row>
-    <row r="77" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD77" s="58"/>
-    </row>
-    <row r="78" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD78" s="58"/>
-    </row>
-    <row r="79" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD79" s="58"/>
-    </row>
-    <row r="80" spans="30:30" x14ac:dyDescent="0.25">
-      <c r="AD80" s="42"/>
-    </row>
-    <row r="81" spans="7:30" x14ac:dyDescent="0.25">
+      <c r="T58" s="58"/>
+    </row>
+    <row r="59" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T59" s="58"/>
+    </row>
+    <row r="60" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T60" s="58"/>
+    </row>
+    <row r="61" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T61" s="58"/>
+    </row>
+    <row r="62" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T62" s="58"/>
+    </row>
+    <row r="63" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T63" s="58"/>
+    </row>
+    <row r="64" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="T64" s="58"/>
+    </row>
+    <row r="65" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T65" s="58"/>
+    </row>
+    <row r="66" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T66" s="58"/>
+    </row>
+    <row r="67" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T67" s="58"/>
+    </row>
+    <row r="68" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T68" s="58"/>
+    </row>
+    <row r="69" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T69" s="58"/>
+    </row>
+    <row r="70" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T70" s="58"/>
+    </row>
+    <row r="71" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T71" s="58"/>
+    </row>
+    <row r="72" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T72" s="58"/>
+    </row>
+    <row r="73" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T73" s="58"/>
+    </row>
+    <row r="74" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T74" s="58"/>
+    </row>
+    <row r="75" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T75" s="58"/>
+    </row>
+    <row r="76" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T76" s="58"/>
+    </row>
+    <row r="77" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T77" s="58"/>
+    </row>
+    <row r="78" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T78" s="58"/>
+    </row>
+    <row r="79" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T79" s="58"/>
+    </row>
+    <row r="80" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T80" s="42"/>
+    </row>
+    <row r="81" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G81" s="42"/>
       <c r="H81" s="42"/>
       <c r="I81" s="42"/>
@@ -11213,16 +10611,6 @@
       <c r="R81" s="42"/>
       <c r="S81" s="42"/>
       <c r="T81" s="42"/>
-      <c r="U81" s="42"/>
-      <c r="V81" s="42"/>
-      <c r="W81" s="42"/>
-      <c r="X81" s="42"/>
-      <c r="Y81" s="42"/>
-      <c r="Z81" s="42"/>
-      <c r="AA81" s="42"/>
-      <c r="AB81" s="42"/>
-      <c r="AC81" s="42"/>
-      <c r="AD81" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11233,7 +10621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37977C-A20A-4B26-8AC1-43F48BE9948E}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>

</xml_diff>

<commit_message>
Add html structure for Building 5
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="700" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6292DC1B-9EAD-4CD1-BA06-7EB1201697EC}"/>
+  <xr:revisionPtr revIDLastSave="1002" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C022AE3-F4F4-4EDC-AD4E-7862F8DC51CE}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="5" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="B3-H2" sheetId="7" r:id="rId5"/>
     <sheet name="B4-H1" sheetId="9" r:id="rId6"/>
     <sheet name="B4-H2" sheetId="10" r:id="rId7"/>
+    <sheet name="B5-H1" sheetId="11" r:id="rId8"/>
+    <sheet name="B5-H2" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="51">
   <si>
     <t>Columns</t>
   </si>
@@ -178,6 +180,24 @@
   <si>
     <t>H: 7</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>W: 7</t>
+  </si>
+  <si>
+    <t>H: 80</t>
+  </si>
+  <si>
+    <t>W: 1</t>
+  </si>
+  <si>
+    <t>H: 67</t>
+  </si>
+  <si>
+    <t>W: 5</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -405,6 +431,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4280,8 +4310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5669387-3D46-4462-BFC6-BE1B7800A31B}">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA46" sqref="AA46"/>
     </sheetView>
   </sheetViews>
@@ -9352,7 +9382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA38ED-18F1-4CB9-A8B5-69652EFF8644}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
@@ -10621,7 +10651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37977C-A20A-4B26-8AC1-43F48BE9948E}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
@@ -11692,4 +11722,2777 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B77A7-FEEC-4A76-A1F9-1AC2C489FB77}">
+  <dimension ref="A1:P96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H1" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="60"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="30"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="27"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>415</v>
+      </c>
+      <c r="C7">
+        <f>B7/5</f>
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <f>B8/5</f>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="59"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="59"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="62">
+        <v>13</v>
+      </c>
+      <c r="I9" s="59"/>
+      <c r="J9" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="59"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="59"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="59"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="62"/>
+      <c r="O11" s="59"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>83</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="59"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="59"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>415</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="59"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="62">
+        <v>12</v>
+      </c>
+      <c r="I15" s="59"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="59"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="59"/>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="59"/>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="59"/>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="59"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="59"/>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="59"/>
+      <c r="H21" s="62">
+        <v>11</v>
+      </c>
+      <c r="I21" s="59"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="59"/>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="59"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="59"/>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="59"/>
+    </row>
+    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="59"/>
+    </row>
+    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="59"/>
+    </row>
+    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="59"/>
+      <c r="H27" s="62">
+        <v>10</v>
+      </c>
+      <c r="I27" s="59"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="59"/>
+    </row>
+    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="59"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="59"/>
+    </row>
+    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="59"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="59"/>
+    </row>
+    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="59"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="59"/>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="59"/>
+    </row>
+    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="59"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="59"/>
+    </row>
+    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="59"/>
+      <c r="H33" s="62">
+        <v>9</v>
+      </c>
+      <c r="I33" s="59"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="59"/>
+    </row>
+    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="59"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="59"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="59"/>
+    </row>
+    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="59"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="59"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="59"/>
+    </row>
+    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="59"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="59"/>
+    </row>
+    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+    </row>
+    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="59"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="59"/>
+    </row>
+    <row r="39" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="59"/>
+      <c r="H39" s="62">
+        <v>8</v>
+      </c>
+      <c r="I39" s="59"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="59"/>
+    </row>
+    <row r="40" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="59"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="59"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="59"/>
+    </row>
+    <row r="41" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="59"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="59"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="59"/>
+    </row>
+    <row r="42" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="59"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="59"/>
+    </row>
+    <row r="43" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="59"/>
+    </row>
+    <row r="44" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="59"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="59"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="59"/>
+    </row>
+    <row r="45" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="59"/>
+      <c r="H45" s="62">
+        <v>7</v>
+      </c>
+      <c r="I45" s="59"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="59"/>
+    </row>
+    <row r="46" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="59"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="59"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="59"/>
+    </row>
+    <row r="47" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="59"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="62"/>
+      <c r="M47" s="59"/>
+      <c r="N47" s="62"/>
+      <c r="O47" s="59"/>
+    </row>
+    <row r="48" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="59"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="62"/>
+      <c r="O48" s="59"/>
+    </row>
+    <row r="49" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="59"/>
+      <c r="J49" s="59"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
+      <c r="O49" s="59"/>
+    </row>
+    <row r="50" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="59"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="62"/>
+      <c r="M50" s="59"/>
+      <c r="N50" s="62"/>
+      <c r="O50" s="59"/>
+    </row>
+    <row r="51" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="59"/>
+      <c r="H51" s="62">
+        <v>6</v>
+      </c>
+      <c r="I51" s="59"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="59"/>
+      <c r="L51" s="62"/>
+      <c r="M51" s="59"/>
+      <c r="N51" s="62"/>
+      <c r="O51" s="59"/>
+    </row>
+    <row r="52" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" s="59"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="59"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="62"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="62"/>
+      <c r="O52" s="59"/>
+    </row>
+    <row r="53" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>51</v>
+      </c>
+      <c r="G53" s="59"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="62"/>
+      <c r="K53" s="59"/>
+      <c r="L53" s="62"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="62"/>
+      <c r="O53" s="59"/>
+    </row>
+    <row r="54" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>52</v>
+      </c>
+      <c r="G54" s="59"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="62"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="62"/>
+      <c r="O54" s="59"/>
+    </row>
+    <row r="55" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>53</v>
+      </c>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+    </row>
+    <row r="56" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>54</v>
+      </c>
+      <c r="G56" s="59"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="59"/>
+      <c r="L56" s="62"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="62"/>
+      <c r="O56" s="59"/>
+    </row>
+    <row r="57" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" s="59"/>
+      <c r="H57" s="62">
+        <v>5</v>
+      </c>
+      <c r="I57" s="59"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="59"/>
+      <c r="L57" s="62"/>
+      <c r="M57" s="59"/>
+      <c r="N57" s="62"/>
+      <c r="O57" s="59"/>
+    </row>
+    <row r="58" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" s="29"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="62"/>
+      <c r="K58" s="59"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="29"/>
+    </row>
+    <row r="59" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>57</v>
+      </c>
+      <c r="G59" s="29"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="62"/>
+      <c r="K59" s="59"/>
+      <c r="L59" s="62"/>
+      <c r="M59" s="59"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="29"/>
+    </row>
+    <row r="60" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="29"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="62"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="62"/>
+      <c r="O60" s="29"/>
+    </row>
+    <row r="61" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="29"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="59"/>
+      <c r="L61" s="59"/>
+      <c r="M61" s="59"/>
+      <c r="N61" s="59"/>
+      <c r="O61" s="29"/>
+    </row>
+    <row r="62" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="29"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="62"/>
+      <c r="K62" s="59"/>
+      <c r="L62" s="62"/>
+      <c r="M62" s="59"/>
+      <c r="N62" s="62"/>
+      <c r="O62" s="29"/>
+    </row>
+    <row r="63" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="29"/>
+      <c r="H63" s="62">
+        <v>4</v>
+      </c>
+      <c r="I63" s="59"/>
+      <c r="J63" s="62"/>
+      <c r="K63" s="59"/>
+      <c r="L63" s="62"/>
+      <c r="M63" s="59"/>
+      <c r="N63" s="62"/>
+      <c r="O63" s="29"/>
+    </row>
+    <row r="64" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="G64" s="29"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="59"/>
+      <c r="J64" s="62"/>
+      <c r="K64" s="59"/>
+      <c r="L64" s="62"/>
+      <c r="M64" s="59"/>
+      <c r="N64" s="62"/>
+      <c r="O64" s="29"/>
+    </row>
+    <row r="65" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="G65" s="29"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="59"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="59"/>
+      <c r="N65" s="62"/>
+      <c r="O65" s="29"/>
+    </row>
+    <row r="66" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66" s="29"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="29"/>
+      <c r="L66" s="62"/>
+      <c r="M66" s="29"/>
+      <c r="N66" s="62"/>
+      <c r="O66" s="29"/>
+    </row>
+    <row r="67" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="29"/>
+      <c r="K67" s="29"/>
+      <c r="L67" s="29"/>
+      <c r="M67" s="29"/>
+      <c r="N67" s="29"/>
+      <c r="O67" s="29"/>
+    </row>
+    <row r="68" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="G68" s="29"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="59"/>
+      <c r="L68" s="62"/>
+      <c r="M68" s="59"/>
+      <c r="N68" s="62"/>
+      <c r="O68" s="29"/>
+    </row>
+    <row r="69" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="G69" s="29"/>
+      <c r="H69" s="62">
+        <v>3</v>
+      </c>
+      <c r="I69" s="59"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="59"/>
+      <c r="L69" s="62"/>
+      <c r="M69" s="59"/>
+      <c r="N69" s="62"/>
+      <c r="O69" s="29"/>
+    </row>
+    <row r="70" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="G70" s="29"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="62"/>
+      <c r="K70" s="59"/>
+      <c r="L70" s="62"/>
+      <c r="M70" s="59"/>
+      <c r="N70" s="62"/>
+      <c r="O70" s="29"/>
+    </row>
+    <row r="71" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
+      </c>
+      <c r="G71" s="29"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="59"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="59"/>
+      <c r="L71" s="62"/>
+      <c r="M71" s="59"/>
+      <c r="N71" s="62"/>
+      <c r="O71" s="29"/>
+    </row>
+    <row r="72" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="G72" s="29"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="62"/>
+      <c r="M72" s="29"/>
+      <c r="N72" s="62"/>
+      <c r="O72" s="29"/>
+    </row>
+    <row r="73" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>71</v>
+      </c>
+      <c r="G73" s="29"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
+      <c r="J73" s="59"/>
+      <c r="K73" s="59"/>
+      <c r="L73" s="59"/>
+      <c r="M73" s="59"/>
+      <c r="N73" s="59"/>
+      <c r="O73" s="29"/>
+    </row>
+    <row r="74" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>72</v>
+      </c>
+      <c r="G74" s="29"/>
+      <c r="H74" s="62"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="62"/>
+      <c r="K74" s="59"/>
+      <c r="L74" s="62"/>
+      <c r="M74" s="59"/>
+      <c r="N74" s="62"/>
+      <c r="O74" s="29"/>
+    </row>
+    <row r="75" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>73</v>
+      </c>
+      <c r="G75" s="29"/>
+      <c r="H75" s="62">
+        <v>2</v>
+      </c>
+      <c r="I75" s="59"/>
+      <c r="J75" s="62"/>
+      <c r="K75" s="59"/>
+      <c r="L75" s="62"/>
+      <c r="M75" s="59"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="29"/>
+    </row>
+    <row r="76" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>74</v>
+      </c>
+      <c r="G76" s="29"/>
+      <c r="H76" s="62"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="62"/>
+      <c r="K76" s="59"/>
+      <c r="L76" s="62"/>
+      <c r="M76" s="59"/>
+      <c r="N76" s="62"/>
+      <c r="O76" s="29"/>
+    </row>
+    <row r="77" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>75</v>
+      </c>
+      <c r="G77" s="29"/>
+      <c r="H77" s="62"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="62"/>
+      <c r="K77" s="59"/>
+      <c r="L77" s="62"/>
+      <c r="M77" s="59"/>
+      <c r="N77" s="62"/>
+      <c r="O77" s="29"/>
+    </row>
+    <row r="78" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>76</v>
+      </c>
+      <c r="G78" s="29"/>
+      <c r="H78" s="62"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="62"/>
+      <c r="K78" s="29"/>
+      <c r="L78" s="62"/>
+      <c r="M78" s="29"/>
+      <c r="N78" s="62"/>
+      <c r="O78" s="29"/>
+    </row>
+    <row r="79" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>77</v>
+      </c>
+      <c r="G79" s="29"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="59"/>
+      <c r="J79" s="59"/>
+      <c r="K79" s="59"/>
+      <c r="L79" s="59"/>
+      <c r="M79" s="59"/>
+      <c r="N79" s="59"/>
+      <c r="O79" s="29"/>
+    </row>
+    <row r="80" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>78</v>
+      </c>
+      <c r="G80" s="29"/>
+      <c r="H80" s="62"/>
+      <c r="I80" s="59"/>
+      <c r="J80" s="62"/>
+      <c r="K80" s="59"/>
+      <c r="L80" s="62"/>
+      <c r="M80" s="59"/>
+      <c r="N80" s="62"/>
+      <c r="O80" s="29"/>
+    </row>
+    <row r="81" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>79</v>
+      </c>
+      <c r="G81" s="29"/>
+      <c r="H81" s="62">
+        <v>1</v>
+      </c>
+      <c r="I81" s="59"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="59"/>
+      <c r="L81" s="62"/>
+      <c r="M81" s="59"/>
+      <c r="N81" s="62"/>
+      <c r="O81" s="29"/>
+    </row>
+    <row r="82" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>80</v>
+      </c>
+      <c r="G82" s="29"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="59"/>
+      <c r="J82" s="62"/>
+      <c r="K82" s="59"/>
+      <c r="L82" s="62"/>
+      <c r="M82" s="59"/>
+      <c r="N82" s="62"/>
+      <c r="O82" s="29"/>
+    </row>
+    <row r="83" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>81</v>
+      </c>
+      <c r="G83" s="29"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="59"/>
+      <c r="J83" s="62"/>
+      <c r="K83" s="59"/>
+      <c r="L83" s="62"/>
+      <c r="M83" s="59"/>
+      <c r="N83" s="62"/>
+      <c r="O83" s="29"/>
+    </row>
+    <row r="84" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>82</v>
+      </c>
+      <c r="G84" s="29"/>
+      <c r="H84" s="62"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="62"/>
+      <c r="K84" s="29"/>
+      <c r="L84" s="62"/>
+      <c r="M84" s="29"/>
+      <c r="N84" s="62"/>
+      <c r="O84" s="29"/>
+    </row>
+    <row r="85" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>83</v>
+      </c>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="59"/>
+      <c r="J85" s="59"/>
+      <c r="K85" s="59"/>
+      <c r="L85" s="59"/>
+      <c r="M85" s="59"/>
+      <c r="N85" s="29"/>
+      <c r="O85" s="29"/>
+    </row>
+    <row r="86" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>84</v>
+      </c>
+      <c r="L86" s="58"/>
+      <c r="M86" s="58"/>
+      <c r="N86" s="58"/>
+      <c r="O86" s="58"/>
+    </row>
+    <row r="87" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L87" s="42"/>
+      <c r="M87" s="58"/>
+      <c r="N87" s="42"/>
+      <c r="O87" s="58"/>
+    </row>
+    <row r="88" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L88" s="58"/>
+      <c r="M88" s="58"/>
+      <c r="N88" s="58"/>
+      <c r="O88" s="58"/>
+    </row>
+    <row r="89" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L89" s="58"/>
+      <c r="M89" s="58"/>
+      <c r="N89" s="58"/>
+      <c r="O89" s="58"/>
+    </row>
+    <row r="90" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L90" s="58"/>
+      <c r="M90" s="58"/>
+      <c r="N90" s="58"/>
+      <c r="O90" s="58"/>
+    </row>
+    <row r="91" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L91" s="58"/>
+      <c r="M91" s="58"/>
+      <c r="N91" s="58"/>
+      <c r="O91" s="58"/>
+    </row>
+    <row r="92" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L92" s="58"/>
+      <c r="M92" s="58"/>
+      <c r="N92" s="58"/>
+      <c r="O92" s="58"/>
+    </row>
+    <row r="93" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L93" s="58"/>
+      <c r="M93" s="58"/>
+      <c r="N93" s="58"/>
+      <c r="O93" s="58"/>
+    </row>
+    <row r="94" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L94" s="58"/>
+      <c r="M94" s="58"/>
+      <c r="N94" s="58"/>
+      <c r="O94" s="58"/>
+    </row>
+    <row r="95" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L95" s="58"/>
+      <c r="M95" s="58"/>
+      <c r="N95" s="58"/>
+      <c r="O95" s="58"/>
+    </row>
+    <row r="96" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="L96" s="58"/>
+      <c r="M96" s="58"/>
+      <c r="N96" s="58"/>
+      <c r="O96" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEB1C13-B4E2-406F-8383-8D9B6AFEA523}">
+  <dimension ref="A1:P96"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G1" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="42">
+        <v>3</v>
+      </c>
+      <c r="J2" s="42">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>415</v>
+      </c>
+      <c r="C7">
+        <f>B7/5</f>
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <f>B8/5</f>
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="63">
+        <v>13</v>
+      </c>
+      <c r="I10" s="61"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>83</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>415</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="63"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="63">
+        <v>12</v>
+      </c>
+      <c r="I16" s="61"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+    </row>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+    </row>
+    <row r="18" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="37"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+    </row>
+    <row r="19" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="61"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="42"/>
+    </row>
+    <row r="20" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="63"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="33"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="33"/>
+    </row>
+    <row r="21" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="61"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="33"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="33"/>
+    </row>
+    <row r="22" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="33"/>
+    </row>
+    <row r="23" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="61"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="33"/>
+    </row>
+    <row r="24" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="61"/>
+      <c r="H24" s="63">
+        <v>11</v>
+      </c>
+      <c r="I24" s="33"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="61"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="61"/>
+      <c r="H27" s="63">
+        <v>10</v>
+      </c>
+      <c r="I27" s="33"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="61"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="33"/>
+    </row>
+    <row r="29" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="61"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="33"/>
+    </row>
+    <row r="30" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="61"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="33"/>
+    </row>
+    <row r="31" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+    </row>
+    <row r="32" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="61"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="33"/>
+    </row>
+    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="61"/>
+      <c r="H33" s="63">
+        <v>9</v>
+      </c>
+      <c r="I33" s="33"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="33"/>
+    </row>
+    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="61"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="64"/>
+      <c r="O34" s="33"/>
+    </row>
+    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="61"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="33"/>
+    </row>
+    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="61"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="33"/>
+    </row>
+    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+    </row>
+    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="61"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="33"/>
+    </row>
+    <row r="39" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="61"/>
+      <c r="H39" s="63">
+        <v>8</v>
+      </c>
+      <c r="I39" s="33"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="33"/>
+    </row>
+    <row r="40" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="61"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="64"/>
+      <c r="O40" s="33"/>
+    </row>
+    <row r="41" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="61"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="64"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="33"/>
+      <c r="N41" s="64"/>
+      <c r="O41" s="33"/>
+    </row>
+    <row r="42" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="61"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="64"/>
+      <c r="O42" s="33"/>
+    </row>
+    <row r="43" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+    </row>
+    <row r="44" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="61"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="33"/>
+    </row>
+    <row r="45" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="61"/>
+      <c r="H45" s="63">
+        <v>7</v>
+      </c>
+      <c r="I45" s="33"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="33"/>
+      <c r="N45" s="64"/>
+      <c r="O45" s="33"/>
+    </row>
+    <row r="46" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="61"/>
+      <c r="H46" s="63"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="33"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="33"/>
+    </row>
+    <row r="47" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="61"/>
+      <c r="H47" s="63"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="64"/>
+      <c r="O47" s="33"/>
+    </row>
+    <row r="48" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="61"/>
+      <c r="H48" s="63"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="64"/>
+      <c r="O48" s="33"/>
+    </row>
+    <row r="49" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+    </row>
+    <row r="50" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="61"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="64"/>
+      <c r="O50" s="33"/>
+    </row>
+    <row r="51" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="61"/>
+      <c r="H51" s="63">
+        <v>6</v>
+      </c>
+      <c r="I51" s="33"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="33"/>
+      <c r="N51" s="64"/>
+      <c r="O51" s="33"/>
+    </row>
+    <row r="52" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" s="61"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="64"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="64"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="64"/>
+      <c r="O52" s="33"/>
+    </row>
+    <row r="53" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>51</v>
+      </c>
+      <c r="G53" s="61"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="64"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="64"/>
+      <c r="M53" s="33"/>
+      <c r="N53" s="64"/>
+      <c r="O53" s="33"/>
+    </row>
+    <row r="54" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>52</v>
+      </c>
+      <c r="G54" s="61"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="64"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="64"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="64"/>
+      <c r="O54" s="33"/>
+    </row>
+    <row r="55" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>53</v>
+      </c>
+      <c r="G55" s="61"/>
+      <c r="H55" s="61"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+      <c r="N55" s="33"/>
+      <c r="O55" s="33"/>
+    </row>
+    <row r="56" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>54</v>
+      </c>
+      <c r="G56" s="61"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="64"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="64"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="64"/>
+      <c r="O56" s="33"/>
+    </row>
+    <row r="57" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" s="61"/>
+      <c r="H57" s="63"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="64"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="33"/>
+      <c r="N57" s="64"/>
+      <c r="O57" s="33"/>
+    </row>
+    <row r="58" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" s="33"/>
+      <c r="H58" s="63">
+        <v>5</v>
+      </c>
+      <c r="I58" s="33"/>
+      <c r="J58" s="64"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="64"/>
+      <c r="M58" s="33"/>
+      <c r="N58" s="64"/>
+      <c r="O58" s="33"/>
+    </row>
+    <row r="59" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>57</v>
+      </c>
+      <c r="G59" s="33"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="64"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="64"/>
+      <c r="M59" s="33"/>
+      <c r="N59" s="64"/>
+      <c r="O59" s="33"/>
+    </row>
+    <row r="60" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="33"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="64"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="64"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="64"/>
+      <c r="O60" s="33"/>
+    </row>
+    <row r="61" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="33"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
+      <c r="O61" s="33"/>
+    </row>
+    <row r="62" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="33"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="64"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="64"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="64"/>
+      <c r="O62" s="33"/>
+    </row>
+    <row r="63" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="33"/>
+      <c r="H63" s="63">
+        <v>4</v>
+      </c>
+      <c r="I63" s="33"/>
+      <c r="J63" s="64"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="64"/>
+      <c r="M63" s="33"/>
+      <c r="N63" s="64"/>
+      <c r="O63" s="33"/>
+    </row>
+    <row r="64" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="G64" s="33"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="64"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="64"/>
+      <c r="M64" s="33"/>
+      <c r="N64" s="64"/>
+      <c r="O64" s="33"/>
+    </row>
+    <row r="65" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="G65" s="33"/>
+      <c r="H65" s="63"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="64"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="64"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="64"/>
+      <c r="O65" s="33"/>
+    </row>
+    <row r="66" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66" s="33"/>
+      <c r="H66" s="63"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="64"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="64"/>
+      <c r="M66" s="33"/>
+      <c r="N66" s="64"/>
+      <c r="O66" s="33"/>
+    </row>
+    <row r="67" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67" s="33"/>
+      <c r="H67" s="61"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="33"/>
+    </row>
+    <row r="68" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="G68" s="33"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="64"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="64"/>
+      <c r="M68" s="33"/>
+      <c r="N68" s="64"/>
+      <c r="O68" s="33"/>
+    </row>
+    <row r="69" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="G69" s="33"/>
+      <c r="H69" s="63"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="64"/>
+      <c r="K69" s="33"/>
+      <c r="L69" s="64"/>
+      <c r="M69" s="33"/>
+      <c r="N69" s="64"/>
+      <c r="O69" s="33"/>
+    </row>
+    <row r="70" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="G70" s="33"/>
+      <c r="H70" s="63">
+        <v>3</v>
+      </c>
+      <c r="I70" s="33"/>
+      <c r="J70" s="64"/>
+      <c r="K70" s="33"/>
+      <c r="L70" s="64"/>
+      <c r="M70" s="33"/>
+      <c r="N70" s="64"/>
+      <c r="O70" s="33"/>
+    </row>
+    <row r="71" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
+      </c>
+      <c r="G71" s="33"/>
+      <c r="H71" s="63"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="64"/>
+      <c r="K71" s="33"/>
+      <c r="L71" s="64"/>
+      <c r="M71" s="33"/>
+      <c r="N71" s="64"/>
+      <c r="O71" s="33"/>
+    </row>
+    <row r="72" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="G72" s="33"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="64"/>
+      <c r="K72" s="33"/>
+      <c r="L72" s="64"/>
+      <c r="M72" s="33"/>
+      <c r="N72" s="64"/>
+      <c r="O72" s="33"/>
+    </row>
+    <row r="73" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>71</v>
+      </c>
+      <c r="G73" s="33"/>
+      <c r="H73" s="61"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="33"/>
+      <c r="M73" s="33"/>
+      <c r="N73" s="33"/>
+      <c r="O73" s="33"/>
+    </row>
+    <row r="74" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>72</v>
+      </c>
+      <c r="G74" s="33"/>
+      <c r="H74" s="63"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="64"/>
+      <c r="K74" s="33"/>
+      <c r="L74" s="64"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="64"/>
+      <c r="O74" s="33"/>
+    </row>
+    <row r="75" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>73</v>
+      </c>
+      <c r="G75" s="33"/>
+      <c r="H75" s="63"/>
+      <c r="I75" s="33"/>
+      <c r="J75" s="64"/>
+      <c r="K75" s="33"/>
+      <c r="L75" s="64"/>
+      <c r="M75" s="33"/>
+      <c r="N75" s="64"/>
+      <c r="O75" s="33"/>
+    </row>
+    <row r="76" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>74</v>
+      </c>
+      <c r="G76" s="33"/>
+      <c r="H76" s="63"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="64"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="64"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="64"/>
+      <c r="O76" s="33"/>
+    </row>
+    <row r="77" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>75</v>
+      </c>
+      <c r="G77" s="33"/>
+      <c r="H77" s="63">
+        <v>2</v>
+      </c>
+      <c r="I77" s="33"/>
+      <c r="J77" s="64"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="64"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="64"/>
+      <c r="O77" s="33"/>
+    </row>
+    <row r="78" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>76</v>
+      </c>
+      <c r="G78" s="33"/>
+      <c r="H78" s="63"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="64"/>
+      <c r="K78" s="33"/>
+      <c r="L78" s="64"/>
+      <c r="M78" s="33"/>
+      <c r="N78" s="64"/>
+      <c r="O78" s="33"/>
+    </row>
+    <row r="79" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>77</v>
+      </c>
+      <c r="G79" s="33"/>
+      <c r="H79" s="61"/>
+      <c r="I79" s="33"/>
+      <c r="J79" s="33"/>
+      <c r="K79" s="33"/>
+      <c r="L79" s="33"/>
+      <c r="M79" s="33"/>
+      <c r="N79" s="33"/>
+      <c r="O79" s="33"/>
+    </row>
+    <row r="80" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>78</v>
+      </c>
+      <c r="G80" s="33"/>
+      <c r="H80" s="63"/>
+      <c r="I80" s="33"/>
+      <c r="J80" s="64"/>
+      <c r="K80" s="33"/>
+      <c r="L80" s="64"/>
+      <c r="M80" s="33"/>
+      <c r="N80" s="64"/>
+      <c r="O80" s="33"/>
+    </row>
+    <row r="81" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>79</v>
+      </c>
+      <c r="G81" s="33"/>
+      <c r="H81" s="63"/>
+      <c r="I81" s="33"/>
+      <c r="J81" s="64"/>
+      <c r="K81" s="33"/>
+      <c r="L81" s="64"/>
+      <c r="M81" s="33"/>
+      <c r="N81" s="64"/>
+      <c r="O81" s="33"/>
+    </row>
+    <row r="82" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>80</v>
+      </c>
+      <c r="G82" s="33"/>
+      <c r="H82" s="63"/>
+      <c r="I82" s="33"/>
+      <c r="J82" s="64"/>
+      <c r="K82" s="33"/>
+      <c r="L82" s="64"/>
+      <c r="M82" s="33"/>
+      <c r="N82" s="64"/>
+      <c r="O82" s="33"/>
+    </row>
+    <row r="83" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <v>81</v>
+      </c>
+      <c r="G83" s="33"/>
+      <c r="H83" s="63">
+        <v>1</v>
+      </c>
+      <c r="I83" s="33"/>
+      <c r="J83" s="64"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="64"/>
+      <c r="M83" s="33"/>
+      <c r="N83" s="64"/>
+      <c r="O83" s="33"/>
+    </row>
+    <row r="84" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <v>82</v>
+      </c>
+      <c r="G84" s="33"/>
+      <c r="H84" s="63"/>
+      <c r="I84" s="33"/>
+      <c r="J84" s="64"/>
+      <c r="K84" s="33"/>
+      <c r="L84" s="64"/>
+      <c r="M84" s="33"/>
+      <c r="N84" s="64"/>
+      <c r="O84" s="33"/>
+    </row>
+    <row r="85" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <v>83</v>
+      </c>
+      <c r="G85" s="33"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="33"/>
+      <c r="J85" s="33"/>
+      <c r="K85" s="33"/>
+      <c r="L85" s="33"/>
+      <c r="M85" s="33"/>
+      <c r="N85" s="33"/>
+      <c r="O85" s="33"/>
+    </row>
+    <row r="86" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <v>84</v>
+      </c>
+      <c r="G86" s="58"/>
+    </row>
+    <row r="87" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G87" s="42"/>
+    </row>
+    <row r="88" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G88" s="58"/>
+    </row>
+    <row r="89" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G89" s="58"/>
+    </row>
+    <row r="90" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G90" s="58"/>
+    </row>
+    <row r="91" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G91" s="58"/>
+    </row>
+    <row r="92" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G92" s="58"/>
+    </row>
+    <row r="93" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G93" s="58"/>
+    </row>
+    <row r="94" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G94" s="58"/>
+    </row>
+    <row r="95" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G95" s="58"/>
+    </row>
+    <row r="96" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="G96" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adjust the blueprint, html structure, and css styling of B1 Half 1 in order to make it consistent with the other buildings
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1002" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C022AE3-F4F4-4EDC-AD4E-7862F8DC51CE}"/>
+  <xr:revisionPtr revIDLastSave="1080" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40A18D8-D84D-457C-B3C0-6668473BD62F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="7" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
-    <sheet name="B1" sheetId="2" r:id="rId1"/>
+    <sheet name="B1-H1 &amp; H2" sheetId="2" r:id="rId1"/>
     <sheet name="B2-H1" sheetId="3" r:id="rId2"/>
     <sheet name="B2-H2" sheetId="5" r:id="rId3"/>
     <sheet name="B3-H1" sheetId="6" r:id="rId4"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="53">
   <si>
     <t>Columns</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>W: 5</t>
+  </si>
+  <si>
+    <t>VERSION 2</t>
+  </si>
+  <si>
+    <t>VERSION 1</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -435,6 +441,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,106 +786,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A560937-3DAF-440C-A6BF-42890318B648}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="19" width="2.85546875" customWidth="1"/>
+    <col min="21" max="29" width="2.85546875" customWidth="1"/>
+    <col min="30" max="32" width="3.28515625" customWidth="1"/>
+    <col min="33" max="33" width="3.42578125" customWidth="1"/>
+    <col min="34" max="34" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C1" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>9</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="M3">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="N3">
         <v>12</v>
       </c>
-      <c r="O2">
+      <c r="O3">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="U3">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <v>6</v>
+      </c>
+      <c r="AA3">
+        <v>7</v>
+      </c>
+      <c r="AB3">
+        <v>8</v>
+      </c>
+      <c r="AC3">
+        <v>9</v>
+      </c>
+      <c r="AD3">
+        <v>10</v>
+      </c>
+      <c r="AE3">
+        <v>11</v>
+      </c>
+      <c r="AF3">
+        <v>12</v>
+      </c>
+      <c r="AG3">
+        <v>13</v>
+      </c>
+      <c r="AH3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>2</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1"/>
@@ -883,141 +949,294 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="6"/>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="9"/>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="66"/>
+      <c r="AD7" s="67"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="2" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="O8" s="4"/>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="X8" s="62"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="62"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AJ8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK8" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL8" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="5" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="O9" s="6"/>
+      <c r="T9">
+        <v>6</v>
+      </c>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="29"/>
+      <c r="AG9" s="29"/>
+      <c r="AJ9" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK9">
+        <v>220</v>
+      </c>
+      <c r="AL9">
+        <f>AK9/5</f>
+        <v>44</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>7</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>8</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="13"/>
+      <c r="E10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="11"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="11"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" s="13"/>
+      <c r="L10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="11"/>
       <c r="N10" s="5"/>
       <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>7</v>
+      </c>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="19">
+        <v>6</v>
+      </c>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="62"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AJ10" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK10">
+        <v>130</v>
+      </c>
+      <c r="AL10">
+        <f>AK10/5</f>
+        <v>26</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="I11" s="17"/>
       <c r="J11" s="13"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="M11" s="13"/>
       <c r="N11" s="5"/>
       <c r="O11" s="6"/>
-      <c r="Q11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>8</v>
+      </c>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="69"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="69"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="29"/>
+      <c r="AG11" s="29"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -1032,134 +1251,301 @@
       <c r="M12" s="13"/>
       <c r="N12" s="5"/>
       <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q12" t="s">
+        <v>7</v>
+      </c>
+      <c r="T12">
+        <v>9</v>
+      </c>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="29"/>
+      <c r="AD12" s="29"/>
+      <c r="AE12" s="29"/>
+      <c r="AF12" s="29"/>
+      <c r="AG12" s="29"/>
+      <c r="AK12" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL12" s="40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="15"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="13"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
       <c r="N13" s="5"/>
       <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>10</v>
+      </c>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
+      <c r="AE13" s="29"/>
+      <c r="AF13" s="29"/>
+      <c r="AG13" s="29"/>
+      <c r="AJ13" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK13">
+        <v>13</v>
+      </c>
+      <c r="AL13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="4"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="5"/>
       <c r="O14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>11</v>
+      </c>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="68"/>
+      <c r="Z14" s="66"/>
+      <c r="AA14" s="67"/>
+      <c r="AB14" s="68"/>
+      <c r="AC14" s="66"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="68"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+      <c r="AJ14" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK14">
+        <v>44</v>
+      </c>
+      <c r="AL14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
+      <c r="E15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="6"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <v>12</v>
+      </c>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="62"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="62"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AJ15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK15">
+        <f>AK13*5</f>
+        <v>65</v>
+      </c>
+      <c r="AL15">
+        <f>AL13*5</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M16" s="11"/>
+      <c r="E16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
       <c r="N16" s="5"/>
       <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <v>13</v>
+      </c>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="62"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="62"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="62"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="29"/>
+      <c r="AJ16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK16">
+        <f>AK14*5</f>
+        <v>220</v>
+      </c>
+      <c r="AL16">
+        <f>AL14*5</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="13"/>
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="13"/>
+      <c r="H17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="11"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M17" s="13"/>
+      <c r="L17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="11"/>
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <v>14</v>
+      </c>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="19">
+        <v>5</v>
+      </c>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="62"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="62"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="12"/>
+      <c r="E18" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="F18" s="13"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="I18" s="17"/>
       <c r="J18" s="13"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="12"/>
+      <c r="L18" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="M18" s="13"/>
       <c r="N18" s="5"/>
       <c r="O18" s="6"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>15</v>
+      </c>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="69"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="21"/>
+      <c r="AD18" s="69"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="29"/>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1174,134 +1560,252 @@
       <c r="M19" s="13"/>
       <c r="N19" s="5"/>
       <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>16</v>
+      </c>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="29"/>
+      <c r="AB19" s="29"/>
+      <c r="AC19" s="29"/>
+      <c r="AD19" s="29"/>
+      <c r="AE19" s="29"/>
+      <c r="AF19" s="29"/>
+      <c r="AG19" s="29"/>
+    </row>
+    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="15"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="15"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13"/>
       <c r="N20" s="5"/>
       <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>17</v>
+      </c>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="29"/>
+      <c r="AB20" s="29"/>
+      <c r="AC20" s="29"/>
+      <c r="AD20" s="29"/>
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="29"/>
+    </row>
+    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="4"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="5"/>
       <c r="O21" s="6"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>18</v>
+      </c>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X21" s="67"/>
+      <c r="Y21" s="68"/>
+      <c r="Z21" s="66"/>
+      <c r="AA21" s="67"/>
+      <c r="AB21" s="68"/>
+      <c r="AC21" s="66"/>
+      <c r="AD21" s="67"/>
+      <c r="AE21" s="68"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+    </row>
+    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
+      <c r="E22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
       <c r="N22" s="5"/>
       <c r="O22" s="6"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>19</v>
+      </c>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="62"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="62"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="29"/>
+    </row>
+    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M23" s="11"/>
+      <c r="E23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="9"/>
       <c r="N23" s="5"/>
       <c r="O23" s="6"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>20</v>
+      </c>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="62"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="62"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="29"/>
+      <c r="AG23" s="29"/>
+    </row>
+    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="13"/>
+      <c r="E24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="13"/>
+      <c r="H24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="11"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M24" s="13"/>
+      <c r="L24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="11"/>
       <c r="N24" s="5"/>
       <c r="O24" s="6"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>21</v>
+      </c>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="19">
+        <v>4</v>
+      </c>
+      <c r="X24" s="62"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="62"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="62"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+    </row>
+    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="F25" s="13"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="12"/>
+      <c r="H25" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="I25" s="17"/>
       <c r="J25" s="13"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="12"/>
+      <c r="L25" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="M25" s="13"/>
       <c r="N25" s="5"/>
       <c r="O25" s="6"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>22</v>
+      </c>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="69"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="69"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="69"/>
+      <c r="AE25" s="22"/>
+      <c r="AF25" s="29"/>
+      <c r="AG25" s="29"/>
+    </row>
+    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1316,134 +1820,252 @@
       <c r="M26" s="13"/>
       <c r="N26" s="5"/>
       <c r="O26" s="6"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <v>23</v>
+      </c>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="29"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="29"/>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="15"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="15"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="13"/>
       <c r="N27" s="5"/>
       <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <v>24</v>
+      </c>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="29"/>
+      <c r="AB27" s="29"/>
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="4"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="15"/>
       <c r="N28" s="5"/>
       <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <v>25</v>
+      </c>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X28" s="67"/>
+      <c r="Y28" s="68"/>
+      <c r="Z28" s="66"/>
+      <c r="AA28" s="67"/>
+      <c r="AB28" s="68"/>
+      <c r="AC28" s="66"/>
+      <c r="AD28" s="67"/>
+      <c r="AE28" s="68"/>
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="29"/>
+    </row>
+    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="9"/>
+      <c r="E29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
       <c r="N29" s="5"/>
       <c r="O29" s="6"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <v>26</v>
+      </c>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X29" s="62"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="62"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="62"/>
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="29"/>
+      <c r="AG29" s="29"/>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="11"/>
+      <c r="E30" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="9"/>
       <c r="N30" s="5"/>
       <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <v>27</v>
+      </c>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="62"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="62"/>
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="62"/>
+      <c r="AE30" s="20"/>
+      <c r="AF30" s="29"/>
+      <c r="AG30" s="29"/>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="13"/>
+      <c r="E31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="11"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="13"/>
+      <c r="H31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="M31" s="13"/>
+      <c r="L31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" s="11"/>
       <c r="N31" s="5"/>
       <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>28</v>
+      </c>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="19">
+        <v>3</v>
+      </c>
+      <c r="X31" s="62"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="62"/>
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="62"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="29"/>
+      <c r="AG31" s="29"/>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="F32" s="13"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="I32" s="17"/>
       <c r="J32" s="13"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="12"/>
+      <c r="L32" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="M32" s="13"/>
       <c r="N32" s="5"/>
       <c r="O32" s="6"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>29</v>
+      </c>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="69"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="21"/>
+      <c r="AA32" s="69"/>
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="21"/>
+      <c r="AD32" s="69"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="29"/>
+      <c r="AG32" s="29"/>
+    </row>
+    <row r="33" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -1458,112 +2080,214 @@
       <c r="M33" s="13"/>
       <c r="N33" s="5"/>
       <c r="O33" s="6"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <v>30</v>
+      </c>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="29"/>
+      <c r="AA33" s="29"/>
+      <c r="AB33" s="29"/>
+      <c r="AC33" s="29"/>
+      <c r="AD33" s="29"/>
+      <c r="AE33" s="29"/>
+      <c r="AF33" s="29"/>
+      <c r="AG33" s="29"/>
+    </row>
+    <row r="34" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="15"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="15"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="13"/>
       <c r="N34" s="5"/>
       <c r="O34" s="6"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <v>31</v>
+      </c>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
+      <c r="AA34" s="29"/>
+      <c r="AB34" s="29"/>
+      <c r="AC34" s="29"/>
+      <c r="AD34" s="29"/>
+      <c r="AE34" s="29"/>
+      <c r="AF34" s="29"/>
+      <c r="AG34" s="29"/>
+    </row>
+    <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="4"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="15"/>
       <c r="N35" s="5"/>
       <c r="O35" s="6"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T35">
+        <v>32</v>
+      </c>
+      <c r="U35" s="29"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="X35" s="67"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="66"/>
+      <c r="AA35" s="67"/>
+      <c r="AB35" s="68"/>
+      <c r="AC35" s="66"/>
+      <c r="AD35" s="67"/>
+      <c r="AE35" s="68"/>
+      <c r="AF35" s="29"/>
+      <c r="AG35" s="29"/>
+    </row>
+    <row r="36" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="9"/>
+      <c r="E36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
       <c r="N36" s="5"/>
       <c r="O36" s="6"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T36">
+        <v>33</v>
+      </c>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="X36" s="62"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="19"/>
+      <c r="AA36" s="62"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="19"/>
+      <c r="AD36" s="62"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="29"/>
+      <c r="AG36" s="29"/>
+    </row>
+    <row r="37" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="6"/>
+      <c r="T37">
+        <v>34</v>
+      </c>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="62"/>
+      <c r="Y37" s="20"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="62"/>
+      <c r="AB37" s="20"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="62"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="29"/>
+      <c r="AG37" s="29"/>
+    </row>
+    <row r="38" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>35</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="2" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="4"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38">
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="4"/>
+      <c r="T38">
+        <v>35</v>
+      </c>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="19">
+        <v>2</v>
+      </c>
+      <c r="X38" s="62"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="62"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="62"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="29"/>
+      <c r="AG38" s="29"/>
+    </row>
+    <row r="39" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>36</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="6"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>37</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
@@ -1574,10 +2298,26 @@
       <c r="M39" s="1"/>
       <c r="N39" s="5"/>
       <c r="O39" s="6"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <v>36</v>
+      </c>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="69"/>
+      <c r="Y39" s="22"/>
+      <c r="Z39" s="21"/>
+      <c r="AA39" s="69"/>
+      <c r="AB39" s="22"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="69"/>
+      <c r="AE39" s="22"/>
+      <c r="AF39" s="29"/>
+      <c r="AG39" s="29"/>
+    </row>
+    <row r="40" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="6"/>
@@ -1592,10 +2332,26 @@
       <c r="M40" s="1"/>
       <c r="N40" s="5"/>
       <c r="O40" s="6"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <v>37</v>
+      </c>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
+      <c r="AC40" s="29"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="29"/>
+      <c r="AF40" s="29"/>
+      <c r="AG40" s="29"/>
+    </row>
+    <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -1610,24 +2366,173 @@
       <c r="M41" s="1"/>
       <c r="N41" s="5"/>
       <c r="O41" s="6"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T41">
+        <v>38</v>
+      </c>
+      <c r="U41" s="29"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="29"/>
+      <c r="AB41" s="29"/>
+      <c r="AC41" s="29"/>
+      <c r="AD41" s="29"/>
+      <c r="AE41" s="29"/>
+      <c r="AF41" s="29"/>
+      <c r="AG41" s="29"/>
+    </row>
+    <row r="42" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="6"/>
+      <c r="T42">
+        <v>39</v>
+      </c>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="X42" s="71"/>
+      <c r="Y42" s="72"/>
+      <c r="Z42" s="70"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="72"/>
+      <c r="AC42" s="70"/>
+      <c r="AD42" s="71"/>
+      <c r="AE42" s="72"/>
+      <c r="AF42" s="29"/>
+      <c r="AG42" s="29"/>
+    </row>
+    <row r="43" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>40</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="9"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="9"/>
+      <c r="T43">
+        <v>40</v>
+      </c>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="X43" s="63"/>
+      <c r="Y43" s="74"/>
+      <c r="Z43" s="73"/>
+      <c r="AA43" s="63"/>
+      <c r="AB43" s="74"/>
+      <c r="AC43" s="73"/>
+      <c r="AD43" s="63"/>
+      <c r="AE43" s="74"/>
+      <c r="AF43" s="29"/>
+      <c r="AG43" s="29"/>
+    </row>
+    <row r="44" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="T44">
+        <v>41</v>
+      </c>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="73"/>
+      <c r="X44" s="63"/>
+      <c r="Y44" s="74"/>
+      <c r="Z44" s="73"/>
+      <c r="AA44" s="63"/>
+      <c r="AB44" s="74"/>
+      <c r="AC44" s="73"/>
+      <c r="AD44" s="63"/>
+      <c r="AE44" s="74"/>
+      <c r="AF44" s="29"/>
+      <c r="AG44" s="29"/>
+    </row>
+    <row r="45" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="T45">
+        <v>42</v>
+      </c>
+      <c r="U45" s="29"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="73">
+        <v>1</v>
+      </c>
+      <c r="X45" s="63"/>
+      <c r="Y45" s="74"/>
+      <c r="Z45" s="73"/>
+      <c r="AA45" s="63"/>
+      <c r="AB45" s="74"/>
+      <c r="AC45" s="73"/>
+      <c r="AD45" s="63"/>
+      <c r="AE45" s="74"/>
+      <c r="AF45" s="29"/>
+      <c r="AG45" s="29"/>
+    </row>
+    <row r="46" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="T46">
+        <v>43</v>
+      </c>
+      <c r="U46" s="29"/>
+      <c r="V46" s="29"/>
+      <c r="W46" s="73"/>
+      <c r="X46" s="63"/>
+      <c r="Y46" s="74"/>
+      <c r="Z46" s="73"/>
+      <c r="AA46" s="63"/>
+      <c r="AB46" s="74"/>
+      <c r="AC46" s="73"/>
+      <c r="AD46" s="63"/>
+      <c r="AE46" s="74"/>
+      <c r="AF46" s="29"/>
+      <c r="AG46" s="29"/>
+    </row>
+    <row r="47" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="T47">
+        <v>44</v>
+      </c>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="75"/>
+      <c r="X47" s="65"/>
+      <c r="Y47" s="76"/>
+      <c r="Z47" s="75"/>
+      <c r="AA47" s="65"/>
+      <c r="AB47" s="76"/>
+      <c r="AC47" s="75"/>
+      <c r="AD47" s="65"/>
+      <c r="AE47" s="76"/>
+      <c r="AF47" s="29"/>
+      <c r="AG47" s="29"/>
+    </row>
+    <row r="48" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9384,7 +10289,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11728,9 +12633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B77A7-FEEC-4A76-A1F9-1AC2C489FB77}">
   <dimension ref="A1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add 2 floors to Building 2
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1080" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40A18D8-D84D-457C-B3C0-6668473BD62F}"/>
+  <xr:revisionPtr revIDLastSave="1147" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D25A0E4-72C0-4F5A-BD03-45665C3C129B}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1-H1 &amp; H2" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
   <si>
     <t>Columns</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Pixels</t>
   </si>
   <si>
-    <t>Ratio: 2/3</t>
-  </si>
-  <si>
     <t>W: 12</t>
   </si>
   <si>
@@ -103,19 +100,7 @@
     <t>W: 8</t>
   </si>
   <si>
-    <t>Half1</t>
-  </si>
-  <si>
-    <t>Half2</t>
-  </si>
-  <si>
-    <t>H: 56</t>
-  </si>
-  <si>
     <t>H: 4</t>
-  </si>
-  <si>
-    <t>Floors: 8</t>
   </si>
   <si>
     <t>#1</t>
@@ -788,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A560937-3DAF-440C-A6BF-42890318B648}">
   <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
@@ -804,10 +789,10 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="C1" s="40" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="U1" s="40" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -1079,7 +1064,7 @@
       <c r="AF8" s="29"/>
       <c r="AG8" s="29"/>
       <c r="AJ8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="AK8" s="40" t="s">
         <v>13</v>
@@ -1271,10 +1256,10 @@
       <c r="AF12" s="29"/>
       <c r="AG12" s="29"/>
       <c r="AK12" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AL12" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -1311,7 +1296,7 @@
       <c r="AF13" s="29"/>
       <c r="AG13" s="29"/>
       <c r="AJ13" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AK13">
         <v>13</v>
@@ -1356,7 +1341,7 @@
       <c r="AF14" s="29"/>
       <c r="AG14" s="29"/>
       <c r="AJ14" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AK14">
         <v>44</v>
@@ -2541,42 +2526,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A03D14-663C-42B7-B26E-A63445663F92}">
-  <dimension ref="A1:AD59"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D3"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="3" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="30" width="3.28515625" customWidth="1"/>
-    <col min="31" max="31" width="3.140625" customWidth="1"/>
+    <col min="7" max="22" width="3.28515625" customWidth="1"/>
+    <col min="23" max="23" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="40" t="s">
         <v>12</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="C2">
         <f>B2/5</f>
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -2632,37 +2620,16 @@
       <c r="W2">
         <v>17</v>
       </c>
-      <c r="X2">
-        <v>18</v>
-      </c>
-      <c r="Y2">
-        <v>19</v>
-      </c>
-      <c r="Z2">
-        <v>20</v>
-      </c>
-      <c r="AA2">
-        <v>21</v>
-      </c>
-      <c r="AB2">
-        <v>22</v>
-      </c>
-      <c r="AC2">
-        <v>23</v>
-      </c>
-      <c r="AD2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B3">
         <v>120</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3" si="0">B3/5</f>
+        <f>B3/5</f>
         <v>24</v>
       </c>
       <c r="D3" t="s">
@@ -2672,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
@@ -2685,43 +2652,35 @@
       <c r="S3" s="24"/>
       <c r="T3" s="24"/>
       <c r="U3" s="24"/>
-      <c r="V3" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="31"/>
-      <c r="X3" s="31"/>
-      <c r="Y3" s="31"/>
-      <c r="Z3" s="31"/>
-      <c r="AA3" s="32"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V3" s="60"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>2</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="34"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="30"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>28</v>
+      </c>
       <c r="F5">
         <v>3</v>
       </c>
@@ -2729,33 +2688,31 @@
         <v>2</v>
       </c>
       <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="33"/>
-      <c r="X5" s="33"/>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="34"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>1</v>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="30"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="25"/>
       <c r="K6" s="26"/>
@@ -2769,19 +2726,20 @@
       <c r="S6" s="26"/>
       <c r="T6" s="26"/>
       <c r="U6" s="26"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="38"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V6" s="27"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>68</v>
+      </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="24"/>
@@ -2797,90 +2755,75 @@
       <c r="S7" s="24"/>
       <c r="T7" s="24"/>
       <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="32"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V7" s="60"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>B6*5</f>
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <f>C6*5</f>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="33"/>
-      <c r="Z8" s="33"/>
-      <c r="AA8" s="33"/>
-      <c r="AB8" s="33"/>
-      <c r="AC8" s="33"/>
-      <c r="AD8" s="34"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="30"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>B7*5</f>
+        <v>340</v>
+      </c>
+      <c r="C9">
+        <f>C7*5</f>
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>7</v>
       </c>
       <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="29"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="33"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
-      <c r="AD9" s="34"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>20</v>
-      </c>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="30"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>8</v>
       </c>
@@ -2899,23 +2842,9 @@
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
       <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="37"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="38"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
+      <c r="V10" s="27"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>9</v>
       </c>
@@ -2937,24 +2866,8 @@
       <c r="T11" s="30"/>
       <c r="U11" s="28"/>
       <c r="V11" s="30"/>
-      <c r="W11" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="32"/>
-      <c r="AA11" s="35"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="32"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>10</v>
       </c>
@@ -2976,24 +2889,12 @@
       <c r="T12" s="30"/>
       <c r="U12" s="28"/>
       <c r="V12" s="30"/>
-      <c r="W12" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="34"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="34"/>
-      <c r="AC12" s="36"/>
-      <c r="AD12" s="34"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>11</v>
       </c>
-      <c r="G13" s="28" t="s">
-        <v>31</v>
-      </c>
+      <c r="G13" s="28"/>
       <c r="H13" s="30"/>
       <c r="I13" s="19"/>
       <c r="J13" s="20"/>
@@ -3009,23 +2910,14 @@
       <c r="T13" s="30"/>
       <c r="U13" s="28"/>
       <c r="V13" s="30"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="36"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="36"/>
-      <c r="AD13" s="34"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>12</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="28">
+        <v>10</v>
+      </c>
       <c r="H14" s="30"/>
       <c r="I14" s="19"/>
       <c r="J14" s="20"/>
@@ -3041,16 +2933,8 @@
       <c r="T14" s="30"/>
       <c r="U14" s="28"/>
       <c r="V14" s="30"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="34"/>
-      <c r="AC14" s="36"/>
-      <c r="AD14" s="34"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>13</v>
       </c>
@@ -3070,16 +2954,8 @@
       <c r="T15" s="30"/>
       <c r="U15" s="28"/>
       <c r="V15" s="30"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="34"/>
-      <c r="AA15" s="36"/>
-      <c r="AB15" s="34"/>
-      <c r="AC15" s="36"/>
-      <c r="AD15" s="34"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>14</v>
       </c>
@@ -3099,47 +2975,29 @@
       <c r="T16" s="27"/>
       <c r="U16" s="25"/>
       <c r="V16" s="27"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="38"/>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="38"/>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="38"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="38"/>
-    </row>
-    <row r="17" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>15</v>
       </c>
-      <c r="G17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="20"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="32"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="32"/>
-    </row>
-    <row r="18" spans="6:30" x14ac:dyDescent="0.25">
+      <c r="G17" s="23"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="60"/>
+    </row>
+    <row r="18" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>16</v>
       </c>
@@ -3155,24 +3013,18 @@
       <c r="P18" s="30"/>
       <c r="Q18" s="28"/>
       <c r="R18" s="30"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="20"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="30"/>
       <c r="U18" s="28"/>
       <c r="V18" s="30"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="36"/>
-      <c r="AB18" s="34"/>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="34"/>
-    </row>
-    <row r="19" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>17</v>
       </c>
-      <c r="G19" s="28"/>
+      <c r="G19" s="28">
+        <v>9</v>
+      </c>
       <c r="H19" s="30"/>
       <c r="I19" s="28"/>
       <c r="J19" s="30"/>
@@ -3184,20 +3036,12 @@
       <c r="P19" s="30"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="30"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="20"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="30"/>
       <c r="U19" s="28"/>
       <c r="V19" s="30"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="34"/>
-      <c r="AA19" s="36"/>
-      <c r="AB19" s="34"/>
-      <c r="AC19" s="36"/>
-      <c r="AD19" s="34"/>
-    </row>
-    <row r="20" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>18</v>
       </c>
@@ -3213,20 +3057,12 @@
       <c r="P20" s="30"/>
       <c r="Q20" s="28"/>
       <c r="R20" s="30"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="20"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="30"/>
       <c r="U20" s="28"/>
       <c r="V20" s="30"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="34"/>
-    </row>
-    <row r="21" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>19</v>
       </c>
@@ -3242,20 +3078,12 @@
       <c r="P21" s="30"/>
       <c r="Q21" s="28"/>
       <c r="R21" s="30"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="20"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="30"/>
       <c r="U21" s="28"/>
       <c r="V21" s="30"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="34"/>
-      <c r="AA21" s="36"/>
-      <c r="AB21" s="34"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="34"/>
-    </row>
-    <row r="22" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>20</v>
       </c>
@@ -3271,25 +3099,17 @@
       <c r="P22" s="27"/>
       <c r="Q22" s="25"/>
       <c r="R22" s="27"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="22"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="27"/>
       <c r="U22" s="25"/>
       <c r="V22" s="27"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="38"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="38"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="38"/>
-      <c r="AC22" s="37"/>
-      <c r="AD22" s="38"/>
-    </row>
-    <row r="23" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>21</v>
       </c>
-      <c r="G23" s="28" t="s">
-        <v>29</v>
+      <c r="G23" s="28">
+        <v>8</v>
       </c>
       <c r="H23" s="30"/>
       <c r="I23" s="28"/>
@@ -3300,22 +3120,14 @@
       <c r="N23" s="30"/>
       <c r="O23" s="28"/>
       <c r="P23" s="30"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="30"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="20"/>
       <c r="U23" s="28"/>
       <c r="V23" s="30"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="35"/>
-      <c r="AB23" s="32"/>
-      <c r="AC23" s="35"/>
-      <c r="AD23" s="32"/>
-    </row>
-    <row r="24" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>22</v>
       </c>
@@ -3329,22 +3141,14 @@
       <c r="N24" s="30"/>
       <c r="O24" s="28"/>
       <c r="P24" s="30"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="30"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="20"/>
       <c r="U24" s="28"/>
       <c r="V24" s="30"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="34"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="34"/>
-      <c r="AC24" s="36"/>
-      <c r="AD24" s="34"/>
-    </row>
-    <row r="25" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>23</v>
       </c>
@@ -3358,22 +3162,14 @@
       <c r="N25" s="30"/>
       <c r="O25" s="28"/>
       <c r="P25" s="30"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="30"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="20"/>
       <c r="U25" s="28"/>
       <c r="V25" s="30"/>
-      <c r="W25" s="36"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="34"/>
-      <c r="AA25" s="36"/>
-      <c r="AB25" s="34"/>
-      <c r="AC25" s="36"/>
-      <c r="AD25" s="34"/>
-    </row>
-    <row r="26" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>24</v>
       </c>
@@ -3387,22 +3183,14 @@
       <c r="N26" s="30"/>
       <c r="O26" s="28"/>
       <c r="P26" s="30"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="30"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="20"/>
       <c r="U26" s="28"/>
       <c r="V26" s="30"/>
-      <c r="W26" s="36"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="34"/>
-      <c r="AA26" s="36"/>
-      <c r="AB26" s="34"/>
-      <c r="AC26" s="36"/>
-      <c r="AD26" s="34"/>
-    </row>
-    <row r="27" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>25</v>
       </c>
@@ -3416,22 +3204,14 @@
       <c r="N27" s="30"/>
       <c r="O27" s="28"/>
       <c r="P27" s="30"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="30"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="20"/>
       <c r="U27" s="28"/>
       <c r="V27" s="30"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="34"/>
-      <c r="AA27" s="36"/>
-      <c r="AB27" s="34"/>
-      <c r="AC27" s="36"/>
-      <c r="AD27" s="34"/>
-    </row>
-    <row r="28" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>26</v>
       </c>
@@ -3445,27 +3225,19 @@
       <c r="N28" s="27"/>
       <c r="O28" s="25"/>
       <c r="P28" s="27"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="25"/>
-      <c r="T28" s="27"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="22"/>
       <c r="U28" s="25"/>
       <c r="V28" s="27"/>
-      <c r="W28" s="37"/>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="37"/>
-      <c r="Z28" s="38"/>
-      <c r="AA28" s="37"/>
-      <c r="AB28" s="38"/>
-      <c r="AC28" s="37"/>
-      <c r="AD28" s="38"/>
-    </row>
-    <row r="29" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F29">
         <v>27</v>
       </c>
-      <c r="G29" s="28" t="s">
-        <v>28</v>
+      <c r="G29" s="28">
+        <v>7</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="28"/>
@@ -3476,22 +3248,14 @@
       <c r="N29" s="30"/>
       <c r="O29" s="28"/>
       <c r="P29" s="30"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="30"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="20"/>
       <c r="S29" s="28"/>
       <c r="T29" s="30"/>
       <c r="U29" s="28"/>
       <c r="V29" s="30"/>
-      <c r="W29" s="35"/>
-      <c r="X29" s="32"/>
-      <c r="Y29" s="35"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="35"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="35"/>
-      <c r="AD29" s="32"/>
-    </row>
-    <row r="30" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F30">
         <v>28</v>
       </c>
@@ -3505,22 +3269,14 @@
       <c r="N30" s="30"/>
       <c r="O30" s="28"/>
       <c r="P30" s="30"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="30"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="20"/>
       <c r="S30" s="28"/>
       <c r="T30" s="30"/>
       <c r="U30" s="28"/>
       <c r="V30" s="30"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="34"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="34"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="34"/>
-      <c r="AC30" s="36"/>
-      <c r="AD30" s="34"/>
-    </row>
-    <row r="31" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F31">
         <v>29</v>
       </c>
@@ -3534,22 +3290,14 @@
       <c r="N31" s="30"/>
       <c r="O31" s="28"/>
       <c r="P31" s="30"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="30"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="20"/>
       <c r="S31" s="28"/>
       <c r="T31" s="30"/>
       <c r="U31" s="28"/>
       <c r="V31" s="30"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="34"/>
-      <c r="AA31" s="36"/>
-      <c r="AB31" s="34"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="34"/>
-    </row>
-    <row r="32" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F32">
         <v>30</v>
       </c>
@@ -3563,22 +3311,14 @@
       <c r="N32" s="30"/>
       <c r="O32" s="28"/>
       <c r="P32" s="30"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="30"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="20"/>
       <c r="S32" s="28"/>
       <c r="T32" s="30"/>
       <c r="U32" s="28"/>
       <c r="V32" s="30"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="34"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="34"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="34"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="34"/>
-    </row>
-    <row r="33" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>31</v>
       </c>
@@ -3592,22 +3332,14 @@
       <c r="N33" s="30"/>
       <c r="O33" s="28"/>
       <c r="P33" s="30"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="30"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="20"/>
       <c r="S33" s="28"/>
       <c r="T33" s="30"/>
       <c r="U33" s="28"/>
       <c r="V33" s="30"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="34"/>
-      <c r="AA33" s="36"/>
-      <c r="AB33" s="34"/>
-      <c r="AC33" s="36"/>
-      <c r="AD33" s="34"/>
-    </row>
-    <row r="34" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>32</v>
       </c>
@@ -3621,27 +3353,19 @@
       <c r="N34" s="27"/>
       <c r="O34" s="25"/>
       <c r="P34" s="27"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="27"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="22"/>
       <c r="S34" s="25"/>
       <c r="T34" s="27"/>
       <c r="U34" s="25"/>
       <c r="V34" s="27"/>
-      <c r="W34" s="37"/>
-      <c r="X34" s="38"/>
-      <c r="Y34" s="37"/>
-      <c r="Z34" s="38"/>
-      <c r="AA34" s="37"/>
-      <c r="AB34" s="38"/>
-      <c r="AC34" s="37"/>
-      <c r="AD34" s="38"/>
-    </row>
-    <row r="35" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>33</v>
       </c>
-      <c r="G35" s="28" t="s">
-        <v>27</v>
+      <c r="G35" s="28">
+        <v>6</v>
       </c>
       <c r="H35" s="30"/>
       <c r="I35" s="28"/>
@@ -3658,16 +3382,8 @@
       <c r="T35" s="30"/>
       <c r="U35" s="28"/>
       <c r="V35" s="30"/>
-      <c r="W35" s="35"/>
-      <c r="X35" s="32"/>
-      <c r="Y35" s="35"/>
-      <c r="Z35" s="32"/>
-      <c r="AA35" s="35"/>
-      <c r="AB35" s="32"/>
-      <c r="AC35" s="35"/>
-      <c r="AD35" s="32"/>
-    </row>
-    <row r="36" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>34</v>
       </c>
@@ -3687,16 +3403,8 @@
       <c r="T36" s="30"/>
       <c r="U36" s="28"/>
       <c r="V36" s="30"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="36"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="36"/>
-      <c r="AB36" s="34"/>
-      <c r="AC36" s="36"/>
-      <c r="AD36" s="34"/>
-    </row>
-    <row r="37" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>35</v>
       </c>
@@ -3716,16 +3424,8 @@
       <c r="T37" s="30"/>
       <c r="U37" s="28"/>
       <c r="V37" s="30"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="34"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="34"/>
-      <c r="AA37" s="36"/>
-      <c r="AB37" s="34"/>
-      <c r="AC37" s="36"/>
-      <c r="AD37" s="34"/>
-    </row>
-    <row r="38" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>36</v>
       </c>
@@ -3745,16 +3445,8 @@
       <c r="T38" s="30"/>
       <c r="U38" s="28"/>
       <c r="V38" s="30"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="36"/>
-      <c r="AB38" s="34"/>
-      <c r="AC38" s="36"/>
-      <c r="AD38" s="34"/>
-    </row>
-    <row r="39" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>37</v>
       </c>
@@ -3774,16 +3466,8 @@
       <c r="T39" s="30"/>
       <c r="U39" s="28"/>
       <c r="V39" s="30"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="36"/>
-      <c r="AB39" s="34"/>
-      <c r="AC39" s="36"/>
-      <c r="AD39" s="34"/>
-    </row>
-    <row r="40" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>38</v>
       </c>
@@ -3803,21 +3487,13 @@
       <c r="T40" s="27"/>
       <c r="U40" s="25"/>
       <c r="V40" s="27"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="38"/>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="38"/>
-      <c r="AA40" s="37"/>
-      <c r="AB40" s="38"/>
-      <c r="AC40" s="37"/>
-      <c r="AD40" s="38"/>
-    </row>
-    <row r="41" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>39</v>
       </c>
-      <c r="G41" s="28" t="s">
-        <v>26</v>
+      <c r="G41" s="28">
+        <v>5</v>
       </c>
       <c r="H41" s="30"/>
       <c r="I41" s="28"/>
@@ -3834,16 +3510,8 @@
       <c r="T41" s="30"/>
       <c r="U41" s="28"/>
       <c r="V41" s="30"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="32"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="32"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="32"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="32"/>
-    </row>
-    <row r="42" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>40</v>
       </c>
@@ -3863,16 +3531,8 @@
       <c r="T42" s="30"/>
       <c r="U42" s="28"/>
       <c r="V42" s="30"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="34"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="34"/>
-      <c r="AA42" s="36"/>
-      <c r="AB42" s="34"/>
-      <c r="AC42" s="36"/>
-      <c r="AD42" s="34"/>
-    </row>
-    <row r="43" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F43">
         <v>41</v>
       </c>
@@ -3892,16 +3552,8 @@
       <c r="T43" s="30"/>
       <c r="U43" s="28"/>
       <c r="V43" s="30"/>
-      <c r="W43" s="36"/>
-      <c r="X43" s="34"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="34"/>
-      <c r="AA43" s="36"/>
-      <c r="AB43" s="34"/>
-      <c r="AC43" s="36"/>
-      <c r="AD43" s="34"/>
-    </row>
-    <row r="44" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F44">
         <v>42</v>
       </c>
@@ -3921,16 +3573,8 @@
       <c r="T44" s="30"/>
       <c r="U44" s="28"/>
       <c r="V44" s="30"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="34"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="34"/>
-      <c r="AA44" s="36"/>
-      <c r="AB44" s="34"/>
-      <c r="AC44" s="36"/>
-      <c r="AD44" s="34"/>
-    </row>
-    <row r="45" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F45">
         <v>43</v>
       </c>
@@ -3950,16 +3594,8 @@
       <c r="T45" s="30"/>
       <c r="U45" s="28"/>
       <c r="V45" s="30"/>
-      <c r="W45" s="36"/>
-      <c r="X45" s="34"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="34"/>
-      <c r="AA45" s="36"/>
-      <c r="AB45" s="34"/>
-      <c r="AC45" s="36"/>
-      <c r="AD45" s="34"/>
-    </row>
-    <row r="46" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F46">
         <v>44</v>
       </c>
@@ -3979,21 +3615,13 @@
       <c r="T46" s="27"/>
       <c r="U46" s="25"/>
       <c r="V46" s="27"/>
-      <c r="W46" s="37"/>
-      <c r="X46" s="38"/>
-      <c r="Y46" s="37"/>
-      <c r="Z46" s="38"/>
-      <c r="AA46" s="37"/>
-      <c r="AB46" s="38"/>
-      <c r="AC46" s="37"/>
-      <c r="AD46" s="38"/>
-    </row>
-    <row r="47" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F47">
         <v>45</v>
       </c>
-      <c r="G47" s="28" t="s">
-        <v>25</v>
+      <c r="G47" s="28">
+        <v>4</v>
       </c>
       <c r="H47" s="30"/>
       <c r="I47" s="28"/>
@@ -4010,16 +3638,8 @@
       <c r="T47" s="30"/>
       <c r="U47" s="28"/>
       <c r="V47" s="30"/>
-      <c r="W47" s="35"/>
-      <c r="X47" s="32"/>
-      <c r="Y47" s="35"/>
-      <c r="Z47" s="32"/>
-      <c r="AA47" s="35"/>
-      <c r="AB47" s="32"/>
-      <c r="AC47" s="35"/>
-      <c r="AD47" s="32"/>
-    </row>
-    <row r="48" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F48">
         <v>46</v>
       </c>
@@ -4039,16 +3659,8 @@
       <c r="T48" s="30"/>
       <c r="U48" s="28"/>
       <c r="V48" s="30"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="34"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="34"/>
-      <c r="AA48" s="36"/>
-      <c r="AB48" s="34"/>
-      <c r="AC48" s="36"/>
-      <c r="AD48" s="34"/>
-    </row>
-    <row r="49" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F49">
         <v>47</v>
       </c>
@@ -4068,16 +3680,8 @@
       <c r="T49" s="30"/>
       <c r="U49" s="28"/>
       <c r="V49" s="30"/>
-      <c r="W49" s="36"/>
-      <c r="X49" s="34"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="34"/>
-      <c r="AA49" s="36"/>
-      <c r="AB49" s="34"/>
-      <c r="AC49" s="36"/>
-      <c r="AD49" s="34"/>
-    </row>
-    <row r="50" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F50">
         <v>48</v>
       </c>
@@ -4097,16 +3701,8 @@
       <c r="T50" s="30"/>
       <c r="U50" s="28"/>
       <c r="V50" s="30"/>
-      <c r="W50" s="36"/>
-      <c r="X50" s="34"/>
-      <c r="Y50" s="36"/>
-      <c r="Z50" s="34"/>
-      <c r="AA50" s="36"/>
-      <c r="AB50" s="34"/>
-      <c r="AC50" s="36"/>
-      <c r="AD50" s="34"/>
-    </row>
-    <row r="51" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F51">
         <v>49</v>
       </c>
@@ -4126,16 +3722,8 @@
       <c r="T51" s="30"/>
       <c r="U51" s="28"/>
       <c r="V51" s="30"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="34"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="34"/>
-      <c r="AA51" s="36"/>
-      <c r="AB51" s="34"/>
-      <c r="AC51" s="36"/>
-      <c r="AD51" s="34"/>
-    </row>
-    <row r="52" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F52">
         <v>50</v>
       </c>
@@ -4155,21 +3743,13 @@
       <c r="T52" s="27"/>
       <c r="U52" s="25"/>
       <c r="V52" s="27"/>
-      <c r="W52" s="37"/>
-      <c r="X52" s="38"/>
-      <c r="Y52" s="37"/>
-      <c r="Z52" s="38"/>
-      <c r="AA52" s="37"/>
-      <c r="AB52" s="38"/>
-      <c r="AC52" s="37"/>
-      <c r="AD52" s="38"/>
-    </row>
-    <row r="53" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F53">
         <v>51</v>
       </c>
-      <c r="G53" s="28" t="s">
-        <v>24</v>
+      <c r="G53" s="28">
+        <v>3</v>
       </c>
       <c r="H53" s="30"/>
       <c r="I53" s="28"/>
@@ -4186,16 +3766,8 @@
       <c r="T53" s="30"/>
       <c r="U53" s="28"/>
       <c r="V53" s="30"/>
-      <c r="W53" s="35"/>
-      <c r="X53" s="32"/>
-      <c r="Y53" s="35"/>
-      <c r="Z53" s="32"/>
-      <c r="AA53" s="35"/>
-      <c r="AB53" s="32"/>
-      <c r="AC53" s="35"/>
-      <c r="AD53" s="32"/>
-    </row>
-    <row r="54" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F54">
         <v>52</v>
       </c>
@@ -4215,16 +3787,8 @@
       <c r="T54" s="30"/>
       <c r="U54" s="28"/>
       <c r="V54" s="30"/>
-      <c r="W54" s="36"/>
-      <c r="X54" s="34"/>
-      <c r="Y54" s="36"/>
-      <c r="Z54" s="34"/>
-      <c r="AA54" s="36"/>
-      <c r="AB54" s="34"/>
-      <c r="AC54" s="36"/>
-      <c r="AD54" s="34"/>
-    </row>
-    <row r="55" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>53</v>
       </c>
@@ -4244,16 +3808,8 @@
       <c r="T55" s="30"/>
       <c r="U55" s="28"/>
       <c r="V55" s="30"/>
-      <c r="W55" s="36"/>
-      <c r="X55" s="34"/>
-      <c r="Y55" s="36"/>
-      <c r="Z55" s="34"/>
-      <c r="AA55" s="36"/>
-      <c r="AB55" s="34"/>
-      <c r="AC55" s="36"/>
-      <c r="AD55" s="34"/>
-    </row>
-    <row r="56" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>54</v>
       </c>
@@ -4273,16 +3829,8 @@
       <c r="T56" s="30"/>
       <c r="U56" s="28"/>
       <c r="V56" s="30"/>
-      <c r="W56" s="36"/>
-      <c r="X56" s="34"/>
-      <c r="Y56" s="36"/>
-      <c r="Z56" s="34"/>
-      <c r="AA56" s="36"/>
-      <c r="AB56" s="34"/>
-      <c r="AC56" s="36"/>
-      <c r="AD56" s="34"/>
-    </row>
-    <row r="57" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>55</v>
       </c>
@@ -4302,16 +3850,8 @@
       <c r="T57" s="30"/>
       <c r="U57" s="28"/>
       <c r="V57" s="30"/>
-      <c r="W57" s="36"/>
-      <c r="X57" s="34"/>
-      <c r="Y57" s="36"/>
-      <c r="Z57" s="34"/>
-      <c r="AA57" s="36"/>
-      <c r="AB57" s="34"/>
-      <c r="AC57" s="36"/>
-      <c r="AD57" s="34"/>
-    </row>
-    <row r="58" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>56</v>
       </c>
@@ -4331,18 +3871,266 @@
       <c r="T58" s="27"/>
       <c r="U58" s="25"/>
       <c r="V58" s="27"/>
-      <c r="W58" s="37"/>
-      <c r="X58" s="38"/>
-      <c r="Y58" s="37"/>
-      <c r="Z58" s="38"/>
-      <c r="AA58" s="37"/>
-      <c r="AB58" s="38"/>
-      <c r="AC58" s="37"/>
-      <c r="AD58" s="38"/>
-    </row>
-    <row r="59" spans="6:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>57</v>
+      </c>
+      <c r="G59" s="28">
+        <v>2</v>
+      </c>
+      <c r="H59" s="30"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="30"/>
+      <c r="M59" s="28"/>
+      <c r="N59" s="30"/>
+      <c r="O59" s="28"/>
+      <c r="P59" s="30"/>
+      <c r="Q59" s="28"/>
+      <c r="R59" s="30"/>
+      <c r="S59" s="28"/>
+      <c r="T59" s="30"/>
+      <c r="U59" s="28"/>
+      <c r="V59" s="30"/>
+    </row>
+    <row r="60" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="28"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="30"/>
+      <c r="K60" s="28"/>
+      <c r="L60" s="30"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="30"/>
+      <c r="O60" s="28"/>
+      <c r="P60" s="30"/>
+      <c r="Q60" s="28"/>
+      <c r="R60" s="30"/>
+      <c r="S60" s="28"/>
+      <c r="T60" s="30"/>
+      <c r="U60" s="28"/>
+      <c r="V60" s="30"/>
+    </row>
+    <row r="61" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="28"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="30"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="30"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="30"/>
+      <c r="O61" s="28"/>
+      <c r="P61" s="30"/>
+      <c r="Q61" s="28"/>
+      <c r="R61" s="30"/>
+      <c r="S61" s="28"/>
+      <c r="T61" s="30"/>
+      <c r="U61" s="28"/>
+      <c r="V61" s="30"/>
+    </row>
+    <row r="62" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="28"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="30"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="30"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="30"/>
+      <c r="Q62" s="28"/>
+      <c r="R62" s="30"/>
+      <c r="S62" s="28"/>
+      <c r="T62" s="30"/>
+      <c r="U62" s="28"/>
+      <c r="V62" s="30"/>
+    </row>
+    <row r="63" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="28"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="28"/>
+      <c r="L63" s="30"/>
+      <c r="M63" s="28"/>
+      <c r="N63" s="30"/>
+      <c r="O63" s="28"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="28"/>
+      <c r="R63" s="30"/>
+      <c r="S63" s="28"/>
+      <c r="T63" s="30"/>
+      <c r="U63" s="28"/>
+      <c r="V63" s="30"/>
+    </row>
+    <row r="64" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="G64" s="25"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="27"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="27"/>
+      <c r="O64" s="25"/>
+      <c r="P64" s="27"/>
+      <c r="Q64" s="25"/>
+      <c r="R64" s="27"/>
+      <c r="S64" s="25"/>
+      <c r="T64" s="27"/>
+      <c r="U64" s="25"/>
+      <c r="V64" s="27"/>
+    </row>
+    <row r="65" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="30"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="30"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="30"/>
+      <c r="O65" s="28"/>
+      <c r="P65" s="30"/>
+      <c r="Q65" s="28"/>
+      <c r="R65" s="30"/>
+      <c r="S65" s="28"/>
+      <c r="T65" s="30"/>
+      <c r="U65" s="28"/>
+      <c r="V65" s="30"/>
+    </row>
+    <row r="66" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66" s="28"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="30"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="30"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="30"/>
+      <c r="O66" s="28"/>
+      <c r="P66" s="30"/>
+      <c r="Q66" s="28"/>
+      <c r="R66" s="30"/>
+      <c r="S66" s="28"/>
+      <c r="T66" s="30"/>
+      <c r="U66" s="28"/>
+      <c r="V66" s="30"/>
+    </row>
+    <row r="67" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67" s="28"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="28"/>
+      <c r="L67" s="30"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="30"/>
+      <c r="O67" s="28"/>
+      <c r="P67" s="30"/>
+      <c r="Q67" s="28"/>
+      <c r="R67" s="30"/>
+      <c r="S67" s="28"/>
+      <c r="T67" s="30"/>
+      <c r="U67" s="28"/>
+      <c r="V67" s="30"/>
+    </row>
+    <row r="68" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="G68" s="28"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="28"/>
+      <c r="L68" s="30"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="30"/>
+      <c r="O68" s="28"/>
+      <c r="P68" s="30"/>
+      <c r="Q68" s="28"/>
+      <c r="R68" s="30"/>
+      <c r="S68" s="28"/>
+      <c r="T68" s="30"/>
+      <c r="U68" s="28"/>
+      <c r="V68" s="30"/>
+    </row>
+    <row r="69" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="G69" s="28"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="30"/>
+      <c r="O69" s="28"/>
+      <c r="P69" s="30"/>
+      <c r="Q69" s="28"/>
+      <c r="R69" s="30"/>
+      <c r="S69" s="28"/>
+      <c r="T69" s="30"/>
+      <c r="U69" s="28"/>
+      <c r="V69" s="30"/>
+    </row>
+    <row r="70" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="G70" s="25"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="25"/>
+      <c r="J70" s="27"/>
+      <c r="K70" s="25"/>
+      <c r="L70" s="27"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="27"/>
+      <c r="O70" s="25"/>
+      <c r="P70" s="27"/>
+      <c r="Q70" s="25"/>
+      <c r="R70" s="27"/>
+      <c r="S70" s="25"/>
+      <c r="T70" s="27"/>
+      <c r="U70" s="25"/>
+      <c r="V70" s="27"/>
+    </row>
+    <row r="71" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4352,11 +4140,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C69FB0-708A-40A2-9151-AAEA467E5F20}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A2:O71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4367,28 +4155,7 @@
     <col min="15" max="15" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>300</v>
-      </c>
-      <c r="C2">
-        <f>B2/5</f>
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1</v>
       </c>
@@ -4418,24 +4185,11 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>120</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3" si="0">B3/5</f>
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="31"/>
@@ -4447,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -4465,8 +4219,14 @@
       <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>1</v>
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>12</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -4478,11 +4238,24 @@
       <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>340</v>
+      </c>
+      <c r="C7">
+        <f>B7/5</f>
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
@@ -4493,14 +4266,24 @@
       <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
+      <c r="A8" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <f>B8/5</f>
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
@@ -4524,11 +4307,11 @@
       <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>20</v>
+      <c r="B10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -4543,11 +4326,11 @@
       <c r="N10" s="38"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+      <c r="A11" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
       </c>
       <c r="F11">
         <v>9</v>
@@ -4564,11 +4347,11 @@
       <c r="N11" s="32"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
+      <c r="A12" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>68</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -4585,12 +4368,21 @@
       <c r="N12" s="34"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f>B11*5</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>C11*5</f>
+        <v>40</v>
+      </c>
       <c r="F13">
         <v>11</v>
       </c>
-      <c r="G13" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="G13" s="36"/>
       <c r="H13" s="34"/>
       <c r="I13" s="36"/>
       <c r="J13" s="34"/>
@@ -4601,12 +4393,22 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <f>B12*5</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>C12*5</f>
+        <v>340</v>
       </c>
       <c r="F14">
         <v>12</v>
       </c>
-      <c r="G14" s="36"/>
+      <c r="G14" s="36">
+        <v>10</v>
+      </c>
       <c r="H14" s="34"/>
       <c r="I14" s="36"/>
       <c r="J14" s="34"/>
@@ -4645,22 +4447,22 @@
       <c r="F17">
         <v>15</v>
       </c>
-      <c r="G17" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="32"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>16</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="36">
+        <v>9</v>
+      </c>
       <c r="H18" s="34"/>
       <c r="I18" s="36"/>
       <c r="J18" s="34"/>
@@ -4712,21 +4514,21 @@
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="38"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="34"/>
     </row>
     <row r="23" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>21</v>
       </c>
-      <c r="G23" s="35" t="s">
-        <v>29</v>
+      <c r="G23" s="35">
+        <v>8</v>
       </c>
       <c r="H23" s="32"/>
       <c r="I23" s="35"/>
@@ -4805,8 +4607,8 @@
       <c r="F29">
         <v>27</v>
       </c>
-      <c r="G29" s="35" t="s">
-        <v>28</v>
+      <c r="G29" s="35">
+        <v>7</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="35"/>
@@ -4885,8 +4687,8 @@
       <c r="F35">
         <v>33</v>
       </c>
-      <c r="G35" s="35" t="s">
-        <v>27</v>
+      <c r="G35" s="35">
+        <v>6</v>
       </c>
       <c r="H35" s="32"/>
       <c r="I35" s="35"/>
@@ -4965,8 +4767,8 @@
       <c r="F41">
         <v>39</v>
       </c>
-      <c r="G41" s="35" t="s">
-        <v>26</v>
+      <c r="G41" s="35">
+        <v>5</v>
       </c>
       <c r="H41" s="32"/>
       <c r="I41" s="35"/>
@@ -5045,8 +4847,8 @@
       <c r="F47">
         <v>45</v>
       </c>
-      <c r="G47" s="35" t="s">
-        <v>25</v>
+      <c r="G47" s="35">
+        <v>4</v>
       </c>
       <c r="H47" s="32"/>
       <c r="I47" s="35"/>
@@ -5125,8 +4927,8 @@
       <c r="F53">
         <v>51</v>
       </c>
-      <c r="G53" s="35" t="s">
-        <v>24</v>
+      <c r="G53" s="35">
+        <v>3</v>
       </c>
       <c r="H53" s="32"/>
       <c r="I53" s="35"/>
@@ -5204,6 +5006,166 @@
     <row r="59" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>57</v>
+      </c>
+      <c r="G59" s="35">
+        <v>2</v>
+      </c>
+      <c r="H59" s="32"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="32"/>
+    </row>
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="36"/>
+      <c r="H60" s="34"/>
+      <c r="I60" s="36"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="34"/>
+      <c r="M60" s="36"/>
+      <c r="N60" s="34"/>
+    </row>
+    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="36"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="36"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="36"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="36"/>
+      <c r="N61" s="34"/>
+    </row>
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="36"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="36"/>
+      <c r="L62" s="34"/>
+      <c r="M62" s="36"/>
+      <c r="N62" s="34"/>
+    </row>
+    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="36"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="36"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="34"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="34"/>
+    </row>
+    <row r="64" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="38"/>
+    </row>
+    <row r="65" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="G65" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="32"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="32"/>
+    </row>
+    <row r="66" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="G66" s="36"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="34"/>
+      <c r="M66" s="36"/>
+      <c r="N66" s="34"/>
+    </row>
+    <row r="67" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="G67" s="36"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="34"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="34"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="34"/>
+    </row>
+    <row r="68" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="G68" s="36"/>
+      <c r="H68" s="34"/>
+      <c r="I68" s="36"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="36"/>
+      <c r="L68" s="34"/>
+      <c r="M68" s="36"/>
+      <c r="N68" s="34"/>
+    </row>
+    <row r="69" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="G69" s="36"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="36"/>
+      <c r="J69" s="34"/>
+      <c r="K69" s="36"/>
+      <c r="L69" s="34"/>
+      <c r="M69" s="36"/>
+      <c r="N69" s="34"/>
+    </row>
+    <row r="70" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="G70" s="37"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="38"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="38"/>
+    </row>
+    <row r="71" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5389,7 +5351,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
@@ -5413,7 +5375,7 @@
       <c r="AA4" s="47"/>
       <c r="AB4" s="48"/>
       <c r="AC4" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="AD4" s="56"/>
       <c r="AE4" s="56"/>
@@ -5667,10 +5629,10 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -5717,7 +5679,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>22</v>
@@ -5766,7 +5728,7 @@
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>78</v>
@@ -5780,7 +5742,7 @@
       <c r="G12" s="46"/>
       <c r="H12" s="47"/>
       <c r="I12" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J12" s="41"/>
       <c r="K12" s="6"/>
@@ -5964,7 +5926,7 @@
       <c r="G16" s="46"/>
       <c r="H16" s="47"/>
       <c r="I16" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J16" s="41"/>
       <c r="K16" s="6"/>
@@ -6206,7 +6168,7 @@
       <c r="G22" s="46"/>
       <c r="H22" s="47"/>
       <c r="I22" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J22" s="41"/>
       <c r="K22" s="6"/>
@@ -6488,7 +6450,7 @@
       <c r="G29" s="46"/>
       <c r="H29" s="47"/>
       <c r="I29" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J29" s="41"/>
       <c r="K29" s="6"/>
@@ -6730,7 +6692,7 @@
       <c r="G35" s="46"/>
       <c r="H35" s="47"/>
       <c r="I35" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J35" s="41"/>
       <c r="K35" s="6"/>
@@ -6972,7 +6934,7 @@
       <c r="G41" s="46"/>
       <c r="H41" s="47"/>
       <c r="I41" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J41" s="41"/>
       <c r="K41" s="6"/>
@@ -7214,7 +7176,7 @@
       <c r="G47" s="46"/>
       <c r="H47" s="47"/>
       <c r="I47" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J47" s="41"/>
       <c r="K47" s="6"/>
@@ -7456,7 +7418,7 @@
       <c r="G53" s="46"/>
       <c r="H53" s="47"/>
       <c r="I53" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J53" s="41"/>
       <c r="K53" s="6"/>
@@ -7698,7 +7660,7 @@
       <c r="G59" s="46"/>
       <c r="H59" s="47"/>
       <c r="I59" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="J59" s="41"/>
       <c r="K59" s="6"/>
@@ -7940,7 +7902,7 @@
       <c r="G65" s="46"/>
       <c r="H65" s="47"/>
       <c r="I65" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J65" s="41"/>
       <c r="K65" s="6"/>
@@ -8182,7 +8144,7 @@
       <c r="G71" s="46"/>
       <c r="H71" s="47"/>
       <c r="I71" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J71" s="41"/>
       <c r="K71" s="6"/>
@@ -8424,7 +8386,7 @@
       <c r="G77" s="46"/>
       <c r="H77" s="47"/>
       <c r="I77" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J77" s="41"/>
       <c r="K77" s="6"/>
@@ -8752,7 +8714,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="56"/>
@@ -8894,10 +8856,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -8920,7 +8882,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>22</v>
@@ -8947,7 +8909,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>78</v>
@@ -10353,7 +10315,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -10374,7 +10336,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H4" s="59"/>
       <c r="I4" s="59"/>
@@ -10526,10 +10488,10 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -10551,7 +10513,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>13</v>
@@ -10576,7 +10538,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>39</v>
@@ -11058,7 +11020,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="30"/>
       <c r="I35" s="36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J35" s="61"/>
       <c r="K35" s="34"/>
@@ -11613,7 +11575,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -11631,7 +11593,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H4" s="59"/>
       <c r="I4" s="59"/>
@@ -11763,10 +11725,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -11785,7 +11747,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -11807,7 +11769,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>39</v>
@@ -12212,7 +12174,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="30"/>
       <c r="I35" s="36" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J35" s="34"/>
       <c r="K35" s="61"/>
@@ -12688,7 +12650,7 @@
       <c r="G3" s="58"/>
       <c r="H3" s="58"/>
       <c r="I3" s="23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
@@ -12704,7 +12666,7 @@
       <c r="G4" s="58"/>
       <c r="H4" s="58"/>
       <c r="I4" s="28" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J4" s="59"/>
       <c r="K4" s="59"/>
@@ -12729,7 +12691,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>13</v>
@@ -12741,7 +12703,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
@@ -12823,7 +12785,7 @@
       </c>
       <c r="I9" s="59"/>
       <c r="J9" s="62" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K9" s="59"/>
       <c r="L9" s="62"/>
@@ -12833,10 +12795,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -12853,7 +12815,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -12873,7 +12835,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>83</v>
@@ -14090,7 +14052,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="32"/>
@@ -14130,7 +14092,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>13</v>
@@ -14142,7 +14104,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H6" s="31"/>
       <c r="I6" s="31"/>
@@ -14172,7 +14134,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="61"/>
@@ -14220,10 +14182,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -14240,7 +14202,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -14258,7 +14220,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12">
         <v>83</v>
@@ -14318,7 +14280,7 @@
         <v>12</v>
       </c>
       <c r="G14" s="36" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H14" s="63"/>
       <c r="I14" s="61"/>
@@ -14397,7 +14359,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="61" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H19" s="61"/>
       <c r="I19" s="33"/>
@@ -14435,7 +14397,7 @@
       <c r="H21" s="63"/>
       <c r="I21" s="33"/>
       <c r="J21" s="64" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="K21" s="33"/>
       <c r="L21" s="64"/>

</xml_diff>

<commit_message>
Add html structure for Building 6
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1438" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0392D9E4-CBFF-43EC-8CBF-71C0DF92AB7F}"/>
+  <xr:revisionPtr revIDLastSave="1540" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{253E2CF4-DC63-4507-B633-490965825E66}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" firstSheet="2" activeTab="7" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" firstSheet="4" activeTab="10" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1-H1 &amp; H2" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="B4-H2" sheetId="10" r:id="rId7"/>
     <sheet name="B5-H1" sheetId="11" r:id="rId8"/>
     <sheet name="B5-H2" sheetId="13" r:id="rId9"/>
+    <sheet name="B6-H1" sheetId="15" r:id="rId10"/>
+    <sheet name="B6-H2" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="44">
   <si>
     <t>Columns</t>
   </si>
@@ -347,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -426,6 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2513,13 +2516,3367 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38302237-DF36-476F-B4B3-F0D47F7977D5}">
+  <dimension ref="A1:V98"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="31" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H1" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>14</v>
+      </c>
+      <c r="U2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="62">
+        <v>9</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E11" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="62">
+        <v>8</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>300</v>
+      </c>
+      <c r="C15">
+        <f>B15/5</f>
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="59"/>
+      <c r="T15" s="59"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <f>B16/5</f>
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="59"/>
+      <c r="T17" s="59"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="68"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="59"/>
+      <c r="T19" s="59"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="59"/>
+      <c r="T20" s="59"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="62">
+        <v>7</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <f>B20*5</f>
+        <v>70</v>
+      </c>
+      <c r="C22">
+        <f>C20*5</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="59"/>
+      <c r="T22" s="59"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <f>B21*5</f>
+        <v>300</v>
+      </c>
+      <c r="C23">
+        <f>C21*5</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="59"/>
+      <c r="T23" s="59"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="59"/>
+      <c r="T24" s="59"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="62"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="62">
+        <v>6</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="59"/>
+      <c r="T27" s="59"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="62"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="62"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="59"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="69"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="59"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="66"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="66"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="59"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="62"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="59"/>
+    </row>
+    <row r="33" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="62">
+        <v>5</v>
+      </c>
+      <c r="J33" s="20"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="59"/>
+      <c r="T33" s="59"/>
+    </row>
+    <row r="34" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="62"/>
+      <c r="S34" s="59"/>
+      <c r="T34" s="59"/>
+    </row>
+    <row r="35" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="59"/>
+      <c r="T35" s="59"/>
+    </row>
+    <row r="36" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="69"/>
+      <c r="S36" s="59"/>
+      <c r="T36" s="59"/>
+    </row>
+    <row r="37" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="68"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="68"/>
+      <c r="Q37" s="66"/>
+      <c r="R37" s="67"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+    </row>
+    <row r="38" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="62"/>
+      <c r="S38" s="59"/>
+      <c r="T38" s="59"/>
+    </row>
+    <row r="39" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="62">
+        <v>4</v>
+      </c>
+      <c r="J39" s="20"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="62"/>
+      <c r="S39" s="59"/>
+      <c r="T39" s="59"/>
+    </row>
+    <row r="40" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="62"/>
+      <c r="S40" s="59"/>
+      <c r="T40" s="59"/>
+    </row>
+    <row r="41" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="59"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="62"/>
+      <c r="S41" s="59"/>
+      <c r="T41" s="59"/>
+    </row>
+    <row r="42" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="69"/>
+      <c r="S42" s="59"/>
+      <c r="T42" s="59"/>
+    </row>
+    <row r="43" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="66"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="66"/>
+      <c r="N43" s="68"/>
+      <c r="O43" s="66"/>
+      <c r="P43" s="68"/>
+      <c r="Q43" s="66"/>
+      <c r="R43" s="67"/>
+      <c r="S43" s="59"/>
+      <c r="T43" s="59"/>
+    </row>
+    <row r="44" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="62"/>
+      <c r="S44" s="59"/>
+      <c r="T44" s="59"/>
+    </row>
+    <row r="45" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="62">
+        <v>3</v>
+      </c>
+      <c r="J45" s="20"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="62"/>
+      <c r="S45" s="59"/>
+      <c r="T45" s="59"/>
+    </row>
+    <row r="46" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="62"/>
+      <c r="S46" s="59"/>
+      <c r="T46" s="59"/>
+    </row>
+    <row r="47" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="62"/>
+      <c r="S47" s="59"/>
+      <c r="T47" s="59"/>
+    </row>
+    <row r="48" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="22"/>
+      <c r="Q48" s="21"/>
+      <c r="R48" s="69"/>
+      <c r="S48" s="59"/>
+      <c r="T48" s="59"/>
+    </row>
+    <row r="49" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="68"/>
+      <c r="M49" s="66"/>
+      <c r="N49" s="68"/>
+      <c r="O49" s="66"/>
+      <c r="P49" s="68"/>
+      <c r="Q49" s="66"/>
+      <c r="R49" s="67"/>
+      <c r="S49" s="59"/>
+      <c r="T49" s="59"/>
+    </row>
+    <row r="50" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="62"/>
+      <c r="S50" s="59"/>
+      <c r="T50" s="59"/>
+    </row>
+    <row r="51" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="62">
+        <v>2</v>
+      </c>
+      <c r="J51" s="20"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="62"/>
+      <c r="S51" s="59"/>
+      <c r="T51" s="59"/>
+    </row>
+    <row r="52" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="62"/>
+      <c r="S52" s="59"/>
+      <c r="T52" s="59"/>
+    </row>
+    <row r="53" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>51</v>
+      </c>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="62"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="62"/>
+      <c r="S53" s="59"/>
+      <c r="T53" s="59"/>
+    </row>
+    <row r="54" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>52</v>
+      </c>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="62"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="20"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="20"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="62"/>
+      <c r="S54" s="59"/>
+      <c r="T54" s="59"/>
+    </row>
+    <row r="55" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>53</v>
+      </c>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="59"/>
+      <c r="S55" s="59"/>
+      <c r="T55" s="59"/>
+    </row>
+    <row r="56" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>54</v>
+      </c>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="59"/>
+      <c r="K56" s="59"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="59"/>
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+      <c r="S56" s="59"/>
+      <c r="T56" s="59"/>
+    </row>
+    <row r="57" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="68"/>
+      <c r="K57" s="66"/>
+      <c r="L57" s="67"/>
+      <c r="M57" s="67"/>
+      <c r="N57" s="67"/>
+      <c r="O57" s="67"/>
+      <c r="P57" s="68"/>
+      <c r="Q57" s="66"/>
+      <c r="R57" s="68"/>
+      <c r="S57" s="59"/>
+      <c r="T57" s="59"/>
+    </row>
+    <row r="58" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="19">
+        <v>1</v>
+      </c>
+      <c r="J58" s="20"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="62"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="20"/>
+      <c r="S58" s="59"/>
+      <c r="T58" s="59"/>
+    </row>
+    <row r="59" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>57</v>
+      </c>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="62"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="20"/>
+      <c r="S59" s="59"/>
+      <c r="T59" s="59"/>
+    </row>
+    <row r="60" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="62"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="62"/>
+      <c r="O60" s="62"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="59"/>
+      <c r="T60" s="59"/>
+    </row>
+    <row r="61" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="62"/>
+      <c r="M61" s="62"/>
+      <c r="N61" s="62"/>
+      <c r="O61" s="62"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="19"/>
+      <c r="R61" s="20"/>
+      <c r="S61" s="59"/>
+      <c r="T61" s="59"/>
+    </row>
+    <row r="62" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="69"/>
+      <c r="M62" s="69"/>
+      <c r="N62" s="69"/>
+      <c r="O62" s="69"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="21"/>
+      <c r="R62" s="22"/>
+      <c r="S62" s="59"/>
+      <c r="T62" s="59"/>
+    </row>
+    <row r="63" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="G63" s="42"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
+      <c r="O63" s="58"/>
+      <c r="P63" s="58"/>
+      <c r="Q63" s="42"/>
+      <c r="R63" s="42"/>
+      <c r="S63" s="42"/>
+      <c r="T63" s="42"/>
+      <c r="U63" s="58"/>
+      <c r="V63" s="58"/>
+    </row>
+    <row r="64" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="G64" s="42"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
+      <c r="J64" s="58"/>
+      <c r="K64" s="58"/>
+      <c r="L64" s="58"/>
+      <c r="M64" s="58"/>
+      <c r="N64" s="58"/>
+      <c r="O64" s="58"/>
+      <c r="P64" s="58"/>
+      <c r="Q64" s="42"/>
+      <c r="R64" s="42"/>
+      <c r="S64" s="42"/>
+      <c r="T64" s="42"/>
+      <c r="U64" s="42"/>
+      <c r="V64" s="42"/>
+    </row>
+    <row r="65" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G65" s="42"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
+      <c r="J65" s="58"/>
+      <c r="K65" s="58"/>
+      <c r="L65" s="58"/>
+      <c r="M65" s="58"/>
+      <c r="N65" s="58"/>
+      <c r="O65" s="42"/>
+      <c r="P65" s="42"/>
+      <c r="Q65" s="42"/>
+      <c r="R65" s="42"/>
+      <c r="S65" s="42"/>
+      <c r="T65" s="42"/>
+      <c r="U65" s="42"/>
+      <c r="V65" s="42"/>
+    </row>
+    <row r="66" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G66" s="42"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
+      <c r="J66" s="58"/>
+      <c r="K66" s="58"/>
+      <c r="L66" s="58"/>
+      <c r="M66" s="58"/>
+      <c r="N66" s="58"/>
+      <c r="O66" s="58"/>
+      <c r="P66" s="58"/>
+      <c r="Q66" s="42"/>
+      <c r="R66" s="42"/>
+      <c r="S66" s="42"/>
+      <c r="T66" s="42"/>
+      <c r="U66" s="42"/>
+      <c r="V66" s="42"/>
+    </row>
+    <row r="67" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G67" s="42"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="58"/>
+      <c r="J67" s="58"/>
+      <c r="K67" s="58"/>
+      <c r="L67" s="58"/>
+      <c r="M67" s="58"/>
+      <c r="N67" s="58"/>
+      <c r="O67" s="58"/>
+      <c r="P67" s="58"/>
+      <c r="Q67" s="42"/>
+      <c r="R67" s="42"/>
+      <c r="S67" s="42"/>
+      <c r="T67" s="42"/>
+      <c r="U67" s="42"/>
+      <c r="V67" s="42"/>
+    </row>
+    <row r="68" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G68" s="42"/>
+      <c r="H68" s="58"/>
+      <c r="I68" s="58"/>
+      <c r="J68" s="58"/>
+      <c r="K68" s="58"/>
+      <c r="L68" s="58"/>
+      <c r="M68" s="58"/>
+      <c r="N68" s="58"/>
+      <c r="O68" s="58"/>
+      <c r="P68" s="58"/>
+      <c r="Q68" s="42"/>
+      <c r="R68" s="42"/>
+      <c r="S68" s="42"/>
+      <c r="T68" s="42"/>
+      <c r="U68" s="42"/>
+      <c r="V68" s="42"/>
+    </row>
+    <row r="69" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="58"/>
+      <c r="J69" s="58"/>
+      <c r="K69" s="58"/>
+      <c r="L69" s="58"/>
+      <c r="M69" s="58"/>
+      <c r="N69" s="58"/>
+      <c r="O69" s="58"/>
+      <c r="P69" s="58"/>
+      <c r="Q69" s="42"/>
+      <c r="R69" s="42"/>
+      <c r="S69" s="42"/>
+      <c r="T69" s="42"/>
+      <c r="U69" s="42"/>
+      <c r="V69" s="42"/>
+    </row>
+    <row r="70" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G70" s="42"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
+      <c r="J70" s="42"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="42"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="42"/>
+      <c r="O70" s="58"/>
+      <c r="P70" s="58"/>
+      <c r="Q70" s="42"/>
+      <c r="R70" s="42"/>
+      <c r="S70" s="42"/>
+      <c r="T70" s="42"/>
+      <c r="U70" s="42"/>
+      <c r="V70" s="42"/>
+    </row>
+    <row r="71" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G71" s="42"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="58"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="58"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="58"/>
+      <c r="O71" s="58"/>
+      <c r="P71" s="58"/>
+      <c r="Q71" s="42"/>
+      <c r="R71" s="42"/>
+      <c r="S71" s="42"/>
+      <c r="T71" s="42"/>
+      <c r="U71" s="42"/>
+      <c r="V71" s="42"/>
+    </row>
+    <row r="72" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G72" s="42"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="58"/>
+      <c r="K72" s="58"/>
+      <c r="L72" s="58"/>
+      <c r="M72" s="58"/>
+      <c r="N72" s="58"/>
+      <c r="O72" s="58"/>
+      <c r="P72" s="58"/>
+      <c r="Q72" s="42"/>
+      <c r="R72" s="42"/>
+      <c r="S72" s="42"/>
+      <c r="T72" s="42"/>
+      <c r="U72" s="42"/>
+      <c r="V72" s="42"/>
+    </row>
+    <row r="73" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G73" s="42"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="58"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="58"/>
+      <c r="M73" s="58"/>
+      <c r="N73" s="58"/>
+      <c r="O73" s="58"/>
+      <c r="P73" s="58"/>
+      <c r="Q73" s="42"/>
+      <c r="R73" s="42"/>
+      <c r="S73" s="42"/>
+      <c r="T73" s="42"/>
+      <c r="U73" s="42"/>
+      <c r="V73" s="42"/>
+    </row>
+    <row r="74" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G74" s="42"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="58"/>
+      <c r="M74" s="58"/>
+      <c r="N74" s="58"/>
+      <c r="O74" s="58"/>
+      <c r="P74" s="58"/>
+      <c r="Q74" s="42"/>
+      <c r="R74" s="42"/>
+      <c r="S74" s="42"/>
+      <c r="T74" s="42"/>
+      <c r="U74" s="42"/>
+      <c r="V74" s="42"/>
+    </row>
+    <row r="75" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G75" s="42"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="58"/>
+      <c r="J75" s="58"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="58"/>
+      <c r="M75" s="58"/>
+      <c r="N75" s="58"/>
+      <c r="O75" s="58"/>
+      <c r="P75" s="58"/>
+      <c r="Q75" s="42"/>
+      <c r="R75" s="42"/>
+      <c r="S75" s="42"/>
+      <c r="T75" s="42"/>
+      <c r="U75" s="42"/>
+      <c r="V75" s="42"/>
+    </row>
+    <row r="76" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G76" s="42"/>
+      <c r="H76" s="58"/>
+      <c r="I76" s="58"/>
+      <c r="J76" s="58"/>
+      <c r="K76" s="58"/>
+      <c r="L76" s="58"/>
+      <c r="M76" s="58"/>
+      <c r="N76" s="58"/>
+      <c r="O76" s="58"/>
+      <c r="P76" s="58"/>
+      <c r="Q76" s="42"/>
+      <c r="R76" s="42"/>
+      <c r="S76" s="42"/>
+      <c r="T76" s="42"/>
+      <c r="U76" s="42"/>
+      <c r="V76" s="42"/>
+    </row>
+    <row r="77" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G77" s="42"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
+      <c r="J77" s="58"/>
+      <c r="K77" s="58"/>
+      <c r="L77" s="58"/>
+      <c r="M77" s="58"/>
+      <c r="N77" s="58"/>
+      <c r="O77" s="58"/>
+      <c r="P77" s="58"/>
+      <c r="Q77" s="42"/>
+      <c r="R77" s="42"/>
+      <c r="S77" s="42"/>
+      <c r="T77" s="42"/>
+      <c r="U77" s="42"/>
+      <c r="V77" s="42"/>
+    </row>
+    <row r="78" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G78" s="42"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="58"/>
+      <c r="J78" s="42"/>
+      <c r="K78" s="58"/>
+      <c r="L78" s="42"/>
+      <c r="M78" s="58"/>
+      <c r="N78" s="42"/>
+      <c r="O78" s="58"/>
+      <c r="P78" s="58"/>
+      <c r="Q78" s="42"/>
+      <c r="R78" s="42"/>
+      <c r="S78" s="42"/>
+      <c r="T78" s="42"/>
+      <c r="U78" s="42"/>
+      <c r="V78" s="42"/>
+    </row>
+    <row r="79" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G79" s="42"/>
+      <c r="H79" s="58"/>
+      <c r="I79" s="58"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="58"/>
+      <c r="M79" s="58"/>
+      <c r="N79" s="58"/>
+      <c r="O79" s="58"/>
+      <c r="P79" s="58"/>
+      <c r="Q79" s="42"/>
+      <c r="R79" s="42"/>
+      <c r="S79" s="42"/>
+      <c r="T79" s="42"/>
+      <c r="U79" s="42"/>
+      <c r="V79" s="42"/>
+    </row>
+    <row r="80" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G80" s="42"/>
+      <c r="H80" s="58"/>
+      <c r="I80" s="58"/>
+      <c r="J80" s="58"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="58"/>
+      <c r="M80" s="58"/>
+      <c r="N80" s="58"/>
+      <c r="O80" s="58"/>
+      <c r="P80" s="58"/>
+      <c r="Q80" s="42"/>
+      <c r="R80" s="42"/>
+      <c r="S80" s="42"/>
+      <c r="T80" s="42"/>
+      <c r="U80" s="42"/>
+      <c r="V80" s="42"/>
+    </row>
+    <row r="81" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G81" s="42"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
+      <c r="J81" s="58"/>
+      <c r="K81" s="58"/>
+      <c r="L81" s="58"/>
+      <c r="M81" s="58"/>
+      <c r="N81" s="58"/>
+      <c r="O81" s="58"/>
+      <c r="P81" s="58"/>
+      <c r="Q81" s="42"/>
+      <c r="R81" s="42"/>
+      <c r="S81" s="42"/>
+      <c r="T81" s="42"/>
+      <c r="U81" s="42"/>
+      <c r="V81" s="42"/>
+    </row>
+    <row r="82" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G82" s="42"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="58"/>
+      <c r="J82" s="58"/>
+      <c r="K82" s="58"/>
+      <c r="L82" s="58"/>
+      <c r="M82" s="58"/>
+      <c r="N82" s="58"/>
+      <c r="O82" s="58"/>
+      <c r="P82" s="58"/>
+      <c r="Q82" s="42"/>
+      <c r="R82" s="42"/>
+      <c r="S82" s="42"/>
+      <c r="T82" s="42"/>
+      <c r="U82" s="42"/>
+      <c r="V82" s="42"/>
+    </row>
+    <row r="83" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G83" s="42"/>
+      <c r="H83" s="58"/>
+      <c r="I83" s="58"/>
+      <c r="J83" s="58"/>
+      <c r="K83" s="58"/>
+      <c r="L83" s="58"/>
+      <c r="M83" s="58"/>
+      <c r="N83" s="58"/>
+      <c r="O83" s="58"/>
+      <c r="P83" s="58"/>
+      <c r="Q83" s="42"/>
+      <c r="R83" s="42"/>
+      <c r="S83" s="42"/>
+      <c r="T83" s="42"/>
+      <c r="U83" s="42"/>
+      <c r="V83" s="42"/>
+    </row>
+    <row r="84" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G84" s="42"/>
+      <c r="H84" s="58"/>
+      <c r="I84" s="58"/>
+      <c r="J84" s="58"/>
+      <c r="K84" s="58"/>
+      <c r="L84" s="58"/>
+      <c r="M84" s="58"/>
+      <c r="N84" s="58"/>
+      <c r="O84" s="58"/>
+      <c r="P84" s="58"/>
+      <c r="Q84" s="42"/>
+      <c r="R84" s="42"/>
+      <c r="S84" s="42"/>
+      <c r="T84" s="42"/>
+      <c r="U84" s="42"/>
+      <c r="V84" s="42"/>
+    </row>
+    <row r="85" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G85" s="42"/>
+      <c r="H85" s="58"/>
+      <c r="I85" s="58"/>
+      <c r="J85" s="58"/>
+      <c r="K85" s="58"/>
+      <c r="L85" s="58"/>
+      <c r="M85" s="58"/>
+      <c r="N85" s="58"/>
+      <c r="O85" s="58"/>
+      <c r="P85" s="58"/>
+      <c r="Q85" s="42"/>
+      <c r="R85" s="42"/>
+      <c r="S85" s="42"/>
+      <c r="T85" s="42"/>
+      <c r="U85" s="42"/>
+      <c r="V85" s="42"/>
+    </row>
+    <row r="86" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G86" s="42"/>
+      <c r="H86" s="58"/>
+      <c r="I86" s="58"/>
+      <c r="J86" s="42"/>
+      <c r="K86" s="58"/>
+      <c r="L86" s="42"/>
+      <c r="M86" s="58"/>
+      <c r="N86" s="42"/>
+      <c r="O86" s="58"/>
+      <c r="P86" s="58"/>
+      <c r="Q86" s="42"/>
+      <c r="R86" s="42"/>
+      <c r="S86" s="42"/>
+      <c r="T86" s="42"/>
+      <c r="U86" s="42"/>
+      <c r="V86" s="42"/>
+    </row>
+    <row r="87" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G87" s="42"/>
+      <c r="H87" s="42"/>
+      <c r="I87" s="58"/>
+      <c r="J87" s="58"/>
+      <c r="K87" s="58"/>
+      <c r="L87" s="58"/>
+      <c r="M87" s="58"/>
+      <c r="N87" s="58"/>
+      <c r="O87" s="58"/>
+      <c r="P87" s="58"/>
+      <c r="Q87" s="42"/>
+      <c r="R87" s="42"/>
+      <c r="S87" s="42"/>
+      <c r="T87" s="42"/>
+      <c r="U87" s="42"/>
+      <c r="V87" s="42"/>
+    </row>
+    <row r="88" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G88" s="42"/>
+      <c r="H88" s="42"/>
+      <c r="I88" s="58"/>
+      <c r="J88" s="58"/>
+      <c r="K88" s="58"/>
+      <c r="L88" s="58"/>
+      <c r="M88" s="58"/>
+      <c r="N88" s="58"/>
+      <c r="O88" s="58"/>
+      <c r="P88" s="58"/>
+      <c r="Q88" s="42"/>
+      <c r="R88" s="42"/>
+      <c r="S88" s="42"/>
+      <c r="T88" s="42"/>
+      <c r="U88" s="42"/>
+      <c r="V88" s="42"/>
+    </row>
+    <row r="89" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="G89" s="42"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="58"/>
+      <c r="J89" s="58"/>
+      <c r="K89" s="58"/>
+      <c r="L89" s="58"/>
+      <c r="M89" s="58"/>
+      <c r="N89" s="58"/>
+      <c r="O89" s="58"/>
+      <c r="P89" s="58"/>
+      <c r="Q89" s="42"/>
+      <c r="R89" s="42"/>
+      <c r="S89" s="42"/>
+      <c r="T89" s="42"/>
+      <c r="U89" s="42"/>
+      <c r="V89" s="42"/>
+    </row>
+    <row r="90" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="I90" s="58"/>
+      <c r="J90" s="58"/>
+      <c r="K90" s="58"/>
+      <c r="L90" s="58"/>
+      <c r="M90" s="58"/>
+      <c r="N90" s="58"/>
+      <c r="O90" s="58"/>
+      <c r="P90" s="58"/>
+    </row>
+    <row r="91" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="I91" s="58"/>
+      <c r="J91" s="42"/>
+      <c r="K91" s="58"/>
+      <c r="L91" s="42"/>
+      <c r="M91" s="58"/>
+      <c r="N91" s="42"/>
+      <c r="O91" s="58"/>
+      <c r="P91" s="58"/>
+    </row>
+    <row r="92" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="I92" s="58"/>
+      <c r="J92" s="58"/>
+      <c r="K92" s="58"/>
+      <c r="L92" s="58"/>
+      <c r="M92" s="58"/>
+      <c r="N92" s="58"/>
+      <c r="O92" s="58"/>
+      <c r="P92" s="58"/>
+    </row>
+    <row r="93" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="L93" s="58"/>
+      <c r="M93" s="58"/>
+      <c r="N93" s="58"/>
+      <c r="O93" s="58"/>
+    </row>
+    <row r="94" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="L94" s="58"/>
+      <c r="M94" s="58"/>
+      <c r="N94" s="58"/>
+      <c r="O94" s="58"/>
+    </row>
+    <row r="95" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="L95" s="58"/>
+      <c r="M95" s="58"/>
+      <c r="N95" s="58"/>
+      <c r="O95" s="58"/>
+    </row>
+    <row r="96" spans="7:22" x14ac:dyDescent="0.25">
+      <c r="L96" s="58"/>
+      <c r="M96" s="58"/>
+      <c r="N96" s="58"/>
+      <c r="O96" s="58"/>
+    </row>
+    <row r="97" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L97" s="58"/>
+      <c r="M97" s="58"/>
+      <c r="N97" s="58"/>
+      <c r="O97" s="58"/>
+    </row>
+    <row r="98" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L98" s="58"/>
+      <c r="M98" s="58"/>
+      <c r="N98" s="58"/>
+      <c r="O98" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ECA445-E2A0-445A-8462-93AEA1A76CDC}">
+  <dimension ref="A1:T98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="18" width="3.7109375" style="42" customWidth="1"/>
+    <col min="19" max="20" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H1" s="78" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G2" s="42">
+        <v>1</v>
+      </c>
+      <c r="H2" s="42">
+        <v>2</v>
+      </c>
+      <c r="I2" s="42">
+        <v>3</v>
+      </c>
+      <c r="J2" s="42">
+        <v>4</v>
+      </c>
+      <c r="K2" s="42">
+        <v>5</v>
+      </c>
+      <c r="L2" s="42">
+        <v>6</v>
+      </c>
+      <c r="M2" s="42">
+        <v>7</v>
+      </c>
+      <c r="N2" s="42">
+        <v>8</v>
+      </c>
+      <c r="O2" s="42">
+        <v>9</v>
+      </c>
+      <c r="P2" s="42">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="42">
+        <v>11</v>
+      </c>
+      <c r="R2" s="42">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="64">
+        <v>9</v>
+      </c>
+      <c r="J10" s="74"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E11" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="75"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="R14" s="58"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>395</v>
+      </c>
+      <c r="C15">
+        <f>B15/5</f>
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f>60+90</f>
+        <v>150</v>
+      </c>
+      <c r="C16">
+        <f>B16/5</f>
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="64">
+        <v>8</v>
+      </c>
+      <c r="J16" s="74"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="75"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="72"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="74"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="R21" s="58"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <f>B20*5</f>
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <f>C20*5</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="64">
+        <v>7</v>
+      </c>
+      <c r="J22" s="74"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <f>B21*5</f>
+        <v>300</v>
+      </c>
+      <c r="C23">
+        <f>C21*5</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="72"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="70"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>25</v>
+      </c>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>26</v>
+      </c>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="64">
+        <v>6</v>
+      </c>
+      <c r="J28" s="74"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="74"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="74"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="74"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>28</v>
+      </c>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>29</v>
+      </c>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="74"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+    </row>
+    <row r="33" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>31</v>
+      </c>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="64">
+        <v>5</v>
+      </c>
+      <c r="J33" s="74"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+    </row>
+    <row r="34" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>32</v>
+      </c>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="74"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+    </row>
+    <row r="35" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>33</v>
+      </c>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="74"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+    </row>
+    <row r="36" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>34</v>
+      </c>
+      <c r="G36" s="59"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="76"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+    </row>
+    <row r="37" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>35</v>
+      </c>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="71"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="70"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+    </row>
+    <row r="38" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+    </row>
+    <row r="39" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>37</v>
+      </c>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="64">
+        <v>4</v>
+      </c>
+      <c r="J39" s="74"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="74"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="74"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+    </row>
+    <row r="40" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>38</v>
+      </c>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="64"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="74"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="74"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+    </row>
+    <row r="41" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>39</v>
+      </c>
+      <c r="G41" s="59"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="74"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="74"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+    </row>
+    <row r="42" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="75"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+    </row>
+    <row r="43" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>41</v>
+      </c>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="71"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="70"/>
+      <c r="N43" s="72"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+    </row>
+    <row r="44" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>42</v>
+      </c>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="74"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+    </row>
+    <row r="45" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>43</v>
+      </c>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="64">
+        <v>3</v>
+      </c>
+      <c r="J45" s="74"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="74"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="74"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+    </row>
+    <row r="46" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>44</v>
+      </c>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="74"/>
+      <c r="M46" s="73"/>
+      <c r="N46" s="74"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="29"/>
+    </row>
+    <row r="47" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="74"/>
+      <c r="K47" s="73"/>
+      <c r="L47" s="74"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="74"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+    </row>
+    <row r="48" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>46</v>
+      </c>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="65"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="75"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="75"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+    </row>
+    <row r="49" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>47</v>
+      </c>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="71"/>
+      <c r="J49" s="72"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="72"/>
+      <c r="M49" s="70"/>
+      <c r="N49" s="72"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="29"/>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>48</v>
+      </c>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="73"/>
+      <c r="L50" s="74"/>
+      <c r="M50" s="73"/>
+      <c r="N50" s="74"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>49</v>
+      </c>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="64">
+        <v>2</v>
+      </c>
+      <c r="J51" s="74"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="74"/>
+      <c r="M51" s="73"/>
+      <c r="N51" s="74"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52" s="59"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="74"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="73"/>
+      <c r="N52" s="74"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="29"/>
+    </row>
+    <row r="53" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>51</v>
+      </c>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="64"/>
+      <c r="J53" s="74"/>
+      <c r="K53" s="73"/>
+      <c r="L53" s="74"/>
+      <c r="M53" s="73"/>
+      <c r="N53" s="74"/>
+      <c r="O53" s="29"/>
+      <c r="P53" s="29"/>
+    </row>
+    <row r="54" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>52</v>
+      </c>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="64"/>
+      <c r="J54" s="74"/>
+      <c r="K54" s="73"/>
+      <c r="L54" s="74"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="74"/>
+      <c r="O54" s="29"/>
+      <c r="P54" s="29"/>
+    </row>
+    <row r="55" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>53</v>
+      </c>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="29"/>
+      <c r="P55" s="29"/>
+    </row>
+    <row r="56" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>54</v>
+      </c>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="59"/>
+      <c r="K56" s="59"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="59"/>
+      <c r="N56" s="59"/>
+      <c r="O56" s="29"/>
+      <c r="P56" s="29"/>
+    </row>
+    <row r="57" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="71"/>
+      <c r="K57" s="71"/>
+      <c r="L57" s="71"/>
+      <c r="M57" s="71"/>
+      <c r="N57" s="72"/>
+      <c r="O57" s="29"/>
+      <c r="P57" s="29"/>
+    </row>
+    <row r="58" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>56</v>
+      </c>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="64"/>
+      <c r="K58" s="64"/>
+      <c r="L58" s="64"/>
+      <c r="M58" s="64"/>
+      <c r="N58" s="74"/>
+      <c r="O58" s="29"/>
+      <c r="P58" s="29"/>
+    </row>
+    <row r="59" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>57</v>
+      </c>
+      <c r="G59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="73">
+        <v>1</v>
+      </c>
+      <c r="J59" s="64"/>
+      <c r="K59" s="64"/>
+      <c r="L59" s="64"/>
+      <c r="M59" s="64"/>
+      <c r="N59" s="74"/>
+      <c r="O59" s="29"/>
+      <c r="P59" s="29"/>
+    </row>
+    <row r="60" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>58</v>
+      </c>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="64"/>
+      <c r="K60" s="64"/>
+      <c r="L60" s="64"/>
+      <c r="M60" s="64"/>
+      <c r="N60" s="74"/>
+      <c r="O60" s="29"/>
+      <c r="P60" s="29"/>
+    </row>
+    <row r="61" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>59</v>
+      </c>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="73"/>
+      <c r="J61" s="64"/>
+      <c r="K61" s="64"/>
+      <c r="L61" s="64"/>
+      <c r="M61" s="64"/>
+      <c r="N61" s="74"/>
+      <c r="O61" s="29"/>
+      <c r="P61" s="29"/>
+    </row>
+    <row r="62" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>60</v>
+      </c>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="75"/>
+      <c r="J62" s="65"/>
+      <c r="K62" s="65"/>
+      <c r="L62" s="65"/>
+      <c r="M62" s="65"/>
+      <c r="N62" s="76"/>
+      <c r="O62" s="29"/>
+      <c r="P62" s="29"/>
+    </row>
+    <row r="63" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>61</v>
+      </c>
+      <c r="H63" s="58"/>
+      <c r="I63" s="58"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="58"/>
+      <c r="O63" s="58"/>
+      <c r="P63" s="58"/>
+    </row>
+    <row r="64" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>62</v>
+      </c>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
+      <c r="J64" s="58"/>
+      <c r="K64" s="58"/>
+      <c r="L64" s="58"/>
+      <c r="M64" s="58"/>
+      <c r="N64" s="58"/>
+      <c r="O64" s="58"/>
+      <c r="P64" s="58"/>
+    </row>
+    <row r="65" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>63</v>
+      </c>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
+      <c r="J65" s="58"/>
+      <c r="K65" s="58"/>
+      <c r="L65" s="58"/>
+      <c r="M65" s="58"/>
+      <c r="N65" s="58"/>
+    </row>
+    <row r="66" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>64</v>
+      </c>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
+      <c r="J66" s="58"/>
+      <c r="K66" s="58"/>
+      <c r="L66" s="58"/>
+      <c r="M66" s="58"/>
+      <c r="N66" s="58"/>
+      <c r="O66" s="58"/>
+      <c r="P66" s="58"/>
+    </row>
+    <row r="67" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>65</v>
+      </c>
+      <c r="H67" s="58"/>
+      <c r="I67" s="58"/>
+      <c r="J67" s="58"/>
+      <c r="K67" s="58"/>
+      <c r="L67" s="58"/>
+      <c r="M67" s="58"/>
+      <c r="N67" s="58"/>
+      <c r="O67" s="58"/>
+      <c r="P67" s="58"/>
+    </row>
+    <row r="68" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>66</v>
+      </c>
+      <c r="H68" s="58"/>
+      <c r="I68" s="58"/>
+      <c r="J68" s="58"/>
+      <c r="K68" s="58"/>
+      <c r="L68" s="58"/>
+      <c r="M68" s="58"/>
+      <c r="N68" s="58"/>
+      <c r="O68" s="58"/>
+      <c r="P68" s="58"/>
+    </row>
+    <row r="69" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>67</v>
+      </c>
+      <c r="I69" s="58"/>
+      <c r="J69" s="58"/>
+      <c r="K69" s="58"/>
+      <c r="L69" s="58"/>
+      <c r="M69" s="58"/>
+      <c r="N69" s="58"/>
+      <c r="O69" s="58"/>
+      <c r="P69" s="58"/>
+    </row>
+    <row r="70" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>68</v>
+      </c>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
+      <c r="K70" s="58"/>
+      <c r="M70" s="58"/>
+      <c r="O70" s="58"/>
+      <c r="P70" s="58"/>
+    </row>
+    <row r="71" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>69</v>
+      </c>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="58"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="58"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="58"/>
+      <c r="O71" s="58"/>
+      <c r="P71" s="58"/>
+    </row>
+    <row r="72" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="58"/>
+      <c r="K72" s="58"/>
+      <c r="L72" s="58"/>
+      <c r="M72" s="58"/>
+      <c r="N72" s="58"/>
+      <c r="O72" s="58"/>
+      <c r="P72" s="58"/>
+    </row>
+    <row r="73" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>71</v>
+      </c>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="58"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="58"/>
+      <c r="M73" s="58"/>
+      <c r="N73" s="58"/>
+      <c r="O73" s="58"/>
+      <c r="P73" s="58"/>
+    </row>
+    <row r="74" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>72</v>
+      </c>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="58"/>
+      <c r="M74" s="58"/>
+      <c r="N74" s="58"/>
+      <c r="O74" s="58"/>
+      <c r="P74" s="58"/>
+    </row>
+    <row r="75" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>73</v>
+      </c>
+      <c r="H75" s="58"/>
+      <c r="I75" s="58"/>
+      <c r="J75" s="58"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="58"/>
+      <c r="M75" s="58"/>
+      <c r="N75" s="58"/>
+      <c r="O75" s="58"/>
+      <c r="P75" s="58"/>
+    </row>
+    <row r="76" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>74</v>
+      </c>
+      <c r="H76" s="58"/>
+      <c r="I76" s="58"/>
+      <c r="J76" s="58"/>
+      <c r="K76" s="58"/>
+      <c r="L76" s="58"/>
+      <c r="M76" s="58"/>
+      <c r="N76" s="58"/>
+      <c r="O76" s="58"/>
+      <c r="P76" s="58"/>
+    </row>
+    <row r="77" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>75</v>
+      </c>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
+      <c r="J77" s="58"/>
+      <c r="K77" s="58"/>
+      <c r="L77" s="58"/>
+      <c r="M77" s="58"/>
+      <c r="N77" s="58"/>
+      <c r="O77" s="58"/>
+      <c r="P77" s="58"/>
+    </row>
+    <row r="78" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <v>76</v>
+      </c>
+      <c r="H78" s="58"/>
+      <c r="I78" s="58"/>
+      <c r="K78" s="58"/>
+      <c r="M78" s="58"/>
+      <c r="O78" s="58"/>
+      <c r="P78" s="58"/>
+    </row>
+    <row r="79" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>77</v>
+      </c>
+      <c r="H79" s="58"/>
+      <c r="I79" s="58"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="58"/>
+      <c r="M79" s="58"/>
+      <c r="N79" s="58"/>
+      <c r="O79" s="58"/>
+      <c r="P79" s="58"/>
+    </row>
+    <row r="80" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <v>78</v>
+      </c>
+      <c r="H80" s="58"/>
+      <c r="I80" s="58"/>
+      <c r="J80" s="58"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="58"/>
+      <c r="M80" s="58"/>
+      <c r="N80" s="58"/>
+      <c r="O80" s="58"/>
+      <c r="P80" s="58"/>
+    </row>
+    <row r="81" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <v>79</v>
+      </c>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
+      <c r="J81" s="58"/>
+      <c r="K81" s="58"/>
+      <c r="L81" s="58"/>
+      <c r="M81" s="58"/>
+      <c r="N81" s="58"/>
+      <c r="O81" s="58"/>
+      <c r="P81" s="58"/>
+    </row>
+    <row r="82" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>80</v>
+      </c>
+      <c r="H82" s="58"/>
+      <c r="I82" s="58"/>
+      <c r="J82" s="58"/>
+      <c r="K82" s="58"/>
+      <c r="L82" s="58"/>
+      <c r="M82" s="58"/>
+      <c r="N82" s="58"/>
+      <c r="O82" s="58"/>
+      <c r="P82" s="58"/>
+    </row>
+    <row r="83" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H83" s="58"/>
+      <c r="I83" s="58"/>
+      <c r="J83" s="58"/>
+      <c r="K83" s="58"/>
+      <c r="L83" s="58"/>
+      <c r="M83" s="58"/>
+      <c r="N83" s="58"/>
+      <c r="O83" s="58"/>
+      <c r="P83" s="58"/>
+    </row>
+    <row r="84" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H84" s="58"/>
+      <c r="I84" s="58"/>
+      <c r="J84" s="58"/>
+      <c r="K84" s="58"/>
+      <c r="L84" s="58"/>
+      <c r="M84" s="58"/>
+      <c r="N84" s="58"/>
+      <c r="O84" s="58"/>
+      <c r="P84" s="58"/>
+    </row>
+    <row r="85" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H85" s="58"/>
+      <c r="I85" s="58"/>
+      <c r="J85" s="58"/>
+      <c r="K85" s="58"/>
+      <c r="L85" s="58"/>
+      <c r="M85" s="58"/>
+      <c r="N85" s="58"/>
+      <c r="O85" s="58"/>
+      <c r="P85" s="58"/>
+    </row>
+    <row r="86" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="H86" s="58"/>
+      <c r="I86" s="58"/>
+      <c r="K86" s="58"/>
+      <c r="M86" s="58"/>
+      <c r="O86" s="58"/>
+      <c r="P86" s="58"/>
+    </row>
+    <row r="87" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I87" s="58"/>
+      <c r="J87" s="58"/>
+      <c r="K87" s="58"/>
+      <c r="L87" s="58"/>
+      <c r="M87" s="58"/>
+      <c r="N87" s="58"/>
+      <c r="O87" s="58"/>
+      <c r="P87" s="58"/>
+    </row>
+    <row r="88" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I88" s="58"/>
+      <c r="J88" s="58"/>
+      <c r="K88" s="58"/>
+      <c r="L88" s="58"/>
+      <c r="M88" s="58"/>
+      <c r="N88" s="58"/>
+      <c r="O88" s="58"/>
+      <c r="P88" s="58"/>
+    </row>
+    <row r="89" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I89" s="58"/>
+      <c r="J89" s="58"/>
+      <c r="K89" s="58"/>
+      <c r="L89" s="58"/>
+      <c r="M89" s="58"/>
+      <c r="N89" s="58"/>
+      <c r="O89" s="58"/>
+      <c r="P89" s="58"/>
+    </row>
+    <row r="90" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I90" s="58"/>
+      <c r="J90" s="58"/>
+      <c r="K90" s="58"/>
+      <c r="L90" s="58"/>
+      <c r="M90" s="58"/>
+      <c r="N90" s="58"/>
+      <c r="O90" s="58"/>
+      <c r="P90" s="58"/>
+    </row>
+    <row r="91" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I91" s="58"/>
+      <c r="K91" s="58"/>
+      <c r="M91" s="58"/>
+      <c r="O91" s="58"/>
+      <c r="P91" s="58"/>
+    </row>
+    <row r="92" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="I92" s="58"/>
+      <c r="J92" s="58"/>
+      <c r="K92" s="58"/>
+      <c r="L92" s="58"/>
+      <c r="M92" s="58"/>
+      <c r="N92" s="58"/>
+      <c r="O92" s="58"/>
+      <c r="P92" s="58"/>
+    </row>
+    <row r="93" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L93" s="58"/>
+      <c r="M93" s="58"/>
+      <c r="N93" s="58"/>
+      <c r="O93" s="58"/>
+    </row>
+    <row r="94" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L94" s="58"/>
+      <c r="M94" s="58"/>
+      <c r="N94" s="58"/>
+      <c r="O94" s="58"/>
+    </row>
+    <row r="95" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L95" s="58"/>
+      <c r="M95" s="58"/>
+      <c r="N95" s="58"/>
+      <c r="O95" s="58"/>
+    </row>
+    <row r="96" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L96" s="58"/>
+      <c r="M96" s="58"/>
+      <c r="N96" s="58"/>
+      <c r="O96" s="58"/>
+    </row>
+    <row r="97" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L97" s="58"/>
+      <c r="M97" s="58"/>
+      <c r="N97" s="58"/>
+      <c r="O97" s="58"/>
+    </row>
+    <row r="98" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L98" s="58"/>
+      <c r="M98" s="58"/>
+      <c r="N98" s="58"/>
+      <c r="O98" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A03D14-663C-42B7-B26E-A63445663F92}">
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:AB71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,7 +5887,7 @@
     <col min="23" max="23" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -2544,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
@@ -2610,7 +5967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>11</v>
       </c>
@@ -2643,7 +6000,7 @@
       <c r="U3" s="24"/>
       <c r="V3" s="60"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>2</v>
       </c>
@@ -2663,7 +6020,7 @@
       <c r="U4" s="59"/>
       <c r="V4" s="30"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
         <v>27</v>
       </c>
@@ -2690,7 +6047,7 @@
       <c r="U5" s="59"/>
       <c r="V5" s="30"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>30</v>
       </c>
@@ -2717,7 +6074,7 @@
       <c r="U6" s="26"/>
       <c r="V6" s="27"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>29</v>
       </c>
@@ -2746,7 +6103,7 @@
       <c r="U7" s="24"/>
       <c r="V7" s="60"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2780,7 +6137,7 @@
       <c r="U8" s="59"/>
       <c r="V8" s="30"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2812,7 +6169,7 @@
       <c r="U9" s="59"/>
       <c r="V9" s="30"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>8</v>
       </c>
@@ -2833,7 +6190,7 @@
       <c r="U10" s="26"/>
       <c r="V10" s="27"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>9</v>
       </c>
@@ -2856,7 +6213,7 @@
       <c r="U11" s="28"/>
       <c r="V11" s="30"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>10</v>
       </c>
@@ -2879,7 +6236,7 @@
       <c r="U12" s="28"/>
       <c r="V12" s="30"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>11</v>
       </c>
@@ -2900,7 +6257,7 @@
       <c r="U13" s="28"/>
       <c r="V13" s="30"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>12</v>
       </c>
@@ -2922,8 +6279,12 @@
       <c r="T14" s="30"/>
       <c r="U14" s="28"/>
       <c r="V14" s="30"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <f>AA49-'B6-H2'!L6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>13</v>
       </c>
@@ -2944,7 +6305,7 @@
       <c r="U15" s="28"/>
       <c r="V15" s="30"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>14</v>
       </c>
@@ -12584,9 +15945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279B77A7-FEEC-4A76-A1F9-1AC2C489FB77}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
style B6 Half 2
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1540" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{253E2CF4-DC63-4507-B633-490965825E66}"/>
+  <xr:revisionPtr revIDLastSave="1544" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61BB8E5B-C4B5-42FC-98E5-2E04B5D04473}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" firstSheet="4" activeTab="10" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
@@ -2522,7 +2522,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,11 +2864,12 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <v>150</v>
+        <f>70+50</f>
+        <v>120</v>
       </c>
       <c r="C16">
         <f>B16/5</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -4385,7 +4386,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4653,11 +4654,11 @@
         <v>10</v>
       </c>
       <c r="B15">
-        <v>395</v>
+        <v>300</v>
       </c>
       <c r="C15">
         <f>B15/5</f>
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -4681,12 +4682,11 @@
         <v>11</v>
       </c>
       <c r="B16">
-        <f>60+90</f>
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C16">
         <f>B16/5</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Add inset border to windows in Building 4
</commit_message>
<xml_diff>
--- a/Cityscape Buildings Blueprints.xlsx
+++ b/Cityscape Buildings Blueprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77dce58db303a22d/25 - Web Development Projects/CSS Drawings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1544" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61BB8E5B-C4B5-42FC-98E5-2E04B5D04473}"/>
+  <xr:revisionPtr revIDLastSave="1545" documentId="8_{DC7B353C-8351-4F27-AB54-C04C0257C2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB7F8905-FE24-4D65-B22D-D45990E42221}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4920" windowWidth="16440" windowHeight="28320" firstSheet="4" activeTab="10" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
+    <workbookView minimized="1" xWindow="-13560" yWindow="3135" windowWidth="15105" windowHeight="13320" firstSheet="4" activeTab="5" xr2:uid="{806AA18A-9C05-4881-971C-BC2F49DF16F6}"/>
   </bookViews>
   <sheets>
     <sheet name="B1-H1 &amp; H2" sheetId="2" r:id="rId1"/>
@@ -4384,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ECA445-E2A0-445A-8462-93AEA1A76CDC}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -13599,9 +13599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEA38ED-18F1-4CB9-A8B5-69652EFF8644}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:D14"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13788,11 +13788,12 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>65</v>
+        <f>65+50</f>
+        <v>115</v>
       </c>
       <c r="C8">
         <f>B8/5</f>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>

</xml_diff>